<commit_message>
+found/fixed uninitialized variable +removed Time from OtherStates just because I didn't like a copy of it there
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@101 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="561">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -1258,9 +1258,6 @@
   </si>
   <si>
     <t>TurbineComponents</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
   <si>
     <t>OldTime</t>
@@ -3054,11 +3051,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K429"/>
+  <dimension ref="A1:K428"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <pane ySplit="15" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A322" sqref="A322:XFD322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,19 +3111,19 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -3208,10 +3205,10 @@
     </row>
     <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -3240,7 +3237,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>26</v>
@@ -3270,7 +3267,7 @@
         <v>117</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>26</v>
@@ -3300,7 +3297,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>26</v>
@@ -3330,7 +3327,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>26</v>
@@ -3694,13 +3691,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>107</v>
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>47</v>
       </c>
@@ -3730,13 +3727,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>108</v>
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>22</v>
       </c>
@@ -3766,7 +3763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>22</v>
       </c>
@@ -3796,7 +3793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>22</v>
       </c>
@@ -3826,7 +3823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>22</v>
       </c>
@@ -3856,7 +3853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>22</v>
       </c>
@@ -3886,7 +3883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>22</v>
       </c>
@@ -3907,7 +3904,7 @@
       </c>
       <c r="I52" s="9"/>
     </row>
-    <row r="53" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>22</v>
       </c>
@@ -3934,7 +3931,7 @@
       </c>
       <c r="I53" s="9"/>
     </row>
-    <row r="54" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>22</v>
       </c>
@@ -3964,7 +3961,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>22</v>
       </c>
@@ -3994,7 +3991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>22</v>
       </c>
@@ -4024,7 +4021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>22</v>
       </c>
@@ -4051,7 +4048,7 @@
       </c>
       <c r="I57" s="9"/>
     </row>
-    <row r="58" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>22</v>
       </c>
@@ -4081,7 +4078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>22</v>
       </c>
@@ -4111,7 +4108,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>22</v>
       </c>
@@ -4134,21 +4131,21 @@
         <v>226</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>537</v>
-      </c>
-      <c r="I62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A63" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>538</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>34</v>
@@ -4170,7 +4167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>22</v>
       </c>
@@ -4178,7 +4175,7 @@
         <v>27</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>34</v>
@@ -4200,7 +4197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>22</v>
       </c>
@@ -4208,7 +4205,7 @@
         <v>27</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>34</v>
@@ -4230,7 +4227,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>22</v>
       </c>
@@ -4238,7 +4235,7 @@
         <v>27</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>34</v>
@@ -4260,7 +4257,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>22</v>
       </c>
@@ -4268,7 +4265,7 @@
         <v>27</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>34</v>
@@ -4290,7 +4287,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>22</v>
       </c>
@@ -4298,7 +4295,7 @@
         <v>27</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>34</v>
@@ -4320,7 +4317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>22</v>
       </c>
@@ -4328,7 +4325,7 @@
         <v>27</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>34</v>
@@ -4350,7 +4347,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>22</v>
       </c>
@@ -4358,7 +4355,7 @@
         <v>27</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>34</v>
@@ -4380,7 +4377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>22</v>
       </c>
@@ -4388,7 +4385,7 @@
         <v>27</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>34</v>
@@ -4410,7 +4407,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>22</v>
       </c>
@@ -4418,7 +4415,7 @@
         <v>27</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>99</v>
@@ -4440,7 +4437,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>22</v>
       </c>
@@ -4448,7 +4445,7 @@
         <v>27</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>99</v>
@@ -4470,7 +4467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>22</v>
       </c>
@@ -4478,7 +4475,7 @@
         <v>27</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>34</v>
@@ -4500,7 +4497,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>22</v>
       </c>
@@ -4508,7 +4505,7 @@
         <v>27</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>34</v>
@@ -4530,7 +4527,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>22</v>
       </c>
@@ -4538,7 +4535,7 @@
         <v>27</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>34</v>
@@ -4560,7 +4557,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>22</v>
       </c>
@@ -4568,7 +4565,7 @@
         <v>27</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>34</v>
@@ -4590,7 +4587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>22</v>
       </c>
@@ -4598,7 +4595,7 @@
         <v>27</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>34</v>
@@ -4620,7 +4617,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>22</v>
       </c>
@@ -4628,7 +4625,7 @@
         <v>27</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>34</v>
@@ -4650,7 +4647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>22</v>
       </c>
@@ -4658,7 +4655,7 @@
         <v>27</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>34</v>
@@ -4680,7 +4677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>22</v>
       </c>
@@ -4688,7 +4685,7 @@
         <v>27</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>34</v>
@@ -4710,7 +4707,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>22</v>
       </c>
@@ -4718,7 +4715,7 @@
         <v>27</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>34</v>
@@ -4740,7 +4737,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>22</v>
       </c>
@@ -4748,7 +4745,7 @@
         <v>27</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>34</v>
@@ -4770,7 +4767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>22</v>
       </c>
@@ -4778,7 +4775,7 @@
         <v>27</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>34</v>
@@ -4800,7 +4797,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>22</v>
       </c>
@@ -4808,7 +4805,7 @@
         <v>27</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>34</v>
@@ -4830,7 +4827,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>22</v>
       </c>
@@ -4838,7 +4835,7 @@
         <v>27</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>34</v>
@@ -4860,7 +4857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>22</v>
       </c>
@@ -4868,7 +4865,7 @@
         <v>27</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>34</v>
@@ -4890,7 +4887,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>22</v>
       </c>
@@ -4898,7 +4895,7 @@
         <v>27</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>34</v>
@@ -4920,7 +4917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>22</v>
       </c>
@@ -4928,7 +4925,7 @@
         <v>27</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>34</v>
@@ -4950,7 +4947,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>22</v>
       </c>
@@ -4958,7 +4955,7 @@
         <v>27</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>34</v>
@@ -4980,7 +4977,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>22</v>
       </c>
@@ -4988,7 +4985,7 @@
         <v>27</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>34</v>
@@ -5010,7 +5007,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>22</v>
       </c>
@@ -5018,7 +5015,7 @@
         <v>27</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>34</v>
@@ -5040,7 +5037,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>22</v>
       </c>
@@ -5048,7 +5045,7 @@
         <v>27</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>34</v>
@@ -5070,7 +5067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>22</v>
       </c>
@@ -5078,7 +5075,7 @@
         <v>27</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>34</v>
@@ -5100,7 +5097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>22</v>
       </c>
@@ -5108,7 +5105,7 @@
         <v>27</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>34</v>
@@ -5130,7 +5127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>22</v>
       </c>
@@ -5138,7 +5135,7 @@
         <v>27</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>34</v>
@@ -5160,7 +5157,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>22</v>
       </c>
@@ -5168,7 +5165,7 @@
         <v>27</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>34</v>
@@ -5190,7 +5187,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>22</v>
       </c>
@@ -5198,7 +5195,7 @@
         <v>27</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>34</v>
@@ -5220,7 +5217,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>22</v>
       </c>
@@ -5228,7 +5225,7 @@
         <v>27</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>34</v>
@@ -5250,7 +5247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>22</v>
       </c>
@@ -5258,7 +5255,7 @@
         <v>27</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>34</v>
@@ -5280,7 +5277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>22</v>
       </c>
@@ -5288,7 +5285,7 @@
         <v>27</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>34</v>
@@ -5310,7 +5307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>22</v>
       </c>
@@ -5318,7 +5315,7 @@
         <v>27</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>34</v>
@@ -5340,7 +5337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>22</v>
       </c>
@@ -5348,7 +5345,7 @@
         <v>27</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>34</v>
@@ -5370,7 +5367,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>22</v>
       </c>
@@ -5378,7 +5375,7 @@
         <v>27</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>34</v>
@@ -5400,7 +5397,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>22</v>
       </c>
@@ -5408,7 +5405,7 @@
         <v>27</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>34</v>
@@ -5430,7 +5427,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
         <v>22</v>
       </c>
@@ -5438,7 +5435,7 @@
         <v>27</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>34</v>
@@ -5460,7 +5457,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
         <v>22</v>
       </c>
@@ -5468,7 +5465,7 @@
         <v>27</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>34</v>
@@ -5490,7 +5487,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
         <v>22</v>
       </c>
@@ -5498,7 +5495,7 @@
         <v>27</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>34</v>
@@ -5520,7 +5517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>22</v>
       </c>
@@ -5528,7 +5525,7 @@
         <v>27</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>34</v>
@@ -5550,7 +5547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
         <v>22</v>
       </c>
@@ -5558,7 +5555,7 @@
         <v>27</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>34</v>
@@ -5580,7 +5577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
         <v>22</v>
       </c>
@@ -5588,7 +5585,7 @@
         <v>27</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>34</v>
@@ -5610,7 +5607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
         <v>22</v>
       </c>
@@ -5618,7 +5615,7 @@
         <v>27</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>34</v>
@@ -5640,7 +5637,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
         <v>22</v>
       </c>
@@ -5648,7 +5645,7 @@
         <v>27</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>34</v>
@@ -5670,7 +5667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
         <v>22</v>
       </c>
@@ -5678,7 +5675,7 @@
         <v>27</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>34</v>
@@ -5700,7 +5697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
         <v>22</v>
       </c>
@@ -5708,7 +5705,7 @@
         <v>27</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>34</v>
@@ -5730,7 +5727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
         <v>22</v>
       </c>
@@ -5738,7 +5735,7 @@
         <v>27</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>34</v>
@@ -5760,7 +5757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
         <v>22</v>
       </c>
@@ -5768,7 +5765,7 @@
         <v>27</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>34</v>
@@ -5790,7 +5787,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
         <v>22</v>
       </c>
@@ -5798,7 +5795,7 @@
         <v>27</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>34</v>
@@ -5820,7 +5817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
         <v>22</v>
       </c>
@@ -5828,7 +5825,7 @@
         <v>27</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>34</v>
@@ -5850,7 +5847,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
         <v>22</v>
       </c>
@@ -5858,7 +5855,7 @@
         <v>27</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>34</v>
@@ -5880,7 +5877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
         <v>22</v>
       </c>
@@ -5888,7 +5885,7 @@
         <v>27</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>34</v>
@@ -5910,7 +5907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
         <v>22</v>
       </c>
@@ -5918,7 +5915,7 @@
         <v>27</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>34</v>
@@ -5940,7 +5937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
         <v>22</v>
       </c>
@@ -5948,7 +5945,7 @@
         <v>27</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>34</v>
@@ -5970,7 +5967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
         <v>22</v>
       </c>
@@ -5978,7 +5975,7 @@
         <v>27</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>34</v>
@@ -6000,7 +5997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
         <v>22</v>
       </c>
@@ -6008,7 +6005,7 @@
         <v>27</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>34</v>
@@ -6030,7 +6027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
         <v>22</v>
       </c>
@@ -6038,7 +6035,7 @@
         <v>27</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>34</v>
@@ -6062,7 +6059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
         <v>22</v>
       </c>
@@ -6070,7 +6067,7 @@
         <v>27</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D127" s="8" t="s">
         <v>34</v>
@@ -6094,7 +6091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
         <v>22</v>
       </c>
@@ -6102,7 +6099,7 @@
         <v>27</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>34</v>
@@ -6126,7 +6123,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
         <v>22</v>
       </c>
@@ -6134,7 +6131,7 @@
         <v>27</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>34</v>
@@ -6158,7 +6155,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
         <v>22</v>
       </c>
@@ -6166,7 +6163,7 @@
         <v>27</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>34</v>
@@ -6190,7 +6187,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
         <v>22</v>
       </c>
@@ -6198,7 +6195,7 @@
         <v>27</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>99</v>
@@ -6220,7 +6217,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>22</v>
       </c>
@@ -6228,7 +6225,7 @@
         <v>27</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>99</v>
@@ -6250,16 +6247,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I133" s="9"/>
     </row>
-    <row r="134" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I134" s="4"/>
     </row>
-    <row r="135" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
         <v>22</v>
       </c>
@@ -6285,10 +6282,10 @@
         <v>26</v>
       </c>
       <c r="I135" s="9" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>22</v>
       </c>
@@ -6314,10 +6311,10 @@
         <v>26</v>
       </c>
       <c r="I136" s="9" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>22</v>
       </c>
@@ -6343,10 +6340,10 @@
         <v>26</v>
       </c>
       <c r="I137" s="9" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
         <v>22</v>
       </c>
@@ -6372,10 +6369,10 @@
         <v>26</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
         <v>22</v>
       </c>
@@ -6401,16 +6398,16 @@
         <v>26</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I141" s="4"/>
     </row>
-    <row r="142" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
         <v>233</v>
       </c>
@@ -6422,7 +6419,7 @@
       </c>
       <c r="I142" s="9"/>
     </row>
-    <row r="143" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
         <v>233</v>
       </c>
@@ -6434,7 +6431,7 @@
       </c>
       <c r="I143" s="9"/>
     </row>
-    <row r="144" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
         <v>233</v>
       </c>
@@ -6446,7 +6443,7 @@
       </c>
       <c r="I144" s="9"/>
     </row>
-    <row r="145" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
         <v>22</v>
       </c>
@@ -6473,7 +6470,7 @@
       </c>
       <c r="I145" s="9"/>
     </row>
-    <row r="146" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>22</v>
       </c>
@@ -6500,7 +6497,7 @@
       </c>
       <c r="I146" s="9"/>
     </row>
-    <row r="147" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
         <v>22</v>
       </c>
@@ -6527,7 +6524,7 @@
       </c>
       <c r="I147" s="9"/>
     </row>
-    <row r="148" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
         <v>22</v>
       </c>
@@ -6554,7 +6551,7 @@
       </c>
       <c r="I148" s="9"/>
     </row>
-    <row r="149" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
         <v>22</v>
       </c>
@@ -6581,7 +6578,7 @@
       </c>
       <c r="I149" s="9"/>
     </row>
-    <row r="150" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
         <v>22</v>
       </c>
@@ -6608,7 +6605,7 @@
       </c>
       <c r="I150" s="9"/>
     </row>
-    <row r="151" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
         <v>22</v>
       </c>
@@ -6635,7 +6632,7 @@
       </c>
       <c r="I151" s="9"/>
     </row>
-    <row r="152" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>22</v>
       </c>
@@ -6662,7 +6659,7 @@
       </c>
       <c r="I152" s="9"/>
     </row>
-    <row r="153" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>22</v>
       </c>
@@ -6689,7 +6686,7 @@
       </c>
       <c r="I153" s="9"/>
     </row>
-    <row r="154" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>22</v>
       </c>
@@ -6716,7 +6713,7 @@
       </c>
       <c r="I154" s="9"/>
     </row>
-    <row r="155" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
         <v>22</v>
       </c>
@@ -6746,7 +6743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>22</v>
       </c>
@@ -6776,7 +6773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
         <v>22</v>
       </c>
@@ -6803,7 +6800,7 @@
       </c>
       <c r="I157" s="9"/>
     </row>
-    <row r="158" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>22</v>
       </c>
@@ -6830,7 +6827,7 @@
       </c>
       <c r="I158" s="9"/>
     </row>
-    <row r="159" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>22</v>
       </c>
@@ -6857,7 +6854,7 @@
       </c>
       <c r="I159" s="9"/>
     </row>
-    <row r="160" spans="1:10" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>22</v>
       </c>
@@ -6884,7 +6881,7 @@
       </c>
       <c r="I160" s="9"/>
     </row>
-    <row r="161" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
         <v>22</v>
       </c>
@@ -6911,7 +6908,7 @@
       </c>
       <c r="I161" s="9"/>
     </row>
-    <row r="162" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
         <v>22</v>
       </c>
@@ -6938,7 +6935,7 @@
       </c>
       <c r="I162" s="9"/>
     </row>
-    <row r="163" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
         <v>22</v>
       </c>
@@ -6965,7 +6962,7 @@
       </c>
       <c r="I163" s="9"/>
     </row>
-    <row r="164" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
         <v>22</v>
       </c>
@@ -6992,7 +6989,7 @@
       </c>
       <c r="I164" s="9"/>
     </row>
-    <row r="165" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
         <v>22</v>
       </c>
@@ -7019,7 +7016,7 @@
       </c>
       <c r="I165" s="9"/>
     </row>
-    <row r="166" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
         <v>22</v>
       </c>
@@ -7046,7 +7043,7 @@
       </c>
       <c r="I166" s="9"/>
     </row>
-    <row r="167" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
         <v>22</v>
       </c>
@@ -7073,7 +7070,7 @@
       </c>
       <c r="I167" s="9"/>
     </row>
-    <row r="168" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
         <v>22</v>
       </c>
@@ -7100,7 +7097,7 @@
       </c>
       <c r="I168" s="9"/>
     </row>
-    <row r="169" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
         <v>22</v>
       </c>
@@ -7127,7 +7124,7 @@
       </c>
       <c r="I169" s="9"/>
     </row>
-    <row r="170" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="8" t="s">
         <v>22</v>
       </c>
@@ -7154,7 +7151,7 @@
       </c>
       <c r="I170" s="9"/>
     </row>
-    <row r="171" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="8" t="s">
         <v>47</v>
       </c>
@@ -7180,10 +7177,10 @@
         <v>26</v>
       </c>
       <c r="I171" s="9" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
         <v>22</v>
       </c>
@@ -7209,10 +7206,10 @@
         <v>26</v>
       </c>
       <c r="I172" s="9" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="8" t="s">
         <v>47</v>
       </c>
@@ -7295,7 +7292,7 @@
     </row>
     <row r="177" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I177" s="4"/>
     </row>
@@ -7449,7 +7446,7 @@
         <v>26</v>
       </c>
       <c r="K182" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="183" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7482,7 +7479,7 @@
         <v>26</v>
       </c>
       <c r="K183" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="184" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7667,7 +7664,7 @@
     </row>
     <row r="191" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I191" s="4"/>
     </row>
@@ -8297,7 +8294,7 @@
         <v>26</v>
       </c>
       <c r="I212" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="213" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8446,12 +8443,12 @@
         <v>26</v>
       </c>
       <c r="I217" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="219" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I219" s="4"/>
     </row>
@@ -8508,7 +8505,7 @@
         <v>26</v>
       </c>
       <c r="I221" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J221" s="8" t="s">
         <v>26</v>
@@ -8540,7 +8537,7 @@
         <v>26</v>
       </c>
       <c r="I222" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="223" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8569,7 +8566,7 @@
         <v>26</v>
       </c>
       <c r="I223" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="224" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8598,7 +8595,7 @@
         <v>26</v>
       </c>
       <c r="I224" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="225" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8627,7 +8624,7 @@
         <v>26</v>
       </c>
       <c r="I225" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="226" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8656,7 +8653,7 @@
         <v>26</v>
       </c>
       <c r="I226" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="227" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8685,12 +8682,12 @@
         <v>26</v>
       </c>
       <c r="I227" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="230" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I230" s="4"/>
     </row>
@@ -8720,7 +8717,7 @@
         <v>26</v>
       </c>
       <c r="I231" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="232" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8968,7 +8965,7 @@
     </row>
     <row r="242" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I242" s="4"/>
     </row>
@@ -9160,7 +9157,7 @@
         <v>26</v>
       </c>
       <c r="I249" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="250" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9189,7 +9186,7 @@
         <v>26</v>
       </c>
       <c r="I250" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="251" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9218,7 +9215,7 @@
         <v>26</v>
       </c>
       <c r="I251" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="252" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9247,7 +9244,7 @@
         <v>26</v>
       </c>
       <c r="I252" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="253" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9276,7 +9273,7 @@
         <v>26</v>
       </c>
       <c r="I253" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="254" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9305,7 +9302,7 @@
         <v>26</v>
       </c>
       <c r="I254" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="255" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9334,7 +9331,7 @@
         <v>26</v>
       </c>
       <c r="I255" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J255" s="8" t="s">
         <v>103</v>
@@ -9366,7 +9363,7 @@
         <v>26</v>
       </c>
       <c r="I256" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="257" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9395,7 +9392,7 @@
         <v>26</v>
       </c>
       <c r="I257" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="258" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9424,7 +9421,7 @@
         <v>26</v>
       </c>
       <c r="I258" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="259" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9453,7 +9450,7 @@
         <v>26</v>
       </c>
       <c r="I259" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="260" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9482,7 +9479,7 @@
         <v>26</v>
       </c>
       <c r="I260" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="261" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9511,7 +9508,7 @@
         <v>26</v>
       </c>
       <c r="I261" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J261" s="8" t="s">
         <v>103</v>
@@ -9531,19 +9528,19 @@
         <v>99</v>
       </c>
       <c r="E262" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="F262" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G262" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H262" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I262" s="9" t="s">
         <v>555</v>
-      </c>
-      <c r="F262" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G262" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H262" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I262" s="9" t="s">
-        <v>556</v>
       </c>
       <c r="J262" s="8" t="s">
         <v>103</v>
@@ -9563,7 +9560,7 @@
         <v>41</v>
       </c>
       <c r="E263" s="8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F263" s="8" t="s">
         <v>26</v>
@@ -9575,7 +9572,7 @@
         <v>26</v>
       </c>
       <c r="I263" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="264" spans="1:10" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -9592,7 +9589,7 @@
         <v>34</v>
       </c>
       <c r="E264" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F264" s="8" t="s">
         <v>31</v>
@@ -9604,7 +9601,7 @@
         <v>26</v>
       </c>
       <c r="I264" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J264" s="8" t="s">
         <v>26</v>
@@ -9615,7 +9612,7 @@
     </row>
     <row r="266" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I266" s="4"/>
     </row>
@@ -9807,7 +9804,7 @@
         <v>26</v>
       </c>
       <c r="I273" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J273" s="8" t="s">
         <v>371</v>
@@ -9839,7 +9836,7 @@
         <v>26</v>
       </c>
       <c r="I274" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J274" s="8" t="s">
         <v>373</v>
@@ -9895,7 +9892,7 @@
         <v>26</v>
       </c>
       <c r="I278" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="279" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9924,7 +9921,7 @@
         <v>26</v>
       </c>
       <c r="I279" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="280" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9995,7 +9992,7 @@
         <v>26</v>
       </c>
       <c r="I284" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="285" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10012,7 +10009,7 @@
         <v>24</v>
       </c>
       <c r="E285" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F285" s="8" t="s">
         <v>26</v>
@@ -10039,7 +10036,7 @@
         <v>24</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F286" s="8" t="s">
         <v>26</v>
@@ -10051,7 +10048,7 @@
         <v>26</v>
       </c>
       <c r="I286" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="287" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10080,7 +10077,7 @@
         <v>26</v>
       </c>
       <c r="I287" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="288" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10109,7 +10106,7 @@
         <v>26</v>
       </c>
       <c r="I288" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="289" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10138,7 +10135,7 @@
         <v>26</v>
       </c>
       <c r="I289" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="290" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10167,7 +10164,7 @@
         <v>26</v>
       </c>
       <c r="I290" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="291" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10196,7 +10193,7 @@
         <v>26</v>
       </c>
       <c r="I291" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="292" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10225,7 +10222,7 @@
         <v>26</v>
       </c>
       <c r="I292" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="293" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10254,7 +10251,7 @@
         <v>26</v>
       </c>
       <c r="I293" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="294" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10283,7 +10280,7 @@
         <v>26</v>
       </c>
       <c r="I294" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="295" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10348,7 +10345,7 @@
         <v>41</v>
       </c>
       <c r="E297" s="8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F297" s="8" t="s">
         <v>26</v>
@@ -10360,7 +10357,7 @@
         <v>26</v>
       </c>
       <c r="I297" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="298" spans="1:10" s="8" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -10377,7 +10374,7 @@
         <v>34</v>
       </c>
       <c r="E298" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F298" s="8" t="s">
         <v>87</v>
@@ -10389,7 +10386,7 @@
         <v>26</v>
       </c>
       <c r="I298" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J298" s="8" t="s">
         <v>26</v>
@@ -10406,10 +10403,10 @@
         <v>23</v>
       </c>
       <c r="D299" s="8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E299" s="8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F299" s="8" t="s">
         <v>26</v>
@@ -10457,7 +10454,7 @@
         <v>26</v>
       </c>
       <c r="I301" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="302" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10471,10 +10468,10 @@
         <v>28</v>
       </c>
       <c r="D302" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="E302" s="8" t="s">
         <v>514</v>
-      </c>
-      <c r="E302" s="8" t="s">
-        <v>515</v>
       </c>
       <c r="F302" s="8" t="s">
         <v>26</v>
@@ -10546,10 +10543,10 @@
         <v>33</v>
       </c>
       <c r="D307" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E307" s="8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F307" s="8" t="s">
         <v>26</v>
@@ -10615,10 +10612,10 @@
         <v>36</v>
       </c>
       <c r="D311" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E311" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F311" s="8" t="s">
         <v>26</v>
@@ -10684,10 +10681,10 @@
         <v>38</v>
       </c>
       <c r="D315" s="8" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E315" s="8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F315" s="8" t="s">
         <v>26</v>
@@ -10708,7 +10705,7 @@
     </row>
     <row r="317" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="318" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10773,7 +10770,7 @@
         <v>26</v>
       </c>
       <c r="I320" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J320" s="8" t="s">
         <v>46</v>
@@ -10847,7 +10844,7 @@
         <v>40</v>
       </c>
       <c r="D323" s="8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E323" s="8" t="s">
         <v>392</v>
@@ -10855,13 +10852,15 @@
       <c r="F323" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G323" s="8" t="s">
-        <v>26</v>
+      <c r="G323" s="8">
+        <v>1</v>
       </c>
       <c r="H323" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I323" s="9"/>
+      <c r="I323" s="9" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="324" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A324" s="8" t="s">
@@ -10889,7 +10888,7 @@
         <v>26</v>
       </c>
       <c r="I324" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="325" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10918,7 +10917,7 @@
         <v>26</v>
       </c>
       <c r="I325" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="326" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10940,8 +10939,8 @@
       <c r="F326" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G326" s="8">
-        <v>1</v>
+      <c r="G326" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="H326" s="8" t="s">
         <v>26</v>
@@ -10961,7 +10960,7 @@
         <v>40</v>
       </c>
       <c r="D327" s="8" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="E327" s="8" t="s">
         <v>396</v>
@@ -10970,7 +10969,7 @@
         <v>26</v>
       </c>
       <c r="G327" s="8" t="s">
-        <v>26</v>
+        <v>397</v>
       </c>
       <c r="H327" s="8" t="s">
         <v>26</v>
@@ -10993,13 +10992,13 @@
         <v>99</v>
       </c>
       <c r="E328" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F328" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G328" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H328" s="8" t="s">
         <v>26</v>
@@ -11022,13 +11021,13 @@
         <v>99</v>
       </c>
       <c r="E329" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="F329" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G329" s="8" t="s">
         <v>399</v>
-      </c>
-      <c r="F329" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G329" s="8" t="s">
-        <v>400</v>
       </c>
       <c r="H329" s="8" t="s">
         <v>26</v>
@@ -11057,13 +11056,13 @@
         <v>26</v>
       </c>
       <c r="G330" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H330" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I330" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="331" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11086,13 +11085,13 @@
         <v>26</v>
       </c>
       <c r="G331" s="8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H331" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I331" s="9" t="s">
-        <v>498</v>
+        <v>1</v>
       </c>
     </row>
     <row r="332" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11115,13 +11114,14 @@
         <v>26</v>
       </c>
       <c r="G332" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H332" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I332" s="9" t="s">
-        <v>1</v>
+      <c r="I332" s="9"/>
+      <c r="J332" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="333" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>40</v>
       </c>
       <c r="D333" s="8" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E333" s="8" t="s">
         <v>404</v>
@@ -11143,15 +11143,14 @@
       <c r="F333" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G333" s="8" t="s">
-        <v>398</v>
+      <c r="G333" s="8">
+        <v>0</v>
       </c>
       <c r="H333" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I333" s="9"/>
-      <c r="J333" s="8" t="s">
-        <v>26</v>
+      <c r="I333" s="9" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="334" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11165,225 +11164,202 @@
         <v>40</v>
       </c>
       <c r="D334" s="8" t="s">
-        <v>89</v>
+        <v>518</v>
       </c>
       <c r="E334" s="8" t="s">
-        <v>405</v>
+        <v>529</v>
       </c>
       <c r="F334" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G334" s="8">
-        <v>0</v>
+      <c r="G334" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="H334" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I334" s="9" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="335" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B335" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C335" s="8" t="s">
+      <c r="I334" s="9"/>
+      <c r="J334" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="I335" s="4"/>
+    </row>
+    <row r="336" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B336" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C336" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D335" s="8" t="s">
-        <v>519</v>
-      </c>
-      <c r="E335" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="F335" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G335" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H335" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I335" s="9"/>
-      <c r="J335" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="336" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A336" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="I336" s="4"/>
-    </row>
-    <row r="337" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B337" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C337" s="8" t="s">
+      <c r="D336" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E336" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I336" s="9"/>
+    </row>
+    <row r="337" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="I337" s="4"/>
+    </row>
+    <row r="338" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B338" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C338" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D337" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E337" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I337" s="9"/>
-    </row>
-    <row r="338" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A338" s="3" t="s">
+      <c r="D338" s="8" t="s">
         <v>537</v>
       </c>
-      <c r="I338" s="4"/>
-    </row>
-    <row r="339" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A339" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B339" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C339" s="8" t="s">
+      <c r="E338" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="I338" s="9"/>
+    </row>
+    <row r="339" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="I339" s="4"/>
+    </row>
+    <row r="340" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B340" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C340" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D339" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="E339" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="I339" s="9"/>
-    </row>
-    <row r="340" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A340" s="3" t="s">
+      <c r="D340" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E340" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="I340" s="9"/>
+    </row>
+    <row r="341" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="I340" s="4"/>
-    </row>
-    <row r="341" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B341" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C341" s="8" t="s">
+      <c r="I341" s="4"/>
+    </row>
+    <row r="342" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B342" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C342" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D341" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E341" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="I341" s="9"/>
-    </row>
-    <row r="342" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A342" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="I342" s="4"/>
-    </row>
-    <row r="343" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B343" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C343" s="8" t="s">
+      <c r="D342" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E342" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="I342" s="9"/>
+    </row>
+    <row r="343" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I343" s="4"/>
+    </row>
+    <row r="344" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B344" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C344" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D343" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E343" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="I343" s="9"/>
-    </row>
-    <row r="344" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A344" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="I344" s="4"/>
-    </row>
-    <row r="345" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A345" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B345" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C345" s="8" t="s">
+      <c r="D344" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="E344" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="I344" s="9"/>
+    </row>
+    <row r="345" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="I345" s="4"/>
+    </row>
+    <row r="346" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B346" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C346" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D345" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="E345" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="I345" s="9"/>
-    </row>
-    <row r="346" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="I346" s="4"/>
-    </row>
-    <row r="347" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B347" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C347" s="8" t="s">
+      <c r="D346" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="E346" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="I346" s="9"/>
+    </row>
+    <row r="347" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="I347" s="4"/>
+    </row>
+    <row r="348" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B348" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C348" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D347" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E347" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="I347" s="9"/>
-    </row>
-    <row r="348" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="I348" s="4"/>
-    </row>
-    <row r="349" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B349" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C349" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D349" s="8" t="s">
+      <c r="D348" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="E349" s="8" t="s">
+      <c r="E348" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="I349" s="9"/>
+      <c r="I348" s="9"/>
+    </row>
+    <row r="349" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I349" s="4"/>
     </row>
     <row r="350" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>109</v>
+        <v>488</v>
       </c>
       <c r="I350" s="4"/>
     </row>
@@ -11393,38 +11369,55 @@
       </c>
       <c r="I351" s="4"/>
     </row>
-    <row r="352" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="I352" s="4"/>
-    </row>
-    <row r="353" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B352" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C352" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D352" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E352" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="B353" s="10" t="s">
+      <c r="F352" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G352" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H352" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I352" s="11" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="353" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B353" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C353" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D353" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E353" s="10" t="s">
+      <c r="D353" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E353" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="F353" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G353" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H353" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I353" s="11" t="s">
+      <c r="F353" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I353" s="8" t="s">
         <v>500</v>
       </c>
     </row>
@@ -11448,7 +11441,7 @@
         <v>88</v>
       </c>
       <c r="I354" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="355" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11462,16 +11455,22 @@
         <v>40</v>
       </c>
       <c r="D355" s="8" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E355" s="8" t="s">
-        <v>409</v>
+        <v>556</v>
       </c>
       <c r="F355" s="8" t="s">
-        <v>88</v>
+        <v>26</v>
+      </c>
+      <c r="G355" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H355" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I355" s="8" t="s">
-        <v>501</v>
+        <v>557</v>
       </c>
     </row>
     <row r="356" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11485,23 +11484,12 @@
         <v>40</v>
       </c>
       <c r="D356" s="8" t="s">
-        <v>99</v>
+        <v>292</v>
       </c>
       <c r="E356" s="8" t="s">
-        <v>557</v>
-      </c>
-      <c r="F356" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G356" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H356" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I356" s="8" t="s">
-        <v>558</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="I356" s="9"/>
     </row>
     <row r="357" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="8" t="s">
@@ -11514,10 +11502,19 @@
         <v>40</v>
       </c>
       <c r="D357" s="8" t="s">
-        <v>292</v>
+        <v>99</v>
       </c>
       <c r="E357" s="8" t="s">
-        <v>436</v>
+        <v>422</v>
+      </c>
+      <c r="F357" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G357" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H357" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I357" s="9"/>
     </row>
@@ -11535,7 +11532,7 @@
         <v>99</v>
       </c>
       <c r="E358" s="8" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F358" s="8" t="s">
         <v>26</v>
@@ -11546,61 +11543,52 @@
       <c r="H358" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I358" s="9"/>
+      <c r="I358" s="9" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="359" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A359" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B359" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C359" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D359" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E359" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="F359" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G359" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H359" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I359" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="360" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I360" s="9"/>
+      <c r="I359" s="9"/>
+    </row>
+    <row r="360" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I360" s="4"/>
     </row>
     <row r="361" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A361" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I361" s="4"/>
     </row>
     <row r="362" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A362" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I362" s="4"/>
     </row>
-    <row r="363" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A363" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I363" s="4"/>
+    <row r="363" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B363" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C363" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D363" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E363" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I363" s="9"/>
     </row>
     <row r="364" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A364" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B364" s="8" t="s">
         <v>27</v>
@@ -11609,12 +11597,23 @@
         <v>43</v>
       </c>
       <c r="D364" s="8" t="s">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I364" s="9"/>
+        <v>383</v>
+      </c>
+      <c r="F364" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G364" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H364" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I364" s="9" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="365" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A365" s="8" t="s">
@@ -11630,7 +11629,7 @@
         <v>24</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F365" s="8" t="s">
         <v>26</v>
@@ -11656,23 +11655,15 @@
         <v>43</v>
       </c>
       <c r="D366" s="8" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>384</v>
+        <v>409</v>
       </c>
       <c r="F366" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G366" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H366" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I366" s="9" t="s">
-        <v>483</v>
-      </c>
+      <c r="I366" s="9"/>
     </row>
     <row r="367" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A367" s="8" t="s">
@@ -11693,6 +11684,12 @@
       <c r="F367" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="G367" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="H367" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="I367" s="9"/>
     </row>
     <row r="368" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11709,15 +11706,9 @@
         <v>99</v>
       </c>
       <c r="E368" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F368" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G368" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="H368" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I368" s="9"/>
@@ -11736,10 +11727,7 @@
         <v>99</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="F369" s="8" t="s">
-        <v>26</v>
+        <v>388</v>
       </c>
       <c r="I369" s="9"/>
     </row>
@@ -11757,7 +11745,13 @@
         <v>99</v>
       </c>
       <c r="E370" s="8" t="s">
-        <v>388</v>
+        <v>413</v>
+      </c>
+      <c r="F370" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G370" s="8" t="s">
+        <v>399</v>
       </c>
       <c r="I370" s="9"/>
     </row>
@@ -11781,9 +11775,15 @@
         <v>26</v>
       </c>
       <c r="G371" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
+      </c>
+      <c r="H371" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I371" s="9"/>
+      <c r="J371" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="372" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A372" s="8" t="s">
@@ -11796,21 +11796,23 @@
         <v>43</v>
       </c>
       <c r="D372" s="8" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>415</v>
+        <v>100</v>
       </c>
       <c r="F372" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G372" s="8" t="s">
-        <v>400</v>
+        <v>26</v>
       </c>
       <c r="H372" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I372" s="9"/>
+      <c r="I372" s="9" t="s">
+        <v>501</v>
+      </c>
       <c r="J372" s="8" t="s">
         <v>26</v>
       </c>
@@ -11826,10 +11828,10 @@
         <v>43</v>
       </c>
       <c r="D373" s="8" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E373" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F373" s="8" t="s">
         <v>26</v>
@@ -11841,10 +11843,7 @@
         <v>26</v>
       </c>
       <c r="I373" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="J373" s="8" t="s">
-        <v>26</v>
+        <v>484</v>
       </c>
     </row>
     <row r="374" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11861,7 +11860,7 @@
         <v>41</v>
       </c>
       <c r="E374" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F374" s="8" t="s">
         <v>26</v>
@@ -11887,10 +11886,10 @@
         <v>43</v>
       </c>
       <c r="D375" s="8" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="E375" s="8" t="s">
-        <v>90</v>
+        <v>389</v>
       </c>
       <c r="F375" s="8" t="s">
         <v>26</v>
@@ -11901,9 +11900,7 @@
       <c r="H375" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I375" s="9" t="s">
-        <v>486</v>
-      </c>
+      <c r="I375" s="9"/>
     </row>
     <row r="376" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="8" t="s">
@@ -11919,7 +11916,7 @@
         <v>99</v>
       </c>
       <c r="E376" s="8" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="F376" s="8" t="s">
         <v>26</v>
@@ -11930,7 +11927,9 @@
       <c r="H376" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I376" s="9"/>
+      <c r="I376" s="9" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="377" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="8" t="s">
@@ -11980,15 +11979,7 @@
       <c r="F378" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G378" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H378" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I378" s="9" t="s">
-        <v>504</v>
-      </c>
+      <c r="I378" s="9"/>
     </row>
     <row r="379" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="8" t="s">
@@ -12004,12 +11995,20 @@
         <v>99</v>
       </c>
       <c r="E379" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F379" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I379" s="9"/>
+      <c r="G379" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H379" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I379" s="9" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="380" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A380" s="8" t="s">
@@ -12066,7 +12065,7 @@
         <v>26</v>
       </c>
       <c r="I381" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="382" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12080,10 +12079,10 @@
         <v>43</v>
       </c>
       <c r="D382" s="8" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="E382" s="8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F382" s="8" t="s">
         <v>26</v>
@@ -12109,10 +12108,10 @@
         <v>43</v>
       </c>
       <c r="D383" s="8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E383" s="8" t="s">
-        <v>424</v>
+        <v>101</v>
       </c>
       <c r="F383" s="8" t="s">
         <v>26</v>
@@ -12126,10 +12125,13 @@
       <c r="I383" s="9" t="s">
         <v>507</v>
       </c>
+      <c r="J383" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="384" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A384" s="8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B384" s="8" t="s">
         <v>27</v>
@@ -12141,7 +12143,7 @@
         <v>34</v>
       </c>
       <c r="E384" s="8" t="s">
-        <v>101</v>
+        <v>424</v>
       </c>
       <c r="F384" s="8" t="s">
         <v>26</v>
@@ -12153,15 +12155,15 @@
         <v>26</v>
       </c>
       <c r="I384" s="9" t="s">
-        <v>508</v>
+        <v>454</v>
       </c>
       <c r="J384" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="385" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B385" s="8" t="s">
         <v>27</v>
@@ -12170,7 +12172,7 @@
         <v>43</v>
       </c>
       <c r="D385" s="8" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E385" s="8" t="s">
         <v>425</v>
@@ -12178,20 +12180,14 @@
       <c r="F385" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G385" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H385" s="8" t="s">
-        <v>26</v>
+      <c r="G385" s="8">
+        <v>19</v>
       </c>
       <c r="I385" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="J385" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="386" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A386" s="8" t="s">
         <v>22</v>
       </c>
@@ -12205,19 +12201,17 @@
         <v>41</v>
       </c>
       <c r="E386" s="8" t="s">
-        <v>426</v>
+        <v>558</v>
       </c>
       <c r="F386" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G386" s="8">
-        <v>19</v>
-      </c>
-      <c r="I386" s="9" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="387" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G386" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="I386" s="9"/>
+    </row>
+    <row r="387" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A387" s="8" t="s">
         <v>22</v>
       </c>
@@ -12231,17 +12225,17 @@
         <v>41</v>
       </c>
       <c r="E387" s="8" t="s">
-        <v>559</v>
+        <v>426</v>
       </c>
       <c r="F387" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G387" s="8" t="s">
-        <v>560</v>
+      <c r="G387" s="8">
+        <v>70</v>
       </c>
       <c r="I387" s="9"/>
     </row>
-    <row r="388" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A388" s="8" t="s">
         <v>22</v>
       </c>
@@ -12261,11 +12255,13 @@
         <v>26</v>
       </c>
       <c r="G388" s="8">
-        <v>70</v>
-      </c>
-      <c r="I388" s="9"/>
-    </row>
-    <row r="389" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I388" s="9" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="8" t="s">
         <v>22</v>
       </c>
@@ -12285,13 +12281,13 @@
         <v>26</v>
       </c>
       <c r="G389" s="8">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I389" s="9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="390" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="8" t="s">
         <v>22</v>
       </c>
@@ -12311,13 +12307,13 @@
         <v>26</v>
       </c>
       <c r="G390" s="8">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I390" s="9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="391" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="391" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A391" s="8" t="s">
         <v>22</v>
       </c>
@@ -12337,13 +12333,13 @@
         <v>26</v>
       </c>
       <c r="G391" s="8">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I391" s="9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="392" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="392" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="8" t="s">
         <v>22</v>
       </c>
@@ -12362,14 +12358,14 @@
       <c r="F392" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G392" s="8">
-        <v>93</v>
+      <c r="G392" s="8" t="s">
+        <v>559</v>
       </c>
       <c r="I392" s="9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="393" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="393" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="8" t="s">
         <v>22</v>
       </c>
@@ -12388,14 +12384,17 @@
       <c r="F393" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G393" s="8" t="s">
-        <v>560</v>
+      <c r="G393" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H393" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I393" s="9" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="394" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="8" t="s">
         <v>22</v>
       </c>
@@ -12406,7 +12405,7 @@
         <v>43</v>
       </c>
       <c r="D394" s="8" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="E394" s="8" t="s">
         <v>433</v>
@@ -12414,17 +12413,17 @@
       <c r="F394" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G394" s="8">
-        <v>1000</v>
+      <c r="G394" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="H394" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I394" s="9" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="395" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="8" t="s">
         <v>22</v>
       </c>
@@ -12435,7 +12434,7 @@
         <v>43</v>
       </c>
       <c r="D395" s="8" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E395" s="8" t="s">
         <v>434</v>
@@ -12443,17 +12442,15 @@
       <c r="F395" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G395" s="8" t="s">
-        <v>398</v>
+      <c r="G395" s="8">
+        <v>-1</v>
       </c>
       <c r="H395" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I395" s="9" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="396" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I395" s="9"/>
+    </row>
+    <row r="396" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A396" s="8" t="s">
         <v>22</v>
       </c>
@@ -12464,23 +12461,14 @@
         <v>43</v>
       </c>
       <c r="D396" s="8" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="E396" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="F396" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G396" s="8">
-        <v>-1</v>
-      </c>
-      <c r="H396" s="8" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="I396" s="9"/>
     </row>
-    <row r="397" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A397" s="8" t="s">
         <v>22</v>
       </c>
@@ -12491,14 +12479,14 @@
         <v>43</v>
       </c>
       <c r="D397" s="8" t="s">
-        <v>141</v>
+        <v>227</v>
       </c>
       <c r="E397" s="8" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="I397" s="9"/>
     </row>
-    <row r="398" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A398" s="8" t="s">
         <v>22</v>
       </c>
@@ -12509,14 +12497,14 @@
         <v>43</v>
       </c>
       <c r="D398" s="8" t="s">
-        <v>227</v>
+        <v>538</v>
       </c>
       <c r="E398" s="8" t="s">
-        <v>125</v>
+        <v>537</v>
       </c>
       <c r="I398" s="9"/>
     </row>
-    <row r="399" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A399" s="8" t="s">
         <v>22</v>
       </c>
@@ -12527,14 +12515,14 @@
         <v>43</v>
       </c>
       <c r="D399" s="8" t="s">
-        <v>539</v>
+        <v>268</v>
       </c>
       <c r="E399" s="8" t="s">
-        <v>538</v>
+        <v>232</v>
       </c>
       <c r="I399" s="9"/>
     </row>
-    <row r="400" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A400" s="8" t="s">
         <v>22</v>
       </c>
@@ -12545,10 +12533,10 @@
         <v>43</v>
       </c>
       <c r="D400" s="8" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="E400" s="8" t="s">
-        <v>232</v>
+        <v>278</v>
       </c>
       <c r="I400" s="9"/>
     </row>
@@ -12563,10 +12551,10 @@
         <v>43</v>
       </c>
       <c r="D401" s="8" t="s">
-        <v>286</v>
+        <v>342</v>
       </c>
       <c r="E401" s="8" t="s">
-        <v>278</v>
+        <v>341</v>
       </c>
       <c r="I401" s="9"/>
     </row>
@@ -12581,10 +12569,10 @@
         <v>43</v>
       </c>
       <c r="D402" s="8" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="E402" s="8" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="I402" s="9"/>
     </row>
@@ -12599,10 +12587,10 @@
         <v>43</v>
       </c>
       <c r="D403" s="8" t="s">
-        <v>321</v>
+        <v>369</v>
       </c>
       <c r="E403" s="8" t="s">
-        <v>319</v>
+        <v>362</v>
       </c>
       <c r="I403" s="9"/>
     </row>
@@ -12617,10 +12605,10 @@
         <v>43</v>
       </c>
       <c r="D404" s="8" t="s">
-        <v>369</v>
+        <v>339</v>
       </c>
       <c r="E404" s="8" t="s">
-        <v>362</v>
+        <v>329</v>
       </c>
       <c r="I404" s="9"/>
     </row>
@@ -12635,96 +12623,110 @@
         <v>43</v>
       </c>
       <c r="D405" s="8" t="s">
-        <v>339</v>
+        <v>519</v>
       </c>
       <c r="E405" s="8" t="s">
-        <v>329</v>
+        <v>526</v>
+      </c>
+      <c r="F405" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G405" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H405" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I405" s="9"/>
-    </row>
-    <row r="406" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A406" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B406" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C406" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D406" s="8" t="s">
-        <v>520</v>
-      </c>
-      <c r="E406" s="8" t="s">
-        <v>527</v>
-      </c>
-      <c r="F406" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G406" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H406" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I406" s="9"/>
-      <c r="J406" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="J405" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="408" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A408" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I408" s="4"/>
     </row>
     <row r="409" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A409" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I409" s="4"/>
     </row>
     <row r="410" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A410" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I410" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="B410" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C410" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D410" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E410" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F410" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G410" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H410" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I410" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J410" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="411" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I411" s="4"/>
+    </row>
+    <row r="412" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A412" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B411" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C411" s="3" t="s">
+      <c r="B412" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C412" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D411" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E411" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F411" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G411" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H411" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I411" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J411" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="412" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A412" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I412" s="4"/>
+      <c r="D412" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E412" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="F412" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G412" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H412" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I412" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="J412" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="413" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A413" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B413" s="8" t="s">
         <v>27</v>
@@ -12733,13 +12735,13 @@
         <v>48</v>
       </c>
       <c r="D413" s="8" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="E413" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F413" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G413" s="8" t="s">
         <v>26</v>
@@ -12748,7 +12750,7 @@
         <v>26</v>
       </c>
       <c r="I413" s="9" t="s">
-        <v>441</v>
+        <v>547</v>
       </c>
       <c r="J413" s="8" t="s">
         <v>26</v>
@@ -12768,10 +12770,10 @@
         <v>56</v>
       </c>
       <c r="E414" s="8" t="s">
-        <v>437</v>
+        <v>543</v>
       </c>
       <c r="F414" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G414" s="8" t="s">
         <v>26</v>
@@ -12780,7 +12782,7 @@
         <v>26</v>
       </c>
       <c r="I414" s="9" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="J414" s="8" t="s">
         <v>26</v>
@@ -12797,10 +12799,10 @@
         <v>48</v>
       </c>
       <c r="D415" s="8" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="E415" s="8" t="s">
-        <v>544</v>
+        <v>390</v>
       </c>
       <c r="F415" s="8" t="s">
         <v>26</v>
@@ -12812,10 +12814,7 @@
         <v>26</v>
       </c>
       <c r="I415" s="9" t="s">
-        <v>545</v>
-      </c>
-      <c r="J415" s="8" t="s">
-        <v>26</v>
+        <v>439</v>
       </c>
     </row>
     <row r="416" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12829,10 +12828,10 @@
         <v>48</v>
       </c>
       <c r="D416" s="8" t="s">
-        <v>124</v>
+        <v>520</v>
       </c>
       <c r="E416" s="8" t="s">
-        <v>390</v>
+        <v>521</v>
       </c>
       <c r="F416" s="8" t="s">
         <v>26</v>
@@ -12843,13 +12842,14 @@
       <c r="H416" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I416" s="9" t="s">
-        <v>440</v>
+      <c r="I416" s="9"/>
+      <c r="J416" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="417" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A417" s="8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B417" s="8" t="s">
         <v>27</v>
@@ -12858,28 +12858,19 @@
         <v>48</v>
       </c>
       <c r="D417" s="8" t="s">
-        <v>521</v>
+        <v>99</v>
       </c>
       <c r="E417" s="8" t="s">
-        <v>522</v>
+        <v>411</v>
       </c>
       <c r="F417" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G417" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H417" s="8" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I417" s="9"/>
-      <c r="J417" s="8" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="418" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A418" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B418" s="8" t="s">
         <v>27</v>
@@ -12888,10 +12879,10 @@
         <v>48</v>
       </c>
       <c r="D418" s="8" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="E418" s="8" t="s">
-        <v>412</v>
+        <v>210</v>
       </c>
       <c r="F418" s="8" t="s">
         <v>87</v>
@@ -12899,82 +12890,93 @@
       <c r="I418" s="9"/>
     </row>
     <row r="419" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A419" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B419" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C419" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D419" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E419" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="F419" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="I419" s="9"/>
     </row>
-    <row r="420" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I420" s="9"/>
+    <row r="420" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A420" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I420" s="4"/>
     </row>
     <row r="421" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A421" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I421" s="4"/>
     </row>
     <row r="422" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A422" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I422" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="B422" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C422" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D422" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E422" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F422" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G422" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H422" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I422" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J422" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="423" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A423" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B423" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C423" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I423" s="4"/>
+    </row>
+    <row r="424" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A424" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="B424" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C424" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D423" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E423" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F423" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G423" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H423" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I423" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J423" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="424" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A424" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I424" s="4"/>
+      <c r="D424" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E424" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="F424" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G424" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H424" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I424" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="J424" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="425" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A425" s="8" t="s">
-        <v>526</v>
+        <v>22</v>
       </c>
       <c r="B425" s="8" t="s">
         <v>27</v>
@@ -12983,13 +12985,13 @@
         <v>50</v>
       </c>
       <c r="D425" s="8" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="E425" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F425" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G425" s="8" t="s">
         <v>26</v>
@@ -12998,7 +13000,7 @@
         <v>26</v>
       </c>
       <c r="I425" s="9" t="s">
-        <v>439</v>
+        <v>548</v>
       </c>
       <c r="J425" s="8" t="s">
         <v>26</v>
@@ -13018,10 +13020,10 @@
         <v>56</v>
       </c>
       <c r="E426" s="8" t="s">
-        <v>438</v>
+        <v>545</v>
       </c>
       <c r="F426" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G426" s="8" t="s">
         <v>26</v>
@@ -13030,7 +13032,7 @@
         <v>26</v>
       </c>
       <c r="I426" s="9" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="J426" s="8" t="s">
         <v>26</v>
@@ -13047,10 +13049,10 @@
         <v>50</v>
       </c>
       <c r="D427" s="8" t="s">
-        <v>56</v>
+        <v>522</v>
       </c>
       <c r="E427" s="8" t="s">
-        <v>546</v>
+        <v>523</v>
       </c>
       <c r="F427" s="8" t="s">
         <v>26</v>
@@ -13061,53 +13063,21 @@
       <c r="H427" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I427" s="9" t="s">
-        <v>547</v>
-      </c>
+      <c r="I427" s="9"/>
       <c r="J427" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="428" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A428" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B428" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C428" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D428" s="8" t="s">
-        <v>523</v>
-      </c>
-      <c r="E428" s="8" t="s">
-        <v>524</v>
-      </c>
-      <c r="F428" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G428" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H428" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I428" s="9"/>
-      <c r="J428" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="429" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I429" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A361:A363">
+  <conditionalFormatting sqref="A360:A362">
     <cfRule type="containsText" dxfId="25" priority="149" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A361)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A360)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="24" priority="150" operator="beginsWith" text="#">
-      <formula>LEFT(A361,LEN("#"))="#"</formula>
+      <formula>LEFT(A360,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A300">
@@ -13142,7 +13112,7 @@
       <formula>LEFT(A318,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A421:A424 A336 A350:A353 B388:B406 B357 A381:A383 A358:B358 B359 B364:B386 B53:B60 B418:B419">
+  <conditionalFormatting sqref="A420:A423 A335 A349:A352 B387:B405 B356 A380:A382 A357:B357 B358 B363:B385 B53:B60 B417:B418 B319:B333">
     <cfRule type="containsText" priority="311" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13150,7 +13120,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B337 B339 B341 B343 B345 B347 B349 B314 B312 A354:B356">
+  <conditionalFormatting sqref="B336 B338 B340 B342 B344 B346 B348 B314 B312 A353:B355">
     <cfRule type="containsText" priority="287" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13158,7 +13128,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A337 A339 A341 A343 A345 A347 A349 A314 A312 B301 B296 B264">
+  <conditionalFormatting sqref="A336 A338 A340 A342 A344 A346 A348 A314 A312 B301 B296 B264">
     <cfRule type="containsText" priority="289" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13166,7 +13136,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B425 B427">
+  <conditionalFormatting sqref="B424 B426">
     <cfRule type="containsText" priority="203" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13174,7 +13144,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A425 A427">
+  <conditionalFormatting sqref="A424 A426">
     <cfRule type="containsText" priority="205" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13182,7 +13152,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A409:A412">
+  <conditionalFormatting sqref="A408:A411">
     <cfRule type="containsText" priority="2623" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13206,7 +13176,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A416 B306 B302">
+  <conditionalFormatting sqref="A415 B306 B302">
     <cfRule type="containsText" priority="2873" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13214,7 +13184,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A384:A386 A319:A334 A310 B311 A288:A292 A294 A299 B288:B295 A388:A405 A357 A359:A360 A364:A380 A418">
+  <conditionalFormatting sqref="A383:A385 A310 B311 A288:A292 A294 A299 B288:B295 A387:A404 A356 A358:A359 A363:A379 A417 A319:A333">
     <cfRule type="containsText" priority="2893" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13222,7 +13192,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A428">
+  <conditionalFormatting sqref="A427">
     <cfRule type="containsText" priority="3085" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13294,7 +13264,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A417">
+  <conditionalFormatting sqref="A416">
     <cfRule type="containsText" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13318,7 +13288,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B417">
+  <conditionalFormatting sqref="B416">
     <cfRule type="containsText" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13326,7 +13296,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B428 A315">
+  <conditionalFormatting sqref="B427 A315">
     <cfRule type="containsText" priority="4419" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13334,7 +13304,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A429 B415:B416 A415 A413:B413">
+  <conditionalFormatting sqref="A428 B414:B415 A414 A412:B412">
     <cfRule type="containsText" priority="4611" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13342,7 +13312,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A420 B308">
+  <conditionalFormatting sqref="A419 B308">
     <cfRule type="containsText" priority="4617" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13350,7 +13320,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B429">
+  <conditionalFormatting sqref="B428">
     <cfRule type="containsText" priority="4685" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13358,7 +13328,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B420">
+  <conditionalFormatting sqref="B419">
     <cfRule type="containsText" priority="5161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13366,7 +13336,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B360 B299 B310 B319:B334">
+  <conditionalFormatting sqref="B359 B299 B310">
     <cfRule type="containsText" priority="5455" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13374,7 +13344,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A406">
+  <conditionalFormatting sqref="A405">
     <cfRule type="containsText" priority="5473" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13406,7 +13376,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A335 A63:A85 A87:A91 A98:A133 A135:A139 A178:A182 A184:A189 A192:A194 A196:A208 A210:A215 A217 A220:A227 A231:A240 A243:A260 A267:A275 A277:A280 A265 A262 A142:A175">
+  <conditionalFormatting sqref="A334 A63:A85 A87:A91 A98:A133 A135:A139 A178:A182 A184:A189 A192:A194 A196:A208 A210:A215 A217 A220:A227 A231:A240 A243:A260 A267:A275 A277:A280 A265 A262 A142:A175">
     <cfRule type="containsText" dxfId="13" priority="5829" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13414,7 +13384,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B335 A303 A307 B63:B85 B87:B133 B135:B139 B178:B189 B192:B217 B220:B227 B231:B240 B243:B260 B267:B275 B277:B280 A86:B86 A93:A97 A183 A44:B44 B265 B262 B142:B175">
+  <conditionalFormatting sqref="B334 A303 A307 B63:B85 B87:B133 B135:B139 B178:B189 B192:B217 B220:B227 B231:B240 B243:B260 B267:B275 B277:B280 A86:B86 A93:A97 A183 A44:B44 B265 B262 B142:B175">
     <cfRule type="containsText" dxfId="11" priority="5849" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13462,7 +13432,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A414:B414">
+  <conditionalFormatting sqref="A413:B413">
     <cfRule type="containsText" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13470,7 +13440,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B426">
+  <conditionalFormatting sqref="B425">
     <cfRule type="containsText" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13478,7 +13448,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A426">
+  <conditionalFormatting sqref="A425">
     <cfRule type="containsText" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13550,7 +13520,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A387">
+  <conditionalFormatting sqref="A386">
     <cfRule type="containsText" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13558,7 +13528,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B387">
+  <conditionalFormatting sqref="B386">
     <cfRule type="containsText" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
+ I added more error checking. Previously, most of the errors returned by a routine were ignored by the calling routine. I am a little scared that this needs to be tested more, but the CertTest runs okay, so I'm going to commit anyway. + I fixed a problem with reading MulTabLoc (i haven't tested it, but the section that reads it should now be equivalent to FAST v7.02) + I moved IfW_Inputs to AD_OtherStates so that it doesn't have to be reallocated on every time step. I also removed the local InW_Inputs variables because they aren't necessary anymore.
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@102 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="562">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -1786,6 +1786,9 @@
   </si>
   <si>
     <t>0.0</t>
+  </si>
+  <si>
+    <t>"inputs to IfW module; set here so we don't have to recreate it every time"</t>
   </si>
 </sst>
 </file>
@@ -3054,8 +3057,8 @@
   <dimension ref="A1:K428"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A322" sqref="A322:XFD322"/>
+      <pane ySplit="15" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F340" sqref="F340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11398,7 +11401,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="353" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A353" s="8" t="s">
         <v>22</v>
       </c>
@@ -11421,7 +11424,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="354" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="8" t="s">
         <v>22</v>
       </c>
@@ -11444,7 +11447,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="355" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="8" t="s">
         <v>22</v>
       </c>
@@ -11473,7 +11476,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="356" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A356" s="8" t="s">
         <v>22</v>
       </c>
@@ -11491,7 +11494,7 @@
       </c>
       <c r="I356" s="9"/>
     </row>
-    <row r="357" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="8" t="s">
         <v>22</v>
       </c>
@@ -11518,7 +11521,7 @@
       </c>
       <c r="I357" s="9"/>
     </row>
-    <row r="358" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A358" s="8" t="s">
         <v>22</v>
       </c>
@@ -11547,48 +11550,62 @@
         <v>504</v>
       </c>
     </row>
-    <row r="359" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I359" s="9"/>
-    </row>
-    <row r="360" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A360" s="3" t="s">
+    <row r="359" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A359" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B359" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C359" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D359" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="E359" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="F359" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G359" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H359" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I359" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="J359" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I360" s="9"/>
+    </row>
+    <row r="361" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I360" s="4"/>
-    </row>
-    <row r="361" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A361" s="3" t="s">
+      <c r="I361" s="4"/>
+    </row>
+    <row r="362" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I361" s="4"/>
-    </row>
-    <row r="362" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A362" s="3" t="s">
+      <c r="I362" s="4"/>
+    </row>
+    <row r="363" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I362" s="4"/>
-    </row>
-    <row r="363" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A363" s="8" t="s">
+      <c r="I363" s="4"/>
+    </row>
+    <row r="364" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="B363" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C363" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D363" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E363" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I363" s="9"/>
-    </row>
-    <row r="364" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A364" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="B364" s="8" t="s">
         <v>27</v>
@@ -11597,25 +11614,14 @@
         <v>43</v>
       </c>
       <c r="D364" s="8" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="F364" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G364" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H364" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I364" s="9" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="365" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="I364" s="9"/>
+    </row>
+    <row r="365" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A365" s="8" t="s">
         <v>22</v>
       </c>
@@ -11629,7 +11635,7 @@
         <v>24</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F365" s="8" t="s">
         <v>26</v>
@@ -11641,10 +11647,10 @@
         <v>26</v>
       </c>
       <c r="I365" s="9" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="366" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A366" s="8" t="s">
         <v>22</v>
       </c>
@@ -11655,17 +11661,25 @@
         <v>43</v>
       </c>
       <c r="D366" s="8" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>409</v>
+        <v>384</v>
       </c>
       <c r="F366" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I366" s="9"/>
-    </row>
-    <row r="367" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G366" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H366" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I366" s="9" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A367" s="8" t="s">
         <v>22</v>
       </c>
@@ -11679,20 +11693,14 @@
         <v>99</v>
       </c>
       <c r="E367" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F367" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G367" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="H367" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I367" s="9"/>
     </row>
-    <row r="368" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A368" s="8" t="s">
         <v>22</v>
       </c>
@@ -11706,9 +11714,15 @@
         <v>99</v>
       </c>
       <c r="E368" s="8" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F368" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G368" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="H368" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I368" s="9"/>
@@ -11727,7 +11741,10 @@
         <v>99</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>388</v>
+        <v>412</v>
+      </c>
+      <c r="F369" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I369" s="9"/>
     </row>
@@ -11745,13 +11762,7 @@
         <v>99</v>
       </c>
       <c r="E370" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="F370" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G370" s="8" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="I370" s="9"/>
     </row>
@@ -11769,7 +11780,7 @@
         <v>99</v>
       </c>
       <c r="E371" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F371" s="8" t="s">
         <v>26</v>
@@ -11777,13 +11788,7 @@
       <c r="G371" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="H371" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I371" s="9"/>
-      <c r="J371" s="8" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="372" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A372" s="8" t="s">
@@ -11796,23 +11801,21 @@
         <v>43</v>
       </c>
       <c r="D372" s="8" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>100</v>
+        <v>414</v>
       </c>
       <c r="F372" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G372" s="8" t="s">
-        <v>26</v>
+        <v>399</v>
       </c>
       <c r="H372" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I372" s="9" t="s">
-        <v>501</v>
-      </c>
+      <c r="I372" s="9"/>
       <c r="J372" s="8" t="s">
         <v>26</v>
       </c>
@@ -11828,10 +11831,10 @@
         <v>43</v>
       </c>
       <c r="D373" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E373" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F373" s="8" t="s">
         <v>26</v>
@@ -11843,7 +11846,10 @@
         <v>26</v>
       </c>
       <c r="I373" s="9" t="s">
-        <v>484</v>
+        <v>501</v>
+      </c>
+      <c r="J373" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="374" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11860,7 +11866,7 @@
         <v>41</v>
       </c>
       <c r="E374" s="8" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F374" s="8" t="s">
         <v>26</v>
@@ -11872,7 +11878,7 @@
         <v>26</v>
       </c>
       <c r="I374" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="375" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11886,10 +11892,10 @@
         <v>43</v>
       </c>
       <c r="D375" s="8" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E375" s="8" t="s">
-        <v>389</v>
+        <v>90</v>
       </c>
       <c r="F375" s="8" t="s">
         <v>26</v>
@@ -11900,7 +11906,9 @@
       <c r="H375" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I375" s="9"/>
+      <c r="I375" s="9" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="376" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="8" t="s">
@@ -11916,7 +11924,7 @@
         <v>99</v>
       </c>
       <c r="E376" s="8" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
       <c r="F376" s="8" t="s">
         <v>26</v>
@@ -11927,9 +11935,7 @@
       <c r="H376" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I376" s="9" t="s">
-        <v>502</v>
-      </c>
+      <c r="I376" s="9"/>
     </row>
     <row r="377" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="8" t="s">
@@ -11945,7 +11951,7 @@
         <v>99</v>
       </c>
       <c r="E377" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F377" s="8" t="s">
         <v>26</v>
@@ -11957,7 +11963,7 @@
         <v>26</v>
       </c>
       <c r="I377" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="378" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11974,12 +11980,20 @@
         <v>99</v>
       </c>
       <c r="E378" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F378" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I378" s="9"/>
+      <c r="G378" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H378" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I378" s="9" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="379" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="8" t="s">
@@ -11995,20 +12009,12 @@
         <v>99</v>
       </c>
       <c r="E379" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F379" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G379" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H379" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I379" s="9" t="s">
-        <v>504</v>
-      </c>
+      <c r="I379" s="9"/>
     </row>
     <row r="380" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A380" s="8" t="s">
@@ -12024,7 +12030,7 @@
         <v>99</v>
       </c>
       <c r="E380" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F380" s="8" t="s">
         <v>26</v>
@@ -12036,7 +12042,7 @@
         <v>26</v>
       </c>
       <c r="I380" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="381" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12053,7 +12059,7 @@
         <v>99</v>
       </c>
       <c r="E381" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F381" s="8" t="s">
         <v>26</v>
@@ -12079,10 +12085,10 @@
         <v>43</v>
       </c>
       <c r="D382" s="8" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="E382" s="8" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F382" s="8" t="s">
         <v>26</v>
@@ -12094,7 +12100,7 @@
         <v>26</v>
       </c>
       <c r="I382" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="383" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12108,10 +12114,10 @@
         <v>43</v>
       </c>
       <c r="D383" s="8" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E383" s="8" t="s">
-        <v>101</v>
+        <v>423</v>
       </c>
       <c r="F383" s="8" t="s">
         <v>26</v>
@@ -12123,15 +12129,12 @@
         <v>26</v>
       </c>
       <c r="I383" s="9" t="s">
-        <v>507</v>
-      </c>
-      <c r="J383" s="8" t="s">
-        <v>103</v>
+        <v>506</v>
       </c>
     </row>
     <row r="384" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A384" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B384" s="8" t="s">
         <v>27</v>
@@ -12143,7 +12146,7 @@
         <v>34</v>
       </c>
       <c r="E384" s="8" t="s">
-        <v>424</v>
+        <v>101</v>
       </c>
       <c r="F384" s="8" t="s">
         <v>26</v>
@@ -12155,15 +12158,15 @@
         <v>26</v>
       </c>
       <c r="I384" s="9" t="s">
-        <v>454</v>
+        <v>507</v>
       </c>
       <c r="J384" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="385" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B385" s="8" t="s">
         <v>27</v>
@@ -12172,22 +12175,28 @@
         <v>43</v>
       </c>
       <c r="D385" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E385" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F385" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G385" s="8">
-        <v>19</v>
+      <c r="G385" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H385" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I385" s="9" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="386" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+      <c r="J385" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A386" s="8" t="s">
         <v>22</v>
       </c>
@@ -12201,17 +12210,19 @@
         <v>41</v>
       </c>
       <c r="E386" s="8" t="s">
-        <v>558</v>
+        <v>425</v>
       </c>
       <c r="F386" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G386" s="8" t="s">
-        <v>559</v>
-      </c>
-      <c r="I386" s="9"/>
-    </row>
-    <row r="387" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G386" s="8">
+        <v>19</v>
+      </c>
+      <c r="I386" s="9" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A387" s="8" t="s">
         <v>22</v>
       </c>
@@ -12225,17 +12236,17 @@
         <v>41</v>
       </c>
       <c r="E387" s="8" t="s">
-        <v>426</v>
+        <v>558</v>
       </c>
       <c r="F387" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G387" s="8">
-        <v>70</v>
+      <c r="G387" s="8" t="s">
+        <v>559</v>
       </c>
       <c r="I387" s="9"/>
     </row>
-    <row r="388" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A388" s="8" t="s">
         <v>22</v>
       </c>
@@ -12249,19 +12260,17 @@
         <v>41</v>
       </c>
       <c r="E388" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F388" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G388" s="8">
-        <v>90</v>
-      </c>
-      <c r="I388" s="9" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="389" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="I388" s="9"/>
+    </row>
+    <row r="389" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="8" t="s">
         <v>22</v>
       </c>
@@ -12275,19 +12284,19 @@
         <v>41</v>
       </c>
       <c r="E389" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F389" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G389" s="8">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I389" s="9" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="390" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="8" t="s">
         <v>22</v>
       </c>
@@ -12301,19 +12310,19 @@
         <v>41</v>
       </c>
       <c r="E390" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F390" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G390" s="8">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I390" s="9" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="391" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A391" s="8" t="s">
         <v>22</v>
       </c>
@@ -12327,19 +12336,19 @@
         <v>41</v>
       </c>
       <c r="E391" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F391" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G391" s="8">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I391" s="9" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="392" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="8" t="s">
         <v>22</v>
       </c>
@@ -12353,19 +12362,19 @@
         <v>41</v>
       </c>
       <c r="E392" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F392" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G392" s="8" t="s">
-        <v>559</v>
+      <c r="G392" s="8">
+        <v>93</v>
       </c>
       <c r="I392" s="9" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="393" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="8" t="s">
         <v>22</v>
       </c>
@@ -12379,22 +12388,19 @@
         <v>41</v>
       </c>
       <c r="E393" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F393" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G393" s="8">
-        <v>1000</v>
-      </c>
-      <c r="H393" s="8" t="s">
-        <v>26</v>
+      <c r="G393" s="8" t="s">
+        <v>559</v>
       </c>
       <c r="I393" s="9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="394" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="394" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="8" t="s">
         <v>22</v>
       </c>
@@ -12405,25 +12411,25 @@
         <v>43</v>
       </c>
       <c r="D394" s="8" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E394" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F394" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G394" s="8" t="s">
-        <v>397</v>
+      <c r="G394" s="8">
+        <v>1000</v>
       </c>
       <c r="H394" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I394" s="9" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="395" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="8" t="s">
         <v>22</v>
       </c>
@@ -12434,23 +12440,25 @@
         <v>43</v>
       </c>
       <c r="D395" s="8" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E395" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F395" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G395" s="8">
-        <v>-1</v>
+      <c r="G395" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="H395" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I395" s="9"/>
-    </row>
-    <row r="396" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I395" s="9" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="396" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A396" s="8" t="s">
         <v>22</v>
       </c>
@@ -12461,14 +12469,23 @@
         <v>43</v>
       </c>
       <c r="D396" s="8" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="E396" s="8" t="s">
-        <v>135</v>
+        <v>434</v>
+      </c>
+      <c r="F396" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G396" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H396" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I396" s="9"/>
     </row>
-    <row r="397" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A397" s="8" t="s">
         <v>22</v>
       </c>
@@ -12479,14 +12496,14 @@
         <v>43</v>
       </c>
       <c r="D397" s="8" t="s">
-        <v>227</v>
+        <v>141</v>
       </c>
       <c r="E397" s="8" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="I397" s="9"/>
     </row>
-    <row r="398" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A398" s="8" t="s">
         <v>22</v>
       </c>
@@ -12497,14 +12514,14 @@
         <v>43</v>
       </c>
       <c r="D398" s="8" t="s">
-        <v>538</v>
+        <v>227</v>
       </c>
       <c r="E398" s="8" t="s">
-        <v>537</v>
+        <v>125</v>
       </c>
       <c r="I398" s="9"/>
     </row>
-    <row r="399" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A399" s="8" t="s">
         <v>22</v>
       </c>
@@ -12515,14 +12532,14 @@
         <v>43</v>
       </c>
       <c r="D399" s="8" t="s">
-        <v>268</v>
+        <v>538</v>
       </c>
       <c r="E399" s="8" t="s">
-        <v>232</v>
+        <v>537</v>
       </c>
       <c r="I399" s="9"/>
     </row>
-    <row r="400" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A400" s="8" t="s">
         <v>22</v>
       </c>
@@ -12533,10 +12550,10 @@
         <v>43</v>
       </c>
       <c r="D400" s="8" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="E400" s="8" t="s">
-        <v>278</v>
+        <v>232</v>
       </c>
       <c r="I400" s="9"/>
     </row>
@@ -12551,10 +12568,10 @@
         <v>43</v>
       </c>
       <c r="D401" s="8" t="s">
-        <v>342</v>
+        <v>286</v>
       </c>
       <c r="E401" s="8" t="s">
-        <v>341</v>
+        <v>278</v>
       </c>
       <c r="I401" s="9"/>
     </row>
@@ -12569,10 +12586,10 @@
         <v>43</v>
       </c>
       <c r="D402" s="8" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="E402" s="8" t="s">
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="I402" s="9"/>
     </row>
@@ -12587,10 +12604,10 @@
         <v>43</v>
       </c>
       <c r="D403" s="8" t="s">
-        <v>369</v>
+        <v>321</v>
       </c>
       <c r="E403" s="8" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="I403" s="9"/>
     </row>
@@ -12605,10 +12622,10 @@
         <v>43</v>
       </c>
       <c r="D404" s="8" t="s">
-        <v>339</v>
+        <v>369</v>
       </c>
       <c r="E404" s="8" t="s">
-        <v>329</v>
+        <v>362</v>
       </c>
       <c r="I404" s="9"/>
     </row>
@@ -12623,110 +12640,96 @@
         <v>43</v>
       </c>
       <c r="D405" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E405" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="I405" s="9"/>
+    </row>
+    <row r="406" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A406" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B406" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C406" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D406" s="8" t="s">
         <v>519</v>
       </c>
-      <c r="E405" s="8" t="s">
+      <c r="E406" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="F405" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G405" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H405" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I405" s="9"/>
-      <c r="J405" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="408" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A408" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I408" s="4"/>
+      <c r="F406" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G406" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H406" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I406" s="9"/>
+      <c r="J406" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="409" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A409" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I409" s="4"/>
     </row>
     <row r="410" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A410" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B410" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C410" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D410" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E410" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F410" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G410" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H410" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I410" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J410" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I410" s="4"/>
     </row>
     <row r="411" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B411" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C411" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D411" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E411" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F411" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G411" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H411" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I411" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J411" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="412" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A412" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I411" s="4"/>
-    </row>
-    <row r="412" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A412" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B412" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C412" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D412" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E412" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="F412" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G412" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H412" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I412" s="9" t="s">
-        <v>440</v>
-      </c>
-      <c r="J412" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="I412" s="4"/>
     </row>
     <row r="413" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A413" s="8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B413" s="8" t="s">
         <v>27</v>
@@ -12735,13 +12738,13 @@
         <v>48</v>
       </c>
       <c r="D413" s="8" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="E413" s="8" t="s">
         <v>436</v>
       </c>
       <c r="F413" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G413" s="8" t="s">
         <v>26</v>
@@ -12750,7 +12753,7 @@
         <v>26</v>
       </c>
       <c r="I413" s="9" t="s">
-        <v>547</v>
+        <v>440</v>
       </c>
       <c r="J413" s="8" t="s">
         <v>26</v>
@@ -12770,10 +12773,10 @@
         <v>56</v>
       </c>
       <c r="E414" s="8" t="s">
-        <v>543</v>
+        <v>436</v>
       </c>
       <c r="F414" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G414" s="8" t="s">
         <v>26</v>
@@ -12782,7 +12785,7 @@
         <v>26</v>
       </c>
       <c r="I414" s="9" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="J414" s="8" t="s">
         <v>26</v>
@@ -12799,10 +12802,10 @@
         <v>48</v>
       </c>
       <c r="D415" s="8" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="E415" s="8" t="s">
-        <v>390</v>
+        <v>543</v>
       </c>
       <c r="F415" s="8" t="s">
         <v>26</v>
@@ -12814,7 +12817,10 @@
         <v>26</v>
       </c>
       <c r="I415" s="9" t="s">
-        <v>439</v>
+        <v>544</v>
+      </c>
+      <c r="J415" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="416" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12828,10 +12834,10 @@
         <v>48</v>
       </c>
       <c r="D416" s="8" t="s">
-        <v>520</v>
+        <v>124</v>
       </c>
       <c r="E416" s="8" t="s">
-        <v>521</v>
+        <v>390</v>
       </c>
       <c r="F416" s="8" t="s">
         <v>26</v>
@@ -12842,9 +12848,8 @@
       <c r="H416" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I416" s="9"/>
-      <c r="J416" s="8" t="s">
-        <v>26</v>
+      <c r="I416" s="9" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="417" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -13072,12 +13077,12 @@
       <c r="I428" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A360:A362">
+  <conditionalFormatting sqref="A361:A363">
     <cfRule type="containsText" dxfId="25" priority="149" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A360)))</formula>
+      <formula>NOT(ISERROR(SEARCH("......",A361)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="24" priority="150" operator="beginsWith" text="#">
-      <formula>LEFT(A360,LEN("#"))="#"</formula>
+      <formula>LEFT(A361,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A300">
@@ -13112,7 +13117,7 @@
       <formula>LEFT(A318,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A420:A423 A335 A349:A352 B387:B405 B356 A380:A382 A357:B357 B358 B363:B385 B53:B60 B417:B418 B319:B333">
+  <conditionalFormatting sqref="A420:A423 A335 A349:A352 B388:B406 B356 A381:A383 A357:B357 B358 B364:B386 B53:B60 B417:B418 B319:B333">
     <cfRule type="containsText" priority="311" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13152,7 +13157,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A408:A411">
+  <conditionalFormatting sqref="A409:A412">
     <cfRule type="containsText" priority="2623" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13176,7 +13181,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A415 B306 B302">
+  <conditionalFormatting sqref="A416 B306 B302">
     <cfRule type="containsText" priority="2873" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13184,7 +13189,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A383:A385 A310 B311 A288:A292 A294 A299 B288:B295 A387:A404 A356 A358:A359 A363:A379 A417 A319:A333">
+  <conditionalFormatting sqref="A384:A386 A310 B311 A288:A292 A294 A299 B288:B295 A388:A405 A356 A358 A364:A380 A417 A319:A333 A360">
     <cfRule type="containsText" priority="2893" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13264,7 +13269,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A416">
+  <conditionalFormatting sqref="A359">
     <cfRule type="containsText" priority="77" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13288,7 +13293,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B416">
+  <conditionalFormatting sqref="B359">
     <cfRule type="containsText" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13304,7 +13309,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A428 B414:B415 A414 A412:B412">
+  <conditionalFormatting sqref="A428 B415:B416 A415 A413:B413">
     <cfRule type="containsText" priority="4611" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13336,7 +13341,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B359 B299 B310">
+  <conditionalFormatting sqref="B360 B299 B310">
     <cfRule type="containsText" priority="5455" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13344,7 +13349,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A405">
+  <conditionalFormatting sqref="A406">
     <cfRule type="containsText" priority="5473" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13432,7 +13437,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A413:B413">
+  <conditionalFormatting sqref="A414:B414">
     <cfRule type="containsText" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13520,7 +13525,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A386">
+  <conditionalFormatting sqref="A387">
     <cfRule type="containsText" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13528,7 +13533,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B386">
+  <conditionalFormatting sqref="B387">
     <cfRule type="containsText" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
+ I cleaned up a few more things in the Init routine. + I got rid of  p%Blade%NB because it's the same as p%NumBl + I added an option to specify "default" as the time step in the input file, which will then use the value from the FAST glue code
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@103 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -3057,8 +3057,8 @@
   <dimension ref="A1:K428"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F340" sqref="F340"/>
+      <pane ySplit="15" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6377,7 +6377,7 @@
     </row>
     <row r="139" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
+ renamed the opt file to <RootName>.AD.sum + renamed the time-series output file from .elm to <RootName>.AD.out + fixed some more error handling + updated formatting in the summary file (opt) + removed some unnecessary variables
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@104 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="557">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -1363,21 +1363,6 @@
   </si>
   <si>
     <t>UnEc</t>
-  </si>
-  <si>
-    <t>UnADPlt</t>
-  </si>
-  <si>
-    <t>UnADin</t>
-  </si>
-  <si>
-    <t>UnWind</t>
-  </si>
-  <si>
-    <t>UnADopt</t>
-  </si>
-  <si>
-    <t>UnAirfl</t>
   </si>
   <si>
     <t>UnWndOut</t>
@@ -3054,11 +3039,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K428"/>
+  <dimension ref="A1:K423"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A140" sqref="A140"/>
+      <pane ySplit="15" topLeftCell="A376" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G387" sqref="G387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,19 +3099,19 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -3208,10 +3193,10 @@
     </row>
     <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -3240,7 +3225,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>26</v>
@@ -3270,7 +3255,7 @@
         <v>117</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>26</v>
@@ -3300,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>26</v>
@@ -3330,7 +3315,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>26</v>
@@ -4136,7 +4121,7 @@
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="I62" s="4"/>
     </row>
@@ -4148,7 +4133,7 @@
         <v>27</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>34</v>
@@ -4178,7 +4163,7 @@
         <v>27</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>34</v>
@@ -4208,7 +4193,7 @@
         <v>27</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>34</v>
@@ -4238,7 +4223,7 @@
         <v>27</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>34</v>
@@ -4268,7 +4253,7 @@
         <v>27</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>34</v>
@@ -4298,7 +4283,7 @@
         <v>27</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>34</v>
@@ -4328,7 +4313,7 @@
         <v>27</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>34</v>
@@ -4358,7 +4343,7 @@
         <v>27</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>34</v>
@@ -4388,7 +4373,7 @@
         <v>27</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>34</v>
@@ -4418,7 +4403,7 @@
         <v>27</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>99</v>
@@ -4448,7 +4433,7 @@
         <v>27</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>99</v>
@@ -4478,7 +4463,7 @@
         <v>27</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>34</v>
@@ -4508,7 +4493,7 @@
         <v>27</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>34</v>
@@ -4538,7 +4523,7 @@
         <v>27</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>34</v>
@@ -4568,7 +4553,7 @@
         <v>27</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>34</v>
@@ -4598,7 +4583,7 @@
         <v>27</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>34</v>
@@ -4628,7 +4613,7 @@
         <v>27</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>34</v>
@@ -4658,7 +4643,7 @@
         <v>27</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>34</v>
@@ -4688,7 +4673,7 @@
         <v>27</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>34</v>
@@ -4718,7 +4703,7 @@
         <v>27</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>34</v>
@@ -4748,7 +4733,7 @@
         <v>27</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>34</v>
@@ -4778,7 +4763,7 @@
         <v>27</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>34</v>
@@ -4808,7 +4793,7 @@
         <v>27</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>34</v>
@@ -4838,7 +4823,7 @@
         <v>27</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>34</v>
@@ -4868,7 +4853,7 @@
         <v>27</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>34</v>
@@ -4898,7 +4883,7 @@
         <v>27</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>34</v>
@@ -4928,7 +4913,7 @@
         <v>27</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>34</v>
@@ -4958,7 +4943,7 @@
         <v>27</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>34</v>
@@ -4988,7 +4973,7 @@
         <v>27</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>34</v>
@@ -5018,7 +5003,7 @@
         <v>27</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>34</v>
@@ -5048,7 +5033,7 @@
         <v>27</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>34</v>
@@ -5078,7 +5063,7 @@
         <v>27</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>34</v>
@@ -5108,7 +5093,7 @@
         <v>27</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>34</v>
@@ -5138,7 +5123,7 @@
         <v>27</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>34</v>
@@ -5168,7 +5153,7 @@
         <v>27</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>34</v>
@@ -5198,7 +5183,7 @@
         <v>27</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>34</v>
@@ -5228,7 +5213,7 @@
         <v>27</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>34</v>
@@ -5258,7 +5243,7 @@
         <v>27</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>34</v>
@@ -5288,7 +5273,7 @@
         <v>27</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>34</v>
@@ -5318,7 +5303,7 @@
         <v>27</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>34</v>
@@ -5348,7 +5333,7 @@
         <v>27</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>34</v>
@@ -5378,7 +5363,7 @@
         <v>27</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>34</v>
@@ -5408,7 +5393,7 @@
         <v>27</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>34</v>
@@ -5438,7 +5423,7 @@
         <v>27</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>34</v>
@@ -5468,7 +5453,7 @@
         <v>27</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>34</v>
@@ -5498,7 +5483,7 @@
         <v>27</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>34</v>
@@ -5528,7 +5513,7 @@
         <v>27</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>34</v>
@@ -5558,7 +5543,7 @@
         <v>27</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>34</v>
@@ -5588,7 +5573,7 @@
         <v>27</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>34</v>
@@ -5618,7 +5603,7 @@
         <v>27</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>34</v>
@@ -5648,7 +5633,7 @@
         <v>27</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>34</v>
@@ -5678,7 +5663,7 @@
         <v>27</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>34</v>
@@ -5708,7 +5693,7 @@
         <v>27</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>34</v>
@@ -5738,7 +5723,7 @@
         <v>27</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>34</v>
@@ -5768,7 +5753,7 @@
         <v>27</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>34</v>
@@ -5798,7 +5783,7 @@
         <v>27</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>34</v>
@@ -5828,7 +5813,7 @@
         <v>27</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>34</v>
@@ -5858,7 +5843,7 @@
         <v>27</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>34</v>
@@ -5888,7 +5873,7 @@
         <v>27</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>34</v>
@@ -5918,7 +5903,7 @@
         <v>27</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>34</v>
@@ -5948,7 +5933,7 @@
         <v>27</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>34</v>
@@ -5978,7 +5963,7 @@
         <v>27</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>34</v>
@@ -6008,7 +5993,7 @@
         <v>27</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>34</v>
@@ -6038,7 +6023,7 @@
         <v>27</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>34</v>
@@ -6070,7 +6055,7 @@
         <v>27</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D127" s="8" t="s">
         <v>34</v>
@@ -6102,7 +6087,7 @@
         <v>27</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>34</v>
@@ -6134,7 +6119,7 @@
         <v>27</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>34</v>
@@ -6166,7 +6151,7 @@
         <v>27</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>34</v>
@@ -6198,7 +6183,7 @@
         <v>27</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>99</v>
@@ -6228,7 +6213,7 @@
         <v>27</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>99</v>
@@ -6255,7 +6240,7 @@
     </row>
     <row r="134" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I134" s="4"/>
     </row>
@@ -6285,7 +6270,7 @@
         <v>26</v>
       </c>
       <c r="I135" s="9" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="136" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6314,7 +6299,7 @@
         <v>26</v>
       </c>
       <c r="I136" s="9" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="137" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6343,7 +6328,7 @@
         <v>26</v>
       </c>
       <c r="I137" s="9" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="138" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6372,7 +6357,7 @@
         <v>26</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="139" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6401,12 +6386,12 @@
         <v>26</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="141" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I141" s="4"/>
     </row>
@@ -7180,7 +7165,7 @@
         <v>26</v>
       </c>
       <c r="I171" s="9" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7209,7 +7194,7 @@
         <v>26</v>
       </c>
       <c r="I172" s="9" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="173" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7295,7 +7280,7 @@
     </row>
     <row r="177" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="I177" s="4"/>
     </row>
@@ -7449,7 +7434,7 @@
         <v>26</v>
       </c>
       <c r="K182" s="8" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="183" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7482,7 +7467,7 @@
         <v>26</v>
       </c>
       <c r="K183" s="8" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="184" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7667,7 +7652,7 @@
     </row>
     <row r="191" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="I191" s="4"/>
     </row>
@@ -8297,7 +8282,7 @@
         <v>26</v>
       </c>
       <c r="I212" s="9" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="213" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8446,12 +8431,12 @@
         <v>26</v>
       </c>
       <c r="I217" s="9" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="219" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I219" s="4"/>
     </row>
@@ -8508,7 +8493,7 @@
         <v>26</v>
       </c>
       <c r="I221" s="9" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="J221" s="8" t="s">
         <v>26</v>
@@ -8540,7 +8525,7 @@
         <v>26</v>
       </c>
       <c r="I222" s="9" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="223" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8569,7 +8554,7 @@
         <v>26</v>
       </c>
       <c r="I223" s="9" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="224" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8598,7 +8583,7 @@
         <v>26</v>
       </c>
       <c r="I224" s="9" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="225" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8627,7 +8612,7 @@
         <v>26</v>
       </c>
       <c r="I225" s="9" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="226" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8656,7 +8641,7 @@
         <v>26</v>
       </c>
       <c r="I226" s="9" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="227" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8685,12 +8670,12 @@
         <v>26</v>
       </c>
       <c r="I227" s="9" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="230" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="I230" s="4"/>
     </row>
@@ -8720,7 +8705,7 @@
         <v>26</v>
       </c>
       <c r="I231" s="9" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="232" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8968,7 +8953,7 @@
     </row>
     <row r="242" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I242" s="4"/>
     </row>
@@ -9160,7 +9145,7 @@
         <v>26</v>
       </c>
       <c r="I249" s="9" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="250" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9189,7 +9174,7 @@
         <v>26</v>
       </c>
       <c r="I250" s="9" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="251" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9218,7 +9203,7 @@
         <v>26</v>
       </c>
       <c r="I251" s="9" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="252" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9247,7 +9232,7 @@
         <v>26</v>
       </c>
       <c r="I252" s="9" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="253" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9276,7 +9261,7 @@
         <v>26</v>
       </c>
       <c r="I253" s="9" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="254" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9305,7 +9290,7 @@
         <v>26</v>
       </c>
       <c r="I254" s="9" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="255" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9334,7 +9319,7 @@
         <v>26</v>
       </c>
       <c r="I255" s="9" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="J255" s="8" t="s">
         <v>103</v>
@@ -9366,7 +9351,7 @@
         <v>26</v>
       </c>
       <c r="I256" s="9" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="257" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9395,7 +9380,7 @@
         <v>26</v>
       </c>
       <c r="I257" s="9" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="258" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9424,7 +9409,7 @@
         <v>26</v>
       </c>
       <c r="I258" s="9" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="259" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9453,7 +9438,7 @@
         <v>26</v>
       </c>
       <c r="I259" s="9" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="260" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9482,7 +9467,7 @@
         <v>26</v>
       </c>
       <c r="I260" s="9" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="261" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9511,7 +9496,7 @@
         <v>26</v>
       </c>
       <c r="I261" s="9" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J261" s="8" t="s">
         <v>103</v>
@@ -9531,7 +9516,7 @@
         <v>99</v>
       </c>
       <c r="E262" s="8" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="F262" s="8" t="s">
         <v>26</v>
@@ -9543,7 +9528,7 @@
         <v>26</v>
       </c>
       <c r="I262" s="9" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="J262" s="8" t="s">
         <v>103</v>
@@ -9563,7 +9548,7 @@
         <v>41</v>
       </c>
       <c r="E263" s="8" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="F263" s="8" t="s">
         <v>26</v>
@@ -9575,7 +9560,7 @@
         <v>26</v>
       </c>
       <c r="I263" s="9" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="264" spans="1:10" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -9592,7 +9577,7 @@
         <v>34</v>
       </c>
       <c r="E264" s="8" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="F264" s="8" t="s">
         <v>31</v>
@@ -9604,7 +9589,7 @@
         <v>26</v>
       </c>
       <c r="I264" s="9" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="J264" s="8" t="s">
         <v>26</v>
@@ -9615,7 +9600,7 @@
     </row>
     <row r="266" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="I266" s="4"/>
     </row>
@@ -9807,7 +9792,7 @@
         <v>26</v>
       </c>
       <c r="I273" s="9" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="J273" s="8" t="s">
         <v>371</v>
@@ -9839,7 +9824,7 @@
         <v>26</v>
       </c>
       <c r="I274" s="9" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="J274" s="8" t="s">
         <v>373</v>
@@ -9895,7 +9880,7 @@
         <v>26</v>
       </c>
       <c r="I278" s="9" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="279" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9924,7 +9909,7 @@
         <v>26</v>
       </c>
       <c r="I279" s="9" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="280" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9995,7 +9980,7 @@
         <v>26</v>
       </c>
       <c r="I284" s="9" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="285" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10012,7 +9997,7 @@
         <v>24</v>
       </c>
       <c r="E285" s="8" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="F285" s="8" t="s">
         <v>26</v>
@@ -10039,7 +10024,7 @@
         <v>24</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="F286" s="8" t="s">
         <v>26</v>
@@ -10051,7 +10036,7 @@
         <v>26</v>
       </c>
       <c r="I286" s="9" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="287" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10080,7 +10065,7 @@
         <v>26</v>
       </c>
       <c r="I287" s="9" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="288" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10109,7 +10094,7 @@
         <v>26</v>
       </c>
       <c r="I288" s="9" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="289" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10138,7 +10123,7 @@
         <v>26</v>
       </c>
       <c r="I289" s="9" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="290" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10167,7 +10152,7 @@
         <v>26</v>
       </c>
       <c r="I290" s="9" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="291" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10196,7 +10181,7 @@
         <v>26</v>
       </c>
       <c r="I291" s="9" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="292" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10225,7 +10210,7 @@
         <v>26</v>
       </c>
       <c r="I292" s="9" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="293" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10254,7 +10239,7 @@
         <v>26</v>
       </c>
       <c r="I293" s="9" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="294" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10283,7 +10268,7 @@
         <v>26</v>
       </c>
       <c r="I294" s="9" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="295" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10348,7 +10333,7 @@
         <v>41</v>
       </c>
       <c r="E297" s="8" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="F297" s="8" t="s">
         <v>26</v>
@@ -10360,7 +10345,7 @@
         <v>26</v>
       </c>
       <c r="I297" s="9" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="298" spans="1:10" s="8" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -10377,7 +10362,7 @@
         <v>34</v>
       </c>
       <c r="E298" s="8" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="F298" s="8" t="s">
         <v>87</v>
@@ -10389,7 +10374,7 @@
         <v>26</v>
       </c>
       <c r="I298" s="9" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="J298" s="8" t="s">
         <v>26</v>
@@ -10406,10 +10391,10 @@
         <v>23</v>
       </c>
       <c r="D299" s="8" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="E299" s="8" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="F299" s="8" t="s">
         <v>26</v>
@@ -10457,7 +10442,7 @@
         <v>26</v>
       </c>
       <c r="I301" s="9" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="302" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10471,10 +10456,10 @@
         <v>28</v>
       </c>
       <c r="D302" s="8" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="E302" s="8" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="F302" s="8" t="s">
         <v>26</v>
@@ -10546,10 +10531,10 @@
         <v>33</v>
       </c>
       <c r="D307" s="8" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="E307" s="8" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="F307" s="8" t="s">
         <v>26</v>
@@ -10615,10 +10600,10 @@
         <v>36</v>
       </c>
       <c r="D311" s="8" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="E311" s="8" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="F311" s="8" t="s">
         <v>26</v>
@@ -10684,10 +10669,10 @@
         <v>38</v>
       </c>
       <c r="D315" s="8" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="E315" s="8" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="F315" s="8" t="s">
         <v>26</v>
@@ -10708,7 +10693,7 @@
     </row>
     <row r="317" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="318" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10773,7 +10758,7 @@
         <v>26</v>
       </c>
       <c r="I320" s="9" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="J320" s="8" t="s">
         <v>46</v>
@@ -10862,7 +10847,7 @@
         <v>26</v>
       </c>
       <c r="I323" s="9" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="324" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10891,7 +10876,7 @@
         <v>26</v>
       </c>
       <c r="I324" s="9" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="325" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10920,7 +10905,7 @@
         <v>26</v>
       </c>
       <c r="I325" s="9" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="326" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10949,7 +10934,7 @@
         <v>26</v>
       </c>
       <c r="I326" s="9" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="327" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10978,7 +10963,7 @@
         <v>26</v>
       </c>
       <c r="I327" s="9" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="328" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11007,7 +10992,7 @@
         <v>26</v>
       </c>
       <c r="I328" s="9" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="329" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11036,7 +11021,7 @@
         <v>26</v>
       </c>
       <c r="I329" s="9" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="330" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11065,7 +11050,7 @@
         <v>26</v>
       </c>
       <c r="I330" s="9" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="331" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11153,7 +11138,7 @@
         <v>26</v>
       </c>
       <c r="I333" s="9" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="334" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11167,10 +11152,10 @@
         <v>40</v>
       </c>
       <c r="D334" s="8" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E334" s="8" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="F334" s="8" t="s">
         <v>26</v>
@@ -11188,7 +11173,7 @@
     </row>
     <row r="335" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A335" s="3" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I335" s="4"/>
     </row>
@@ -11212,7 +11197,7 @@
     </row>
     <row r="337" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="I337" s="4"/>
     </row>
@@ -11227,16 +11212,16 @@
         <v>40</v>
       </c>
       <c r="D338" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="E338" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="I338" s="9"/>
     </row>
     <row r="339" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A339" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I339" s="4"/>
     </row>
@@ -11260,7 +11245,7 @@
     </row>
     <row r="341" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="I341" s="4"/>
     </row>
@@ -11284,7 +11269,7 @@
     </row>
     <row r="343" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A343" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="I343" s="4"/>
     </row>
@@ -11308,7 +11293,7 @@
     </row>
     <row r="345" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="I345" s="4"/>
     </row>
@@ -11332,7 +11317,7 @@
     </row>
     <row r="347" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I347" s="4"/>
     </row>
@@ -11362,13 +11347,13 @@
     </row>
     <row r="350" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="I350" s="4"/>
     </row>
     <row r="351" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="I351" s="4"/>
     </row>
@@ -11398,7 +11383,7 @@
         <v>26</v>
       </c>
       <c r="I352" s="11" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="353" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11421,7 +11406,7 @@
         <v>88</v>
       </c>
       <c r="I353" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="354" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11444,7 +11429,7 @@
         <v>88</v>
       </c>
       <c r="I354" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="355" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11461,7 +11446,7 @@
         <v>99</v>
       </c>
       <c r="E355" s="8" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="F355" s="8" t="s">
         <v>26</v>
@@ -11473,7 +11458,7 @@
         <v>26</v>
       </c>
       <c r="I355" s="8" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="356" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11490,7 +11475,7 @@
         <v>292</v>
       </c>
       <c r="E356" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I356" s="9"/>
     </row>
@@ -11547,7 +11532,7 @@
         <v>26</v>
       </c>
       <c r="I358" s="9" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="359" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11561,10 +11546,10 @@
         <v>40</v>
       </c>
       <c r="D359" s="8" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E359" s="8" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="F359" s="8" t="s">
         <v>26</v>
@@ -11576,7 +11561,7 @@
         <v>26</v>
       </c>
       <c r="I359" s="9" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="J359" s="8" t="s">
         <v>26</v>
@@ -11647,7 +11632,7 @@
         <v>26</v>
       </c>
       <c r="I365" s="9" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="366" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11676,7 +11661,7 @@
         <v>26</v>
       </c>
       <c r="I366" s="9" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="367" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11846,7 +11831,7 @@
         <v>26</v>
       </c>
       <c r="I373" s="9" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="J373" s="8" t="s">
         <v>26</v>
@@ -11878,7 +11863,7 @@
         <v>26</v>
       </c>
       <c r="I374" s="9" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="375" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11907,7 +11892,7 @@
         <v>26</v>
       </c>
       <c r="I375" s="9" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="376" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11963,7 +11948,7 @@
         <v>26</v>
       </c>
       <c r="I377" s="9" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="378" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11992,7 +11977,7 @@
         <v>26</v>
       </c>
       <c r="I378" s="9" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="379" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12042,7 +12027,7 @@
         <v>26</v>
       </c>
       <c r="I380" s="9" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="381" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12071,7 +12056,7 @@
         <v>26</v>
       </c>
       <c r="I381" s="9" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="382" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12100,7 +12085,7 @@
         <v>26</v>
       </c>
       <c r="I382" s="9" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="383" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12129,7 +12114,7 @@
         <v>26</v>
       </c>
       <c r="I383" s="9" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="384" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12158,7 +12143,7 @@
         <v>26</v>
       </c>
       <c r="I384" s="9" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="J384" s="8" t="s">
         <v>103</v>
@@ -12190,7 +12175,7 @@
         <v>26</v>
       </c>
       <c r="I385" s="9" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="J385" s="8" t="s">
         <v>103</v>
@@ -12215,11 +12200,11 @@
       <c r="F386" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G386" s="8">
-        <v>19</v>
+      <c r="G386" s="8" t="s">
+        <v>554</v>
       </c>
       <c r="I386" s="9" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="387" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12236,13 +12221,13 @@
         <v>41</v>
       </c>
       <c r="E387" s="8" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="F387" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G387" s="8" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="I387" s="9"/>
     </row>
@@ -12265,10 +12250,12 @@
       <c r="F388" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G388" s="8">
-        <v>70</v>
-      </c>
-      <c r="I388" s="9"/>
+      <c r="G388" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="I388" s="9" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="389" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="8" t="s">
@@ -12290,10 +12277,13 @@
         <v>26</v>
       </c>
       <c r="G389" s="8">
-        <v>90</v>
+        <v>1000</v>
+      </c>
+      <c r="H389" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I389" s="9" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="390" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12307,7 +12297,7 @@
         <v>43</v>
       </c>
       <c r="D390" s="8" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="E390" s="8" t="s">
         <v>428</v>
@@ -12315,11 +12305,14 @@
       <c r="F390" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G390" s="8">
-        <v>91</v>
+      <c r="G390" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="H390" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I390" s="9" t="s">
-        <v>509</v>
+        <v>478</v>
       </c>
     </row>
     <row r="391" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12333,7 +12326,7 @@
         <v>43</v>
       </c>
       <c r="D391" s="8" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="E391" s="8" t="s">
         <v>429</v>
@@ -12342,11 +12335,12 @@
         <v>26</v>
       </c>
       <c r="G391" s="8">
-        <v>92</v>
-      </c>
-      <c r="I391" s="9" t="s">
-        <v>509</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="H391" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I391" s="9"/>
     </row>
     <row r="392" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="8" t="s">
@@ -12359,20 +12353,12 @@
         <v>43</v>
       </c>
       <c r="D392" s="8" t="s">
-        <v>41</v>
+        <v>141</v>
       </c>
       <c r="E392" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="F392" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G392" s="8">
-        <v>93</v>
-      </c>
-      <c r="I392" s="9" t="s">
-        <v>509</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="I392" s="9"/>
     </row>
     <row r="393" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="8" t="s">
@@ -12385,20 +12371,12 @@
         <v>43</v>
       </c>
       <c r="D393" s="8" t="s">
-        <v>41</v>
+        <v>227</v>
       </c>
       <c r="E393" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="F393" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G393" s="8" t="s">
-        <v>559</v>
-      </c>
-      <c r="I393" s="9" t="s">
-        <v>509</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="I393" s="9"/>
     </row>
     <row r="394" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="8" t="s">
@@ -12411,23 +12389,12 @@
         <v>43</v>
       </c>
       <c r="D394" s="8" t="s">
-        <v>41</v>
+        <v>533</v>
       </c>
       <c r="E394" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="F394" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G394" s="8">
-        <v>1000</v>
-      </c>
-      <c r="H394" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I394" s="9" t="s">
-        <v>510</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="I394" s="9"/>
     </row>
     <row r="395" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="8" t="s">
@@ -12440,23 +12407,12 @@
         <v>43</v>
       </c>
       <c r="D395" s="8" t="s">
-        <v>99</v>
+        <v>268</v>
       </c>
       <c r="E395" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="F395" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G395" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="H395" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I395" s="9" t="s">
-        <v>483</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="I395" s="9"/>
     </row>
     <row r="396" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A396" s="8" t="s">
@@ -12469,19 +12425,10 @@
         <v>43</v>
       </c>
       <c r="D396" s="8" t="s">
-        <v>89</v>
+        <v>286</v>
       </c>
       <c r="E396" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="F396" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G396" s="8">
-        <v>-1</v>
-      </c>
-      <c r="H396" s="8" t="s">
-        <v>26</v>
+        <v>278</v>
       </c>
       <c r="I396" s="9"/>
     </row>
@@ -12496,10 +12443,10 @@
         <v>43</v>
       </c>
       <c r="D397" s="8" t="s">
-        <v>141</v>
+        <v>342</v>
       </c>
       <c r="E397" s="8" t="s">
-        <v>135</v>
+        <v>341</v>
       </c>
       <c r="I397" s="9"/>
     </row>
@@ -12514,10 +12461,10 @@
         <v>43</v>
       </c>
       <c r="D398" s="8" t="s">
-        <v>227</v>
+        <v>321</v>
       </c>
       <c r="E398" s="8" t="s">
-        <v>125</v>
+        <v>319</v>
       </c>
       <c r="I398" s="9"/>
     </row>
@@ -12532,10 +12479,10 @@
         <v>43</v>
       </c>
       <c r="D399" s="8" t="s">
-        <v>538</v>
+        <v>369</v>
       </c>
       <c r="E399" s="8" t="s">
-        <v>537</v>
+        <v>362</v>
       </c>
       <c r="I399" s="9"/>
     </row>
@@ -12550,10 +12497,10 @@
         <v>43</v>
       </c>
       <c r="D400" s="8" t="s">
-        <v>268</v>
+        <v>339</v>
       </c>
       <c r="E400" s="8" t="s">
-        <v>232</v>
+        <v>329</v>
       </c>
       <c r="I400" s="9"/>
     </row>
@@ -12568,168 +12515,224 @@
         <v>43</v>
       </c>
       <c r="D401" s="8" t="s">
-        <v>286</v>
+        <v>514</v>
       </c>
       <c r="E401" s="8" t="s">
-        <v>278</v>
+        <v>521</v>
+      </c>
+      <c r="F401" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G401" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H401" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I401" s="9"/>
-    </row>
-    <row r="402" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A402" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B402" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C402" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D402" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="E402" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="I402" s="9"/>
-    </row>
-    <row r="403" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A403" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B403" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C403" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D403" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="E403" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="I403" s="9"/>
-    </row>
-    <row r="404" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A404" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B404" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C404" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D404" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="E404" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="I404" s="9"/>
-    </row>
-    <row r="405" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A405" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B405" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C405" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D405" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="E405" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="I405" s="9"/>
-    </row>
-    <row r="406" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A406" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B406" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C406" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D406" s="8" t="s">
-        <v>519</v>
-      </c>
-      <c r="E406" s="8" t="s">
-        <v>526</v>
-      </c>
-      <c r="F406" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G406" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H406" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I406" s="9"/>
-      <c r="J406" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="409" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A409" s="3" t="s">
+      <c r="J401" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="404" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A404" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I409" s="4"/>
-    </row>
-    <row r="410" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A410" s="3" t="s">
+      <c r="I404" s="4"/>
+    </row>
+    <row r="405" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A405" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I410" s="4"/>
-    </row>
-    <row r="411" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A411" s="3" t="s">
+      <c r="I405" s="4"/>
+    </row>
+    <row r="406" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A406" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B411" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C411" s="3" t="s">
+      <c r="B406" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C406" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D411" s="3" t="s">
+      <c r="D406" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E411" s="3" t="s">
+      <c r="E406" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F411" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G411" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H411" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I411" s="4" t="s">
+      <c r="F406" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G406" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H406" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I406" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="J411" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="412" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A412" s="3" t="s">
+      <c r="J406" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="407" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A407" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I412" s="4"/>
+      <c r="I407" s="4"/>
+    </row>
+    <row r="408" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A408" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B408" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C408" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D408" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E408" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="F408" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G408" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H408" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I408" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="J408" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A409" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B409" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C409" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D409" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E409" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="F409" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G409" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H409" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I409" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="J409" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="410" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A410" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B410" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C410" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D410" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E410" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="F410" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G410" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H410" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I410" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="J410" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="411" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A411" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B411" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C411" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D411" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E411" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="F411" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G411" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H411" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I411" s="9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="412" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A412" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B412" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C412" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D412" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E412" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="F412" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I412" s="9"/>
     </row>
     <row r="413" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A413" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B413" s="8" t="s">
         <v>27</v>
@@ -12738,343 +12741,197 @@
         <v>48</v>
       </c>
       <c r="D413" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E413" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F413" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I413" s="9"/>
+    </row>
+    <row r="414" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I414" s="9"/>
+    </row>
+    <row r="415" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A415" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I415" s="4"/>
+    </row>
+    <row r="416" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A416" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I416" s="4"/>
+    </row>
+    <row r="417" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A417" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B417" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C417" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D417" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E417" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F417" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G417" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H417" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I417" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J417" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="418" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A418" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I418" s="4"/>
+    </row>
+    <row r="419" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A419" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="B419" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C419" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D419" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E413" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="F413" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G413" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H413" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I413" s="9" t="s">
-        <v>440</v>
-      </c>
-      <c r="J413" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="414" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A414" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B414" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C414" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D414" s="8" t="s">
+      <c r="E419" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="F419" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G419" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H419" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I419" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="J419" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="420" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A420" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B420" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C420" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D420" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E414" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="F414" s="8" t="s">
+      <c r="E420" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="F420" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G414" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H414" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I414" s="9" t="s">
-        <v>547</v>
-      </c>
-      <c r="J414" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="415" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A415" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B415" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C415" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D415" s="8" t="s">
+      <c r="G420" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H420" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I420" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="J420" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="421" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A421" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B421" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C421" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D421" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E415" s="8" t="s">
-        <v>543</v>
-      </c>
-      <c r="F415" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G415" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H415" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I415" s="9" t="s">
-        <v>544</v>
-      </c>
-      <c r="J415" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="416" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A416" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B416" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C416" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D416" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E416" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="F416" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G416" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H416" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I416" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="417" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A417" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B417" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C417" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D417" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E417" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="F417" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I417" s="9"/>
-    </row>
-    <row r="418" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A418" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B418" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C418" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D418" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E418" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="F418" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I418" s="9"/>
-    </row>
-    <row r="419" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I419" s="9"/>
-    </row>
-    <row r="420" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A420" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I420" s="4"/>
-    </row>
-    <row r="421" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A421" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I421" s="4"/>
-    </row>
-    <row r="422" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A422" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B422" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C422" s="3" t="s">
+      <c r="E421" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="F421" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G421" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H421" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I421" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="J421" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="422" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A422" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B422" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C422" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D422" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E422" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F422" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G422" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H422" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I422" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J422" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="423" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A423" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I423" s="4"/>
-    </row>
-    <row r="424" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A424" s="8" t="s">
-        <v>525</v>
-      </c>
-      <c r="B424" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C424" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D424" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E424" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="F424" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G424" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H424" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I424" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="J424" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="425" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A425" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B425" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C425" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D425" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E425" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="F425" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G425" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H425" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I425" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="J425" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="426" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A426" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B426" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C426" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D426" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E426" s="8" t="s">
-        <v>545</v>
-      </c>
-      <c r="F426" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G426" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H426" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I426" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="J426" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="427" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A427" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B427" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C427" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D427" s="8" t="s">
-        <v>522</v>
-      </c>
-      <c r="E427" s="8" t="s">
-        <v>523</v>
-      </c>
-      <c r="F427" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G427" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H427" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I427" s="9"/>
-      <c r="J427" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="428" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I428" s="9"/>
+      <c r="D422" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="E422" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="F422" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G422" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H422" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I422" s="9"/>
+      <c r="J422" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="423" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I423" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A361:A363">
@@ -13117,7 +12974,7 @@
       <formula>LEFT(A318,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A420:A423 A335 A349:A352 B388:B406 B356 A381:A383 A357:B357 B358 B364:B386 B53:B60 B417:B418 B319:B333">
+  <conditionalFormatting sqref="A415:A418 A335 A349:A352 B356 A381:A383 A357:B357 B358 B364:B386 B53:B60 B412:B413 B319:B333 B388:B401">
     <cfRule type="containsText" priority="311" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13141,7 +12998,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B424 B426">
+  <conditionalFormatting sqref="B419 B421">
     <cfRule type="containsText" priority="203" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13149,7 +13006,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A424 A426">
+  <conditionalFormatting sqref="A419 A421">
     <cfRule type="containsText" priority="205" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13157,7 +13014,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A409:A412">
+  <conditionalFormatting sqref="A404:A407">
     <cfRule type="containsText" priority="2623" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13181,7 +13038,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A416 B306 B302">
+  <conditionalFormatting sqref="A411 B306 B302">
     <cfRule type="containsText" priority="2873" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13189,7 +13046,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A384:A386 A310 B311 A288:A292 A294 A299 B288:B295 A388:A405 A356 A358 A364:A380 A417 A319:A333 A360">
+  <conditionalFormatting sqref="A384:A386 A310 B311 A288:A292 A294 A299 B288:B295 A356 A358 A364:A380 A412 A319:A333 A360 A388:A400">
     <cfRule type="containsText" priority="2893" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13197,7 +13054,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A427">
+  <conditionalFormatting sqref="A422">
     <cfRule type="containsText" priority="3085" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13301,7 +13158,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B427 A315">
+  <conditionalFormatting sqref="B422 A315">
     <cfRule type="containsText" priority="4419" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13309,7 +13166,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A428 B415:B416 A415 A413:B413">
+  <conditionalFormatting sqref="A423 B410:B411 A410 A408:B408">
     <cfRule type="containsText" priority="4611" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13317,7 +13174,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A419 B308">
+  <conditionalFormatting sqref="A414 B308">
     <cfRule type="containsText" priority="4617" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13325,7 +13182,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B428">
+  <conditionalFormatting sqref="B423">
     <cfRule type="containsText" priority="4685" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13333,7 +13190,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B419">
+  <conditionalFormatting sqref="B414">
     <cfRule type="containsText" priority="5161" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13349,7 +13206,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A406">
+  <conditionalFormatting sqref="A401">
     <cfRule type="containsText" priority="5473" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13437,7 +13294,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A414:B414">
+  <conditionalFormatting sqref="A409:B409">
     <cfRule type="containsText" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13445,7 +13302,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B425">
+  <conditionalFormatting sqref="B420">
     <cfRule type="containsText" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13453,7 +13310,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A425">
+  <conditionalFormatting sqref="A420">
     <cfRule type="containsText" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
added flag for using DWM
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@143 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3066" uniqueCount="555">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -1320,9 +1320,6 @@
     <t>Echo</t>
   </si>
   <si>
-    <t>SetMulTabLoc</t>
-  </si>
-  <si>
     <t>MultiTab</t>
   </si>
   <si>
@@ -1386,15 +1383,9 @@
     <t>OutputLoads</t>
   </si>
   <si>
-    <t>"Output Loads (mesh)"</t>
-  </si>
-  <si>
     <t>"Current locations of components"</t>
   </si>
   <si>
-    <t>"Input Forces and positions (mesh)"</t>
-  </si>
-  <si>
     <t>#Blade</t>
   </si>
   <si>
@@ -1644,30 +1635,6 @@
     <t>IfW_Outputs</t>
   </si>
   <si>
-    <t>Reg-InflowWind.txt</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>typedef</t>
-    </r>
-  </si>
-  <si>
     <t>IfW_Params</t>
   </si>
   <si>
@@ -1774,13 +1741,22 @@
   </si>
   <si>
     <t>"inputs to IfW module; set here so we don't have to recreate it every time"</t>
+  </si>
+  <si>
+    <t>UseDWM</t>
+  </si>
+  <si>
+    <t>"flag to determine if DWM module should be used"</t>
+  </si>
+  <si>
+    <t>InflowWind.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1813,13 +1789,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
@@ -3039,11 +3008,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K423"/>
+  <dimension ref="A1:K422"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A376" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G387" sqref="G387"/>
+      <pane ySplit="15" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C296" sqref="C296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,19 +3068,19 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -3193,10 +3162,10 @@
     </row>
     <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>519</v>
+        <v>554</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -3225,7 +3194,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>26</v>
@@ -3255,7 +3224,7 @@
         <v>117</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>26</v>
@@ -3285,7 +3254,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>26</v>
@@ -3315,7 +3284,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>26</v>
@@ -4121,7 +4090,7 @@
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="I62" s="4"/>
     </row>
@@ -4133,7 +4102,7 @@
         <v>27</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>34</v>
@@ -4163,7 +4132,7 @@
         <v>27</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>34</v>
@@ -4193,7 +4162,7 @@
         <v>27</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>34</v>
@@ -4223,7 +4192,7 @@
         <v>27</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>34</v>
@@ -4253,7 +4222,7 @@
         <v>27</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>34</v>
@@ -4283,7 +4252,7 @@
         <v>27</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>34</v>
@@ -4313,7 +4282,7 @@
         <v>27</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>34</v>
@@ -4343,7 +4312,7 @@
         <v>27</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>34</v>
@@ -4373,7 +4342,7 @@
         <v>27</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>34</v>
@@ -4403,7 +4372,7 @@
         <v>27</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>99</v>
@@ -4433,7 +4402,7 @@
         <v>27</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>99</v>
@@ -4463,7 +4432,7 @@
         <v>27</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>34</v>
@@ -4493,7 +4462,7 @@
         <v>27</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>34</v>
@@ -4523,7 +4492,7 @@
         <v>27</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>34</v>
@@ -4553,7 +4522,7 @@
         <v>27</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>34</v>
@@ -4583,7 +4552,7 @@
         <v>27</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>34</v>
@@ -4613,7 +4582,7 @@
         <v>27</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>34</v>
@@ -4643,7 +4612,7 @@
         <v>27</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>34</v>
@@ -4673,7 +4642,7 @@
         <v>27</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>34</v>
@@ -4703,7 +4672,7 @@
         <v>27</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>34</v>
@@ -4733,7 +4702,7 @@
         <v>27</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>34</v>
@@ -4763,7 +4732,7 @@
         <v>27</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>34</v>
@@ -4793,7 +4762,7 @@
         <v>27</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>34</v>
@@ -4823,7 +4792,7 @@
         <v>27</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>34</v>
@@ -4853,7 +4822,7 @@
         <v>27</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>34</v>
@@ -4883,7 +4852,7 @@
         <v>27</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>34</v>
@@ -4913,7 +4882,7 @@
         <v>27</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>34</v>
@@ -4943,7 +4912,7 @@
         <v>27</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>34</v>
@@ -4973,7 +4942,7 @@
         <v>27</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>34</v>
@@ -5003,7 +4972,7 @@
         <v>27</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>34</v>
@@ -5033,7 +5002,7 @@
         <v>27</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>34</v>
@@ -5063,7 +5032,7 @@
         <v>27</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>34</v>
@@ -5093,7 +5062,7 @@
         <v>27</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>34</v>
@@ -5123,7 +5092,7 @@
         <v>27</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>34</v>
@@ -5153,7 +5122,7 @@
         <v>27</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>34</v>
@@ -5183,7 +5152,7 @@
         <v>27</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>34</v>
@@ -5213,7 +5182,7 @@
         <v>27</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>34</v>
@@ -5243,7 +5212,7 @@
         <v>27</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>34</v>
@@ -5273,7 +5242,7 @@
         <v>27</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>34</v>
@@ -5303,7 +5272,7 @@
         <v>27</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>34</v>
@@ -5333,7 +5302,7 @@
         <v>27</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>34</v>
@@ -5363,7 +5332,7 @@
         <v>27</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>34</v>
@@ -5393,7 +5362,7 @@
         <v>27</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>34</v>
@@ -5423,7 +5392,7 @@
         <v>27</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>34</v>
@@ -5453,7 +5422,7 @@
         <v>27</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>34</v>
@@ -5483,7 +5452,7 @@
         <v>27</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>34</v>
@@ -5513,7 +5482,7 @@
         <v>27</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>34</v>
@@ -5543,7 +5512,7 @@
         <v>27</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>34</v>
@@ -5573,7 +5542,7 @@
         <v>27</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>34</v>
@@ -5603,7 +5572,7 @@
         <v>27</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>34</v>
@@ -5633,7 +5602,7 @@
         <v>27</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>34</v>
@@ -5663,7 +5632,7 @@
         <v>27</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>34</v>
@@ -5693,7 +5662,7 @@
         <v>27</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>34</v>
@@ -5723,7 +5692,7 @@
         <v>27</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>34</v>
@@ -5753,7 +5722,7 @@
         <v>27</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>34</v>
@@ -5783,7 +5752,7 @@
         <v>27</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>34</v>
@@ -5813,7 +5782,7 @@
         <v>27</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>34</v>
@@ -5843,7 +5812,7 @@
         <v>27</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>34</v>
@@ -5873,7 +5842,7 @@
         <v>27</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>34</v>
@@ -5903,7 +5872,7 @@
         <v>27</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>34</v>
@@ -5933,7 +5902,7 @@
         <v>27</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>34</v>
@@ -5963,7 +5932,7 @@
         <v>27</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>34</v>
@@ -5993,7 +5962,7 @@
         <v>27</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>34</v>
@@ -6023,7 +5992,7 @@
         <v>27</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>34</v>
@@ -6055,7 +6024,7 @@
         <v>27</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D127" s="8" t="s">
         <v>34</v>
@@ -6087,7 +6056,7 @@
         <v>27</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>34</v>
@@ -6119,7 +6088,7 @@
         <v>27</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>34</v>
@@ -6151,7 +6120,7 @@
         <v>27</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>34</v>
@@ -6183,7 +6152,7 @@
         <v>27</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>99</v>
@@ -6213,7 +6182,7 @@
         <v>27</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>99</v>
@@ -6240,7 +6209,7 @@
     </row>
     <row r="134" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I134" s="4"/>
     </row>
@@ -6270,7 +6239,7 @@
         <v>26</v>
       </c>
       <c r="I135" s="9" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="136" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6299,7 +6268,7 @@
         <v>26</v>
       </c>
       <c r="I136" s="9" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="137" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6328,7 +6297,7 @@
         <v>26</v>
       </c>
       <c r="I137" s="9" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="138" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6357,7 +6326,7 @@
         <v>26</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="139" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6386,12 +6355,12 @@
         <v>26</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="141" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I141" s="4"/>
     </row>
@@ -7165,7 +7134,7 @@
         <v>26</v>
       </c>
       <c r="I171" s="9" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7194,7 +7163,7 @@
         <v>26</v>
       </c>
       <c r="I172" s="9" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="173" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7280,7 +7249,7 @@
     </row>
     <row r="177" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I177" s="4"/>
     </row>
@@ -7434,7 +7403,7 @@
         <v>26</v>
       </c>
       <c r="K182" s="8" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="183" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7467,7 +7436,7 @@
         <v>26</v>
       </c>
       <c r="K183" s="8" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="184" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7652,7 +7621,7 @@
     </row>
     <row r="191" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I191" s="4"/>
     </row>
@@ -8282,7 +8251,7 @@
         <v>26</v>
       </c>
       <c r="I212" s="9" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="213" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8431,12 +8400,12 @@
         <v>26</v>
       </c>
       <c r="I217" s="9" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="219" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I219" s="4"/>
     </row>
@@ -8493,7 +8462,7 @@
         <v>26</v>
       </c>
       <c r="I221" s="9" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J221" s="8" t="s">
         <v>26</v>
@@ -8525,7 +8494,7 @@
         <v>26</v>
       </c>
       <c r="I222" s="9" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="223" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8554,7 +8523,7 @@
         <v>26</v>
       </c>
       <c r="I223" s="9" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="224" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8583,7 +8552,7 @@
         <v>26</v>
       </c>
       <c r="I224" s="9" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="225" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8612,7 +8581,7 @@
         <v>26</v>
       </c>
       <c r="I225" s="9" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="226" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8641,7 +8610,7 @@
         <v>26</v>
       </c>
       <c r="I226" s="9" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="227" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8670,12 +8639,12 @@
         <v>26</v>
       </c>
       <c r="I227" s="9" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="230" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I230" s="4"/>
     </row>
@@ -8705,7 +8674,7 @@
         <v>26</v>
       </c>
       <c r="I231" s="9" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="232" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8953,7 +8922,7 @@
     </row>
     <row r="242" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="I242" s="4"/>
     </row>
@@ -9145,7 +9114,7 @@
         <v>26</v>
       </c>
       <c r="I249" s="9" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="250" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9174,7 +9143,7 @@
         <v>26</v>
       </c>
       <c r="I250" s="9" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="251" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9203,7 +9172,7 @@
         <v>26</v>
       </c>
       <c r="I251" s="9" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="252" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9232,7 +9201,7 @@
         <v>26</v>
       </c>
       <c r="I252" s="9" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="253" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9261,7 +9230,7 @@
         <v>26</v>
       </c>
       <c r="I253" s="9" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="254" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9290,7 +9259,7 @@
         <v>26</v>
       </c>
       <c r="I254" s="9" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="255" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9319,7 +9288,7 @@
         <v>26</v>
       </c>
       <c r="I255" s="9" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J255" s="8" t="s">
         <v>103</v>
@@ -9351,7 +9320,7 @@
         <v>26</v>
       </c>
       <c r="I256" s="9" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="257" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9380,7 +9349,7 @@
         <v>26</v>
       </c>
       <c r="I257" s="9" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="258" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9409,7 +9378,7 @@
         <v>26</v>
       </c>
       <c r="I258" s="9" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="259" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9438,7 +9407,7 @@
         <v>26</v>
       </c>
       <c r="I259" s="9" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="260" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9467,7 +9436,7 @@
         <v>26</v>
       </c>
       <c r="I260" s="9" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="261" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9496,7 +9465,7 @@
         <v>26</v>
       </c>
       <c r="I261" s="9" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="J261" s="8" t="s">
         <v>103</v>
@@ -9516,7 +9485,7 @@
         <v>99</v>
       </c>
       <c r="E262" s="8" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="F262" s="8" t="s">
         <v>26</v>
@@ -9528,7 +9497,7 @@
         <v>26</v>
       </c>
       <c r="I262" s="9" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="J262" s="8" t="s">
         <v>103</v>
@@ -9548,7 +9517,7 @@
         <v>41</v>
       </c>
       <c r="E263" s="8" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="F263" s="8" t="s">
         <v>26</v>
@@ -9560,7 +9529,7 @@
         <v>26</v>
       </c>
       <c r="I263" s="9" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="264" spans="1:10" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -9577,7 +9546,7 @@
         <v>34</v>
       </c>
       <c r="E264" s="8" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="F264" s="8" t="s">
         <v>31</v>
@@ -9589,7 +9558,7 @@
         <v>26</v>
       </c>
       <c r="I264" s="9" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="J264" s="8" t="s">
         <v>26</v>
@@ -9600,7 +9569,7 @@
     </row>
     <row r="266" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="I266" s="4"/>
     </row>
@@ -9792,7 +9761,7 @@
         <v>26</v>
       </c>
       <c r="I273" s="9" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="J273" s="8" t="s">
         <v>371</v>
@@ -9824,7 +9793,7 @@
         <v>26</v>
       </c>
       <c r="I274" s="9" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="J274" s="8" t="s">
         <v>373</v>
@@ -9880,7 +9849,7 @@
         <v>26</v>
       </c>
       <c r="I278" s="9" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="279" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9909,7 +9878,7 @@
         <v>26</v>
       </c>
       <c r="I279" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="280" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9980,7 +9949,7 @@
         <v>26</v>
       </c>
       <c r="I284" s="9" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="285" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -9997,7 +9966,7 @@
         <v>24</v>
       </c>
       <c r="E285" s="8" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="F285" s="8" t="s">
         <v>26</v>
@@ -10024,7 +9993,7 @@
         <v>24</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="F286" s="8" t="s">
         <v>26</v>
@@ -10036,7 +10005,7 @@
         <v>26</v>
       </c>
       <c r="I286" s="9" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="287" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10065,7 +10034,7 @@
         <v>26</v>
       </c>
       <c r="I287" s="9" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="288" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10094,7 +10063,7 @@
         <v>26</v>
       </c>
       <c r="I288" s="9" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="289" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10123,7 +10092,7 @@
         <v>26</v>
       </c>
       <c r="I289" s="9" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="290" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10152,7 +10121,7 @@
         <v>26</v>
       </c>
       <c r="I290" s="9" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="291" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10181,7 +10150,7 @@
         <v>26</v>
       </c>
       <c r="I291" s="9" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="292" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10210,7 +10179,7 @@
         <v>26</v>
       </c>
       <c r="I292" s="9" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="293" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10239,7 +10208,7 @@
         <v>26</v>
       </c>
       <c r="I293" s="9" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="294" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10268,7 +10237,7 @@
         <v>26</v>
       </c>
       <c r="I294" s="9" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="295" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10300,26 +10269,28 @@
         <v>23</v>
       </c>
       <c r="D296" s="8" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="E296" s="8" t="s">
-        <v>390</v>
+        <v>552</v>
       </c>
       <c r="F296" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G296" s="8" t="s">
-        <v>26</v>
+        <v>399</v>
       </c>
       <c r="H296" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I296" s="9"/>
+      <c r="I296" s="9" t="s">
+        <v>553</v>
+      </c>
       <c r="J296" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A297" s="8" t="s">
         <v>22</v>
       </c>
@@ -10330,10 +10301,10 @@
         <v>23</v>
       </c>
       <c r="D297" s="8" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="E297" s="8" t="s">
-        <v>537</v>
+        <v>390</v>
       </c>
       <c r="F297" s="8" t="s">
         <v>26</v>
@@ -10344,11 +10315,12 @@
       <c r="H297" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I297" s="9" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="298" spans="1:10" s="8" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I297" s="9"/>
+      <c r="J297" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="8" t="s">
         <v>22</v>
       </c>
@@ -10359,13 +10331,13 @@
         <v>23</v>
       </c>
       <c r="D298" s="8" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E298" s="8" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="F298" s="8" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="G298" s="8" t="s">
         <v>26</v>
@@ -10374,13 +10346,10 @@
         <v>26</v>
       </c>
       <c r="I298" s="9" t="s">
-        <v>547</v>
-      </c>
-      <c r="J298" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" s="8" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="8" t="s">
         <v>22</v>
       </c>
@@ -10391,13 +10360,13 @@
         <v>23</v>
       </c>
       <c r="D299" s="8" t="s">
-        <v>507</v>
+        <v>34</v>
       </c>
       <c r="E299" s="8" t="s">
-        <v>526</v>
+        <v>539</v>
       </c>
       <c r="F299" s="8" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="G299" s="8" t="s">
         <v>26</v>
@@ -10405,61 +10374,64 @@
       <c r="H299" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I299" s="9"/>
+      <c r="I299" s="9" t="s">
+        <v>542</v>
+      </c>
       <c r="J299" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="3" t="s">
+    <row r="300" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B300" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C300" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D300" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="E300" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="F300" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G300" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H300" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I300" s="9"/>
+      <c r="J300" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I300" s="4"/>
-    </row>
-    <row r="301" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A301" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B301" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C301" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D301" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E301" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F301" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G301" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H301" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I301" s="9" t="s">
-        <v>528</v>
-      </c>
+      <c r="I301" s="4"/>
     </row>
     <row r="302" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A302" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B302" s="8" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="C302" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D302" s="8" t="s">
-        <v>508</v>
+        <v>91</v>
       </c>
       <c r="E302" s="8" t="s">
-        <v>509</v>
+        <v>92</v>
       </c>
       <c r="F302" s="8" t="s">
         <v>26</v>
@@ -10470,55 +10442,54 @@
       <c r="H302" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I302" s="9"/>
-      <c r="J302" s="8" t="s">
-        <v>26</v>
+      <c r="I302" s="9" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="303" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B303" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C303" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D303" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E303" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="F303" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G303" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H303" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="I303" s="9"/>
-    </row>
-    <row r="304" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I304" s="4"/>
+      <c r="J303" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I304" s="9"/>
     </row>
     <row r="305" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I305" s="4"/>
+    </row>
+    <row r="306" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I305" s="4"/>
-    </row>
-    <row r="306" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B306" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C306" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D306" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E306" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F306" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G306" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H306" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I306" s="9"/>
-      <c r="J306" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="I306" s="4"/>
     </row>
     <row r="307" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A307" s="8" t="s">
@@ -10531,10 +10502,10 @@
         <v>33</v>
       </c>
       <c r="D307" s="8" t="s">
-        <v>510</v>
+        <v>34</v>
       </c>
       <c r="E307" s="8" t="s">
-        <v>525</v>
+        <v>37</v>
       </c>
       <c r="F307" s="8" t="s">
         <v>26</v>
@@ -10551,43 +10522,43 @@
       </c>
     </row>
     <row r="308" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B308" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C308" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D308" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E308" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="F308" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G308" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H308" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="I308" s="9"/>
-    </row>
-    <row r="309" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A309" s="3" t="s">
+      <c r="J308" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I309" s="9"/>
+    </row>
+    <row r="310" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I309" s="4"/>
-    </row>
-    <row r="310" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B310" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C310" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D310" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E310" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F310" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G310" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H310" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I310" s="9"/>
-      <c r="J310" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="I310" s="4"/>
     </row>
     <row r="311" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" s="8" t="s">
@@ -10600,10 +10571,10 @@
         <v>36</v>
       </c>
       <c r="D311" s="8" t="s">
-        <v>511</v>
+        <v>34</v>
       </c>
       <c r="E311" s="8" t="s">
-        <v>523</v>
+        <v>37</v>
       </c>
       <c r="F311" s="8" t="s">
         <v>26</v>
@@ -10620,43 +10591,43 @@
       </c>
     </row>
     <row r="312" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B312" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C312" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D312" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="E312" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="F312" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G312" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H312" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="I312" s="9"/>
-    </row>
-    <row r="313" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A313" s="3" t="s">
+      <c r="J312" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I313" s="9"/>
+    </row>
+    <row r="314" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A314" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I313" s="4"/>
-    </row>
-    <row r="314" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A314" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B314" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C314" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D314" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E314" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F314" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G314" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H314" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I314" s="9"/>
-      <c r="J314" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="I314" s="4"/>
     </row>
     <row r="315" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" s="8" t="s">
@@ -10669,10 +10640,10 @@
         <v>38</v>
       </c>
       <c r="D315" s="8" t="s">
-        <v>512</v>
+        <v>34</v>
       </c>
       <c r="E315" s="8" t="s">
-        <v>522</v>
+        <v>39</v>
       </c>
       <c r="F315" s="8" t="s">
         <v>26</v>
@@ -10689,48 +10660,48 @@
       </c>
     </row>
     <row r="316" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B316" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C316" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D316" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="E316" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="F316" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G316" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H316" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="I316" s="9"/>
-    </row>
-    <row r="317" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A317" s="3" t="s">
-        <v>486</v>
-      </c>
+      <c r="J316" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I317" s="9"/>
     </row>
     <row r="318" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" s="3" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I318" s="4"/>
-    </row>
-    <row r="319" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A319" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B319" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C319" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D319" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E319" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F319" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G319" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H319" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I319" s="9"/>
-      <c r="J319" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="I319" s="4"/>
     </row>
     <row r="320" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" s="8" t="s">
@@ -10743,10 +10714,10 @@
         <v>40</v>
       </c>
       <c r="D320" s="8" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="E320" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F320" s="8" t="s">
         <v>26</v>
@@ -10757,11 +10728,9 @@
       <c r="H320" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I320" s="9" t="s">
-        <v>487</v>
-      </c>
+      <c r="I320" s="9"/>
       <c r="J320" s="8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="321" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10775,13 +10744,13 @@
         <v>40</v>
       </c>
       <c r="D321" s="8" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="E321" s="8" t="s">
-        <v>317</v>
+        <v>45</v>
       </c>
       <c r="F321" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G321" s="8" t="s">
         <v>26</v>
@@ -10789,9 +10758,11 @@
       <c r="H321" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I321" s="9"/>
+      <c r="I321" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="J321" s="8" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="322" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10805,13 +10776,13 @@
         <v>40</v>
       </c>
       <c r="D322" s="8" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="E322" s="8" t="s">
-        <v>391</v>
+        <v>317</v>
       </c>
       <c r="F322" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G322" s="8" t="s">
         <v>26</v>
@@ -10820,6 +10791,9 @@
         <v>26</v>
       </c>
       <c r="I322" s="9"/>
+      <c r="J322" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="323" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="8" t="s">
@@ -10832,23 +10806,21 @@
         <v>40</v>
       </c>
       <c r="D323" s="8" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E323" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F323" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G323" s="8">
-        <v>1</v>
+      <c r="G323" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="H323" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I323" s="9" t="s">
-        <v>488</v>
-      </c>
+      <c r="I323" s="9"/>
     </row>
     <row r="324" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A324" s="8" t="s">
@@ -10864,7 +10836,7 @@
         <v>34</v>
       </c>
       <c r="E324" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F324" s="8" t="s">
         <v>26</v>
@@ -10876,7 +10848,7 @@
         <v>26</v>
       </c>
       <c r="I324" s="9" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="325" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10893,7 +10865,7 @@
         <v>34</v>
       </c>
       <c r="E325" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F325" s="8" t="s">
         <v>26</v>
@@ -10905,7 +10877,7 @@
         <v>26</v>
       </c>
       <c r="I325" s="9" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="326" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10922,19 +10894,19 @@
         <v>34</v>
       </c>
       <c r="E326" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F326" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G326" s="8" t="s">
-        <v>26</v>
+      <c r="G326" s="8">
+        <v>1</v>
       </c>
       <c r="H326" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I326" s="9" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="327" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10948,22 +10920,22 @@
         <v>40</v>
       </c>
       <c r="D327" s="8" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="E327" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F327" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G327" s="8" t="s">
-        <v>397</v>
+        <v>26</v>
       </c>
       <c r="H327" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I327" s="9" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="328" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -10980,19 +10952,19 @@
         <v>99</v>
       </c>
       <c r="E328" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F328" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G328" s="8" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H328" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I328" s="9" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="329" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11009,7 +10981,7 @@
         <v>99</v>
       </c>
       <c r="E329" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F329" s="8" t="s">
         <v>26</v>
@@ -11021,7 +10993,7 @@
         <v>26</v>
       </c>
       <c r="I329" s="9" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="330" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11038,7 +11010,7 @@
         <v>99</v>
       </c>
       <c r="E330" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F330" s="8" t="s">
         <v>26</v>
@@ -11050,7 +11022,7 @@
         <v>26</v>
       </c>
       <c r="I330" s="9" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="331" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11067,19 +11039,19 @@
         <v>99</v>
       </c>
       <c r="E331" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F331" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G331" s="8" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="H331" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I331" s="9" t="s">
-        <v>1</v>
+        <v>489</v>
       </c>
     </row>
     <row r="332" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11096,7 +11068,7 @@
         <v>99</v>
       </c>
       <c r="E332" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F332" s="8" t="s">
         <v>26</v>
@@ -11107,9 +11079,8 @@
       <c r="H332" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I332" s="9"/>
-      <c r="J332" s="8" t="s">
-        <v>26</v>
+      <c r="I332" s="9" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="333" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11123,22 +11094,23 @@
         <v>40</v>
       </c>
       <c r="D333" s="8" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E333" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F333" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G333" s="8">
-        <v>0</v>
+      <c r="G333" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="H333" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I333" s="9" t="s">
-        <v>493</v>
+      <c r="I333" s="9"/>
+      <c r="J333" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="334" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11152,261 +11124,267 @@
         <v>40</v>
       </c>
       <c r="D334" s="8" t="s">
-        <v>513</v>
+        <v>89</v>
       </c>
       <c r="E334" s="8" t="s">
-        <v>524</v>
+        <v>404</v>
       </c>
       <c r="F334" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G334" s="8" t="s">
-        <v>26</v>
+      <c r="G334" s="8">
+        <v>0</v>
       </c>
       <c r="H334" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I334" s="9"/>
-      <c r="J334" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="335" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="I335" s="4"/>
-    </row>
-    <row r="336" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A336" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B336" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C336" s="8" t="s">
+      <c r="I334" s="9" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B335" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C335" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D336" s="8" t="s">
+      <c r="D335" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="E335" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="F335" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G335" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H335" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I335" s="9"/>
+      <c r="J335" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="I336" s="4"/>
+    </row>
+    <row r="337" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B337" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C337" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D337" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E336" s="8" t="s">
+      <c r="E337" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="I336" s="9"/>
-    </row>
-    <row r="337" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="I337" s="4"/>
-    </row>
-    <row r="338" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A338" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B338" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C338" s="8" t="s">
+      <c r="I337" s="9"/>
+    </row>
+    <row r="338" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="I338" s="4"/>
+    </row>
+    <row r="339" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B339" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C339" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D338" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="E338" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="I338" s="9"/>
-    </row>
-    <row r="339" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A339" s="3" t="s">
+      <c r="D339" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="E339" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="I339" s="9"/>
+    </row>
+    <row r="340" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="I340" s="4"/>
+    </row>
+    <row r="341" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B341" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C341" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D341" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E341" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="I341" s="9"/>
+    </row>
+    <row r="342" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="I342" s="4"/>
+    </row>
+    <row r="343" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B343" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C343" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D343" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E343" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="I343" s="9"/>
+    </row>
+    <row r="344" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="I344" s="4"/>
+    </row>
+    <row r="345" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B345" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C345" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D345" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="E345" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="I345" s="9"/>
+    </row>
+    <row r="346" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="I346" s="4"/>
+    </row>
+    <row r="347" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B347" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C347" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D347" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="E347" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="I347" s="9"/>
+    </row>
+    <row r="348" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="I339" s="4"/>
-    </row>
-    <row r="340" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A340" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B340" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C340" s="8" t="s">
+      <c r="I348" s="4"/>
+    </row>
+    <row r="349" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B349" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C349" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D340" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E340" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="I340" s="9"/>
-    </row>
-    <row r="341" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="I341" s="4"/>
-    </row>
-    <row r="342" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A342" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B342" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C342" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D342" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E342" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="I342" s="9"/>
-    </row>
-    <row r="343" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="I343" s="4"/>
-    </row>
-    <row r="344" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A344" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B344" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C344" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D344" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="E344" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="I344" s="9"/>
-    </row>
-    <row r="345" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A345" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="I345" s="4"/>
-    </row>
-    <row r="346" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B346" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C346" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D346" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E346" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="I346" s="9"/>
-    </row>
-    <row r="347" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="I347" s="4"/>
-    </row>
-    <row r="348" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B348" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C348" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D348" s="8" t="s">
+      <c r="D349" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="E348" s="8" t="s">
+      <c r="E349" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="I348" s="9"/>
-    </row>
-    <row r="349" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I349" s="4"/>
+      <c r="I349" s="9"/>
     </row>
     <row r="350" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>483</v>
+        <v>109</v>
       </c>
       <c r="I350" s="4"/>
     </row>
     <row r="351" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="I351" s="4"/>
     </row>
-    <row r="352" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="I352" s="4"/>
+    </row>
+    <row r="353" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="B352" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C352" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D352" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E352" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="F352" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G352" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H352" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I352" s="11" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="353" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B353" s="8" t="s">
+      <c r="B353" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C353" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D353" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E353" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="F353" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I353" s="8" t="s">
-        <v>495</v>
+      <c r="D353" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E353" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F353" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G353" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H353" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I353" s="11" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="354" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11423,13 +11401,13 @@
         <v>114</v>
       </c>
       <c r="E354" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F354" s="8" t="s">
         <v>88</v>
       </c>
       <c r="I354" s="8" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="355" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11443,22 +11421,16 @@
         <v>40</v>
       </c>
       <c r="D355" s="8" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="E355" s="8" t="s">
-        <v>551</v>
+        <v>408</v>
       </c>
       <c r="F355" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G355" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H355" s="8" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="I355" s="8" t="s">
-        <v>552</v>
+        <v>492</v>
       </c>
     </row>
     <row r="356" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11472,12 +11444,23 @@
         <v>40</v>
       </c>
       <c r="D356" s="8" t="s">
-        <v>292</v>
+        <v>99</v>
       </c>
       <c r="E356" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="I356" s="9"/>
+        <v>546</v>
+      </c>
+      <c r="F356" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G356" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H356" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I356" s="8" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="357" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="8" t="s">
@@ -11490,19 +11473,10 @@
         <v>40</v>
       </c>
       <c r="D357" s="8" t="s">
-        <v>99</v>
+        <v>292</v>
       </c>
       <c r="E357" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="F357" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G357" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H357" s="8" t="s">
-        <v>26</v>
+        <v>429</v>
       </c>
       <c r="I357" s="9"/>
     </row>
@@ -11520,7 +11494,7 @@
         <v>99</v>
       </c>
       <c r="E358" s="8" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="F358" s="8" t="s">
         <v>26</v>
@@ -11531,11 +11505,9 @@
       <c r="H358" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I358" s="9" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="359" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="I358" s="9"/>
+    </row>
+    <row r="359" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A359" s="8" t="s">
         <v>22</v>
       </c>
@@ -11546,10 +11518,10 @@
         <v>40</v>
       </c>
       <c r="D359" s="8" t="s">
-        <v>515</v>
+        <v>99</v>
       </c>
       <c r="E359" s="8" t="s">
-        <v>516</v>
+        <v>417</v>
       </c>
       <c r="F359" s="8" t="s">
         <v>26</v>
@@ -11561,54 +11533,65 @@
         <v>26</v>
       </c>
       <c r="I359" s="9" t="s">
-        <v>556</v>
-      </c>
-      <c r="J359" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="360" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I360" s="9"/>
-    </row>
-    <row r="361" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A361" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I361" s="4"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A360" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B360" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C360" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D360" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="E360" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="F360" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G360" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H360" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I360" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="J360" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="361" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I361" s="9"/>
     </row>
     <row r="362" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A362" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I362" s="4"/>
     </row>
     <row r="363" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A363" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I363" s="4"/>
+    </row>
+    <row r="364" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I363" s="4"/>
-    </row>
-    <row r="364" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A364" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B364" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C364" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D364" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E364" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I364" s="9"/>
+      <c r="I364" s="4"/>
     </row>
     <row r="365" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A365" s="8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B365" s="8" t="s">
         <v>27</v>
@@ -11617,23 +11600,12 @@
         <v>43</v>
       </c>
       <c r="D365" s="8" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="F365" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G365" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H365" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I365" s="9" t="s">
-        <v>476</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="I365" s="9"/>
     </row>
     <row r="366" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A366" s="8" t="s">
@@ -11649,7 +11621,7 @@
         <v>24</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F366" s="8" t="s">
         <v>26</v>
@@ -11661,7 +11633,7 @@
         <v>26</v>
       </c>
       <c r="I366" s="9" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="367" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11675,15 +11647,23 @@
         <v>43</v>
       </c>
       <c r="D367" s="8" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="E367" s="8" t="s">
-        <v>409</v>
+        <v>384</v>
       </c>
       <c r="F367" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I367" s="9"/>
+      <c r="G367" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H367" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I367" s="9" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="368" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A368" s="8" t="s">
@@ -11699,15 +11679,9 @@
         <v>99</v>
       </c>
       <c r="E368" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F368" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G368" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="H368" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I368" s="9"/>
@@ -11726,9 +11700,15 @@
         <v>99</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F369" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G369" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="H369" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I369" s="9"/>
@@ -11747,7 +11727,10 @@
         <v>99</v>
       </c>
       <c r="E370" s="8" t="s">
-        <v>388</v>
+        <v>411</v>
+      </c>
+      <c r="F370" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I370" s="9"/>
     </row>
@@ -11765,13 +11748,7 @@
         <v>99</v>
       </c>
       <c r="E371" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="F371" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G371" s="8" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="I371" s="9"/>
     </row>
@@ -11789,7 +11766,7 @@
         <v>99</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F372" s="8" t="s">
         <v>26</v>
@@ -11797,13 +11774,7 @@
       <c r="G372" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="H372" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I372" s="9"/>
-      <c r="J372" s="8" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="373" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="8" t="s">
@@ -11816,23 +11787,21 @@
         <v>43</v>
       </c>
       <c r="D373" s="8" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="E373" s="8" t="s">
-        <v>100</v>
+        <v>413</v>
       </c>
       <c r="F373" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G373" s="8" t="s">
-        <v>26</v>
+        <v>399</v>
       </c>
       <c r="H373" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I373" s="9" t="s">
-        <v>496</v>
-      </c>
+      <c r="I373" s="9"/>
       <c r="J373" s="8" t="s">
         <v>26</v>
       </c>
@@ -11848,22 +11817,25 @@
         <v>43</v>
       </c>
       <c r="D374" s="8" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="E374" s="8" t="s">
-        <v>98</v>
+        <v>552</v>
       </c>
       <c r="F374" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G374" s="8" t="s">
-        <v>26</v>
+        <v>399</v>
       </c>
       <c r="H374" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I374" s="9" t="s">
-        <v>479</v>
+        <v>553</v>
+      </c>
+      <c r="J374" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="375" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11877,10 +11849,10 @@
         <v>43</v>
       </c>
       <c r="D375" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E375" s="8" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F375" s="8" t="s">
         <v>26</v>
@@ -11892,7 +11864,10 @@
         <v>26</v>
       </c>
       <c r="I375" s="9" t="s">
-        <v>480</v>
+        <v>493</v>
+      </c>
+      <c r="J375" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="376" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11906,10 +11881,10 @@
         <v>43</v>
       </c>
       <c r="D376" s="8" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E376" s="8" t="s">
-        <v>389</v>
+        <v>98</v>
       </c>
       <c r="F376" s="8" t="s">
         <v>26</v>
@@ -11920,7 +11895,9 @@
       <c r="H376" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I376" s="9"/>
+      <c r="I376" s="9" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="377" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="8" t="s">
@@ -11933,10 +11910,10 @@
         <v>43</v>
       </c>
       <c r="D377" s="8" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E377" s="8" t="s">
-        <v>415</v>
+        <v>90</v>
       </c>
       <c r="F377" s="8" t="s">
         <v>26</v>
@@ -11948,7 +11925,7 @@
         <v>26</v>
       </c>
       <c r="I377" s="9" t="s">
-        <v>497</v>
+        <v>477</v>
       </c>
     </row>
     <row r="378" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11965,7 +11942,7 @@
         <v>99</v>
       </c>
       <c r="E378" s="8" t="s">
-        <v>416</v>
+        <v>389</v>
       </c>
       <c r="F378" s="8" t="s">
         <v>26</v>
@@ -11976,9 +11953,7 @@
       <c r="H378" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I378" s="9" t="s">
-        <v>498</v>
-      </c>
+      <c r="I378" s="9"/>
     </row>
     <row r="379" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="8" t="s">
@@ -11994,12 +11969,20 @@
         <v>99</v>
       </c>
       <c r="E379" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F379" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I379" s="9"/>
+      <c r="G379" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H379" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I379" s="9" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="380" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A380" s="8" t="s">
@@ -12015,7 +11998,7 @@
         <v>99</v>
       </c>
       <c r="E380" s="8" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F380" s="8" t="s">
         <v>26</v>
@@ -12027,7 +12010,7 @@
         <v>26</v>
       </c>
       <c r="I380" s="9" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="381" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12044,20 +12027,12 @@
         <v>99</v>
       </c>
       <c r="E381" s="8" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F381" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G381" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H381" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I381" s="9" t="s">
-        <v>500</v>
-      </c>
+      <c r="I381" s="9"/>
     </row>
     <row r="382" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A382" s="8" t="s">
@@ -12073,7 +12048,7 @@
         <v>99</v>
       </c>
       <c r="E382" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F382" s="8" t="s">
         <v>26</v>
@@ -12085,7 +12060,7 @@
         <v>26</v>
       </c>
       <c r="I382" s="9" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="383" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12099,10 +12074,10 @@
         <v>43</v>
       </c>
       <c r="D383" s="8" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="E383" s="8" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F383" s="8" t="s">
         <v>26</v>
@@ -12114,7 +12089,7 @@
         <v>26</v>
       </c>
       <c r="I383" s="9" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="384" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12128,10 +12103,10 @@
         <v>43</v>
       </c>
       <c r="D384" s="8" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="E384" s="8" t="s">
-        <v>101</v>
+        <v>420</v>
       </c>
       <c r="F384" s="8" t="s">
         <v>26</v>
@@ -12143,15 +12118,12 @@
         <v>26</v>
       </c>
       <c r="I384" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="J384" s="8" t="s">
-        <v>103</v>
+        <v>497</v>
       </c>
     </row>
     <row r="385" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B385" s="8" t="s">
         <v>27</v>
@@ -12160,10 +12132,10 @@
         <v>43</v>
       </c>
       <c r="D385" s="8" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E385" s="8" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F385" s="8" t="s">
         <v>26</v>
@@ -12175,10 +12147,7 @@
         <v>26</v>
       </c>
       <c r="I385" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="J385" s="8" t="s">
-        <v>103</v>
+        <v>498</v>
       </c>
     </row>
     <row r="386" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12192,24 +12161,30 @@
         <v>43</v>
       </c>
       <c r="D386" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E386" s="8" t="s">
-        <v>425</v>
+        <v>101</v>
       </c>
       <c r="F386" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G386" s="8" t="s">
-        <v>554</v>
+        <v>26</v>
+      </c>
+      <c r="H386" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I386" s="9" t="s">
-        <v>503</v>
+        <v>499</v>
+      </c>
+      <c r="J386" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="387" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A387" s="8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B387" s="8" t="s">
         <v>27</v>
@@ -12218,18 +12193,26 @@
         <v>43</v>
       </c>
       <c r="D387" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E387" s="8" t="s">
-        <v>553</v>
+        <v>423</v>
       </c>
       <c r="F387" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G387" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="I387" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="H387" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I387" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="J387" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="388" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A388" s="8" t="s">
@@ -12245,16 +12228,16 @@
         <v>41</v>
       </c>
       <c r="E388" s="8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F388" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G388" s="8" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="I388" s="9" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="389" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12271,20 +12254,15 @@
         <v>41</v>
       </c>
       <c r="E389" s="8" t="s">
-        <v>427</v>
+        <v>548</v>
       </c>
       <c r="F389" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G389" s="8">
-        <v>1000</v>
-      </c>
-      <c r="H389" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I389" s="9" t="s">
-        <v>505</v>
-      </c>
+      <c r="G389" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="I389" s="9"/>
     </row>
     <row r="390" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="8" t="s">
@@ -12297,22 +12275,19 @@
         <v>43</v>
       </c>
       <c r="D390" s="8" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E390" s="8" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F390" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G390" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="H390" s="8" t="s">
-        <v>26</v>
+        <v>549</v>
       </c>
       <c r="I390" s="9" t="s">
-        <v>478</v>
+        <v>501</v>
       </c>
     </row>
     <row r="391" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -12326,21 +12301,23 @@
         <v>43</v>
       </c>
       <c r="D391" s="8" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="E391" s="8" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F391" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G391" s="8">
-        <v>-1</v>
+        <v>1000</v>
       </c>
       <c r="H391" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I391" s="9"/>
+      <c r="I391" s="9" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="392" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="8" t="s">
@@ -12353,12 +12330,23 @@
         <v>43</v>
       </c>
       <c r="D392" s="8" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="E392" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I392" s="9"/>
+        <v>427</v>
+      </c>
+      <c r="F392" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G392" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="H392" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I392" s="9" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="393" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="8" t="s">
@@ -12371,10 +12359,19 @@
         <v>43</v>
       </c>
       <c r="D393" s="8" t="s">
-        <v>227</v>
+        <v>89</v>
       </c>
       <c r="E393" s="8" t="s">
-        <v>125</v>
+        <v>428</v>
+      </c>
+      <c r="F393" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G393" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H393" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="I393" s="9"/>
     </row>
@@ -12389,10 +12386,10 @@
         <v>43</v>
       </c>
       <c r="D394" s="8" t="s">
-        <v>533</v>
+        <v>141</v>
       </c>
       <c r="E394" s="8" t="s">
-        <v>532</v>
+        <v>135</v>
       </c>
       <c r="I394" s="9"/>
     </row>
@@ -12407,10 +12404,10 @@
         <v>43</v>
       </c>
       <c r="D395" s="8" t="s">
-        <v>268</v>
+        <v>227</v>
       </c>
       <c r="E395" s="8" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="I395" s="9"/>
     </row>
@@ -12425,10 +12422,10 @@
         <v>43</v>
       </c>
       <c r="D396" s="8" t="s">
-        <v>286</v>
+        <v>528</v>
       </c>
       <c r="E396" s="8" t="s">
-        <v>278</v>
+        <v>527</v>
       </c>
       <c r="I396" s="9"/>
     </row>
@@ -12443,10 +12440,10 @@
         <v>43</v>
       </c>
       <c r="D397" s="8" t="s">
-        <v>342</v>
+        <v>268</v>
       </c>
       <c r="E397" s="8" t="s">
-        <v>341</v>
+        <v>232</v>
       </c>
       <c r="I397" s="9"/>
     </row>
@@ -12461,10 +12458,10 @@
         <v>43</v>
       </c>
       <c r="D398" s="8" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="E398" s="8" t="s">
-        <v>319</v>
+        <v>278</v>
       </c>
       <c r="I398" s="9"/>
     </row>
@@ -12479,10 +12476,10 @@
         <v>43</v>
       </c>
       <c r="D399" s="8" t="s">
-        <v>369</v>
+        <v>342</v>
       </c>
       <c r="E399" s="8" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="I399" s="9"/>
     </row>
@@ -12497,10 +12494,10 @@
         <v>43</v>
       </c>
       <c r="D400" s="8" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="E400" s="8" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="I400" s="9"/>
     </row>
@@ -12515,138 +12512,110 @@
         <v>43</v>
       </c>
       <c r="D401" s="8" t="s">
-        <v>514</v>
+        <v>369</v>
       </c>
       <c r="E401" s="8" t="s">
-        <v>521</v>
-      </c>
-      <c r="F401" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G401" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H401" s="8" t="s">
-        <v>26</v>
+        <v>362</v>
       </c>
       <c r="I401" s="9"/>
-      <c r="J401" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="404" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A404" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I404" s="4"/>
-    </row>
-    <row r="405" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A405" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I405" s="4"/>
+    </row>
+    <row r="402" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A402" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B402" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C402" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D402" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E402" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="I402" s="9"/>
+    </row>
+    <row r="403" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A403" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B403" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C403" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D403" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="E403" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="F403" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G403" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H403" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I403" s="9"/>
+      <c r="J403" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="406" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A406" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B406" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C406" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D406" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E406" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F406" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G406" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H406" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I406" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J406" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I406" s="4"/>
     </row>
     <row r="407" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A407" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I407" s="4"/>
+    </row>
+    <row r="408" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A408" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B408" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C408" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D408" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E408" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F408" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G408" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H408" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I408" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J408" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A409" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I407" s="4"/>
-    </row>
-    <row r="408" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A408" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B408" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C408" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D408" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E408" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="F408" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G408" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H408" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I408" s="9" t="s">
-        <v>435</v>
-      </c>
-      <c r="J408" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="409" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A409" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B409" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C409" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D409" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E409" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="F409" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G409" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H409" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I409" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="J409" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="I409" s="4"/>
     </row>
     <row r="410" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A410" s="8" t="s">
@@ -12662,10 +12631,10 @@
         <v>56</v>
       </c>
       <c r="E410" s="8" t="s">
-        <v>538</v>
+        <v>430</v>
       </c>
       <c r="F410" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G410" s="8" t="s">
         <v>26</v>
@@ -12674,7 +12643,7 @@
         <v>26</v>
       </c>
       <c r="I410" s="9" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J410" s="8" t="s">
         <v>26</v>
@@ -12691,10 +12660,10 @@
         <v>48</v>
       </c>
       <c r="D411" s="8" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="E411" s="8" t="s">
-        <v>390</v>
+        <v>533</v>
       </c>
       <c r="F411" s="8" t="s">
         <v>26</v>
@@ -12706,12 +12675,15 @@
         <v>26</v>
       </c>
       <c r="I411" s="9" t="s">
-        <v>434</v>
+        <v>534</v>
+      </c>
+      <c r="J411" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="412" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A412" s="8" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B412" s="8" t="s">
         <v>27</v>
@@ -12720,15 +12692,23 @@
         <v>48</v>
       </c>
       <c r="D412" s="8" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="E412" s="8" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
       <c r="F412" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I412" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="G412" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H412" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I412" s="9" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="413" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A413" s="8" t="s">
@@ -12806,7 +12786,7 @@
     </row>
     <row r="419" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A419" s="8" t="s">
-        <v>520</v>
+        <v>22</v>
       </c>
       <c r="B419" s="8" t="s">
         <v>27</v>
@@ -12815,13 +12795,13 @@
         <v>50</v>
       </c>
       <c r="D419" s="8" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="E419" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F419" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G419" s="8" t="s">
         <v>26</v>
@@ -12830,7 +12810,7 @@
         <v>26</v>
       </c>
       <c r="I419" s="9" t="s">
-        <v>433</v>
+        <v>538</v>
       </c>
       <c r="J419" s="8" t="s">
         <v>26</v>
@@ -12850,10 +12830,10 @@
         <v>56</v>
       </c>
       <c r="E420" s="8" t="s">
-        <v>432</v>
+        <v>535</v>
       </c>
       <c r="F420" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G420" s="8" t="s">
         <v>26</v>
@@ -12862,7 +12842,7 @@
         <v>26</v>
       </c>
       <c r="I420" s="9" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="J420" s="8" t="s">
         <v>26</v>
@@ -12879,10 +12859,10 @@
         <v>50</v>
       </c>
       <c r="D421" s="8" t="s">
-        <v>56</v>
+        <v>514</v>
       </c>
       <c r="E421" s="8" t="s">
-        <v>540</v>
+        <v>515</v>
       </c>
       <c r="F421" s="8" t="s">
         <v>26</v>
@@ -12893,392 +12873,384 @@
       <c r="H421" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I421" s="9" t="s">
-        <v>541</v>
-      </c>
+      <c r="I421" s="9"/>
       <c r="J421" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="422" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A422" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B422" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C422" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D422" s="8" t="s">
-        <v>517</v>
-      </c>
-      <c r="E422" s="8" t="s">
-        <v>518</v>
-      </c>
-      <c r="F422" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G422" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H422" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I422" s="9"/>
-      <c r="J422" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="423" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I423" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A361:A363">
-    <cfRule type="containsText" dxfId="25" priority="149" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A361)))</formula>
+  <conditionalFormatting sqref="A362:A364">
+    <cfRule type="containsText" dxfId="25" priority="157" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A362)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="150" operator="beginsWith" text="#">
-      <formula>LEFT(A361,LEN("#"))="#"</formula>
+    <cfRule type="beginsWith" dxfId="24" priority="158" operator="beginsWith" text="#">
+      <formula>LEFT(A362,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A300">
-    <cfRule type="containsText" dxfId="23" priority="121" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A300)))</formula>
+  <conditionalFormatting sqref="A301">
+    <cfRule type="containsText" dxfId="23" priority="129" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A301)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="122" operator="beginsWith" text="#">
-      <formula>LEFT(A300,LEN("#"))="#"</formula>
+    <cfRule type="beginsWith" dxfId="22" priority="130" operator="beginsWith" text="#">
+      <formula>LEFT(A301,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A309">
-    <cfRule type="containsText" dxfId="21" priority="117" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A309)))</formula>
+  <conditionalFormatting sqref="A310">
+    <cfRule type="containsText" dxfId="21" priority="125" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A310)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="118" operator="beginsWith" text="#">
-      <formula>LEFT(A309,LEN("#"))="#"</formula>
+    <cfRule type="beginsWith" dxfId="20" priority="126" operator="beginsWith" text="#">
+      <formula>LEFT(A310,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A313">
-    <cfRule type="containsText" dxfId="19" priority="113" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A313)))</formula>
+  <conditionalFormatting sqref="A314">
+    <cfRule type="containsText" dxfId="19" priority="121" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A314)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="114" operator="beginsWith" text="#">
-      <formula>LEFT(A313,LEN("#"))="#"</formula>
+    <cfRule type="beginsWith" dxfId="18" priority="122" operator="beginsWith" text="#">
+      <formula>LEFT(A314,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A318">
-    <cfRule type="containsText" dxfId="17" priority="111" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A318)))</formula>
+  <conditionalFormatting sqref="A319">
+    <cfRule type="containsText" dxfId="17" priority="119" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A319)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="112" operator="beginsWith" text="#">
-      <formula>LEFT(A318,LEN("#"))="#"</formula>
+    <cfRule type="beginsWith" dxfId="16" priority="120" operator="beginsWith" text="#">
+      <formula>LEFT(A319,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A415:A418 A335 A349:A352 B356 A381:A383 A357:B357 B358 B364:B386 B53:B60 B412:B413 B319:B333 B388:B401">
-    <cfRule type="containsText" priority="311" operator="containsText" text="......">
+  <conditionalFormatting sqref="A415:A418 A336 A350:A353 B357 A383:A385 A358:B358 B359 B365:B373 B53:B60 B320:B334 B390:B403 B375:B388 B413">
+    <cfRule type="containsText" priority="319" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="312" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="320" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B336 B338 B340 B342 B344 B346 B348 B314 B312 A353:B355">
-    <cfRule type="containsText" priority="287" operator="containsText" text="......">
+  <conditionalFormatting sqref="B337 B339 B341 B343 B345 B347 B349 B315 B313 A354:B356">
+    <cfRule type="containsText" priority="295" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="288" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="296" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A336 A338 A340 A342 A344 A346 A348 A314 A312 B301 B296 B264">
-    <cfRule type="containsText" priority="289" operator="containsText" text="......">
+  <conditionalFormatting sqref="A337 A339 A341 A343 A345 A347 A349 A315 A313 B302 B297 B264">
+    <cfRule type="containsText" priority="297" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="290" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="298" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B419 B421">
-    <cfRule type="containsText" priority="203" operator="containsText" text="......">
+  <conditionalFormatting sqref="B420">
+    <cfRule type="containsText" priority="211" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="204" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="212" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A419 A421">
-    <cfRule type="containsText" priority="205" operator="containsText" text="......">
+  <conditionalFormatting sqref="A420">
+    <cfRule type="containsText" priority="213" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="206" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="214" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A404:A407">
-    <cfRule type="containsText" priority="2623" operator="containsText" text="......">
+  <conditionalFormatting sqref="A406:A409">
+    <cfRule type="containsText" priority="2631" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2624" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2632" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A24 A33:A41 A27:A30">
-    <cfRule type="containsText" priority="2725" operator="containsText" text="......">
+    <cfRule type="containsText" priority="2733" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2726" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2734" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A317">
-    <cfRule type="containsText" priority="2869" operator="containsText" text="......">
+  <conditionalFormatting sqref="A318">
+    <cfRule type="containsText" priority="2877" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2870" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2878" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A411 B306 B302">
-    <cfRule type="containsText" priority="2873" operator="containsText" text="......">
+  <conditionalFormatting sqref="A412 B307 B303">
+    <cfRule type="containsText" priority="2881" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2874" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2882" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A384:A386 A310 B311 A288:A292 A294 A299 B288:B295 A356 A358 A364:A380 A412 A319:A333 A360 A388:A400">
-    <cfRule type="containsText" priority="2893" operator="containsText" text="......">
+  <conditionalFormatting sqref="A386:A388 A311 B312 A288:A292 A294 A300 B288:B295 A357 A359 A365:A373 A320:A334 A361 A390:A402 A375:A382">
+    <cfRule type="containsText" priority="2901" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2894" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2902" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A422">
-    <cfRule type="containsText" priority="3085" operator="containsText" text="......">
+  <conditionalFormatting sqref="A421">
+    <cfRule type="containsText" priority="3093" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3086" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3094" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46 A62 A134 A141 A177 A191 A20 A26 A32 A43">
-    <cfRule type="containsText" priority="3335" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3343" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3336" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3344" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A219">
-    <cfRule type="containsText" priority="3357" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3365" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3358" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3366" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:B51 A47">
-    <cfRule type="containsText" priority="3507" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3515" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3508" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3516" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A5 A11:A16 A9">
-    <cfRule type="containsText" priority="3627" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3635" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3628" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3636" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A242 A266 A276">
-    <cfRule type="containsText" priority="3693" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3701" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3694" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3702" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A296 B27:B30 B33:B41 B21:B24 A264">
-    <cfRule type="containsText" priority="101" operator="containsText" text="......">
+  <conditionalFormatting sqref="A297 B27:B30 B33:B41 B21:B24 A264">
+    <cfRule type="containsText" priority="109" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="102" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="110" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A281:A282 A230">
-    <cfRule type="containsText" priority="3803" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3811" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3804" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3812" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A301">
-    <cfRule type="containsText" priority="4147" operator="containsText" text="......">
+  <conditionalFormatting sqref="A302">
+    <cfRule type="containsText" priority="4155" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4148" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4156" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A359">
-    <cfRule type="containsText" priority="77" operator="containsText" text="......">
+  <conditionalFormatting sqref="A360">
+    <cfRule type="containsText" priority="85" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="86" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A304:A305">
-    <cfRule type="containsText" priority="4215" operator="containsText" text="......">
+  <conditionalFormatting sqref="A305:A306">
+    <cfRule type="containsText" priority="4223" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4216" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4224" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A308 A286:B286">
-    <cfRule type="containsText" priority="4315" operator="containsText" text="......">
+  <conditionalFormatting sqref="A309 A286:B286">
+    <cfRule type="containsText" priority="4323" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4316" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4324" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B359">
-    <cfRule type="containsText" priority="71" operator="containsText" text="......">
+  <conditionalFormatting sqref="B360">
+    <cfRule type="containsText" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="72" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="80" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B422 A315">
-    <cfRule type="containsText" priority="4419" operator="containsText" text="......">
+  <conditionalFormatting sqref="B421 A316">
+    <cfRule type="containsText" priority="4427" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4420" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4428" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A423 B410:B411 A410 A408:B408">
-    <cfRule type="containsText" priority="4611" operator="containsText" text="......">
+  <conditionalFormatting sqref="A422 B411:B412 A411">
+    <cfRule type="containsText" priority="4619" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4612" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4620" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A414 B308">
-    <cfRule type="containsText" priority="4617" operator="containsText" text="......">
+  <conditionalFormatting sqref="A414 B309">
+    <cfRule type="containsText" priority="4625" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4618" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4626" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B423">
-    <cfRule type="containsText" priority="4685" operator="containsText" text="......">
+  <conditionalFormatting sqref="B422">
+    <cfRule type="containsText" priority="4693" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4686" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4694" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B414">
-    <cfRule type="containsText" priority="5161" operator="containsText" text="......">
+    <cfRule type="containsText" priority="5169" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5170" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B360 B299 B310">
-    <cfRule type="containsText" priority="5455" operator="containsText" text="......">
+  <conditionalFormatting sqref="B361 B300 B311">
+    <cfRule type="containsText" priority="5463" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5456" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5464" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A401">
-    <cfRule type="containsText" priority="5473" operator="containsText" text="......">
+  <conditionalFormatting sqref="A403">
+    <cfRule type="containsText" priority="5481" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5474" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5482" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A295 A311">
-    <cfRule type="containsText" priority="5607" operator="containsText" text="......">
+  <conditionalFormatting sqref="A295 A312">
+    <cfRule type="containsText" priority="5615" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5608" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5616" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A316 B303 B307">
-    <cfRule type="containsText" priority="5683" operator="containsText" text="......">
+  <conditionalFormatting sqref="A317 B304 B308">
+    <cfRule type="containsText" priority="5691" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5684" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5692" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B316">
-    <cfRule type="containsText" dxfId="15" priority="5825" operator="containsText" text="......">
+  <conditionalFormatting sqref="B317">
+    <cfRule type="containsText" dxfId="15" priority="5833" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="5826" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="14" priority="5834" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A334 A63:A85 A87:A91 A98:A133 A135:A139 A178:A182 A184:A189 A192:A194 A196:A208 A210:A215 A217 A220:A227 A231:A240 A243:A260 A267:A275 A277:A280 A265 A262 A142:A175">
-    <cfRule type="containsText" dxfId="13" priority="5829" operator="containsText" text="......">
+  <conditionalFormatting sqref="A335 A63:A85 A87:A91 A98:A133 A135:A139 A178:A182 A184:A189 A192:A194 A196:A208 A210:A215 A217 A220:A227 A231:A240 A243:A260 A267:A275 A277:A280 A265 A262 A142:A175">
+    <cfRule type="containsText" dxfId="13" priority="5837" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="5830" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="12" priority="5838" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B334 A303 A307 B63:B85 B87:B133 B135:B139 B178:B189 B192:B217 B220:B227 B231:B240 B243:B260 B267:B275 B277:B280 A86:B86 A93:A97 A183 A44:B44 B265 B262 B142:B175">
-    <cfRule type="containsText" dxfId="11" priority="5849" operator="containsText" text="......">
+  <conditionalFormatting sqref="B335 A304 A308 B63:B85 B87:B133 B135:B139 B178:B189 B192:B217 B220:B227 B231:B240 B243:B260 B267:B275 B277:B280 A86:B86 A93:A97 A183 A44:B44 B265 B262 B142:B175">
+    <cfRule type="containsText" dxfId="11" priority="5857" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="5850" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="10" priority="5858" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B315 A283:B284 A302 A306">
-    <cfRule type="containsText" dxfId="9" priority="6083" operator="containsText" text="......">
+  <conditionalFormatting sqref="B316 A283:B284 A303 A307">
+    <cfRule type="containsText" dxfId="9" priority="6091" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="6084" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="8" priority="6092" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A287:B287">
-    <cfRule type="containsText" dxfId="7" priority="39" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="7" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="40" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="6" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A285:B285">
-    <cfRule type="containsText" dxfId="5" priority="37" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="5" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="38" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="4" priority="46" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
+    <cfRule type="containsText" priority="43" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="44" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A8">
+    <cfRule type="containsText" priority="41" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="42" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A410:B410">
+    <cfRule type="containsText" priority="39" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="40" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B419">
     <cfRule type="containsText" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13286,23 +13258,15 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A8">
-    <cfRule type="containsText" priority="33" operator="containsText" text="......">
+  <conditionalFormatting sqref="A419">
+    <cfRule type="containsText" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="38" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A409:B409">
-    <cfRule type="containsText" priority="31" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="32" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B420">
+  <conditionalFormatting sqref="A263">
     <cfRule type="containsText" priority="27" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13310,7 +13274,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A420">
+  <conditionalFormatting sqref="B263">
     <cfRule type="containsText" priority="29" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13318,7 +13282,23 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A263">
+  <conditionalFormatting sqref="B299">
+    <cfRule type="containsText" priority="25" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="26" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A299">
+    <cfRule type="containsText" priority="23" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="24" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A298">
     <cfRule type="containsText" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13326,7 +13306,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B263">
+  <conditionalFormatting sqref="B298">
     <cfRule type="containsText" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13334,23 +13314,23 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B298">
-    <cfRule type="containsText" priority="17" operator="containsText" text="......">
+  <conditionalFormatting sqref="A261">
+    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="18" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="2" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A298">
-    <cfRule type="containsText" priority="15" operator="containsText" text="......">
+  <conditionalFormatting sqref="B261">
+    <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="16" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="0" priority="18" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A297">
+  <conditionalFormatting sqref="A389">
     <cfRule type="containsText" priority="11" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13358,7 +13338,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B297">
+  <conditionalFormatting sqref="B389">
     <cfRule type="containsText" priority="13" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13366,23 +13346,39 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A261">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="......">
+  <conditionalFormatting sqref="B52">
+    <cfRule type="containsText" priority="9" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="10" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B261">
-    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="......">
+  <conditionalFormatting sqref="B374">
+    <cfRule type="containsText" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="10" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A387">
+  <conditionalFormatting sqref="A374">
+    <cfRule type="containsText" priority="7" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="8" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B296">
+    <cfRule type="containsText" priority="1" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="2" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A296">
     <cfRule type="containsText" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13390,22 +13386,6 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B387">
-    <cfRule type="containsText" priority="5" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="6" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="containsText" priority="1" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="2" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
+removed non-standard use of IFPORT in DWM +updated some files for archiving and exporting to FAST with DWM names
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@149 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -1900,7 +1900,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="40">
     <dxf>
       <font>
         <u val="none"/>
@@ -2221,108 +2221,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -3269,8 +3167,8 @@
   <dimension ref="A1:K424"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I362" sqref="I362"/>
+      <pane ySplit="15" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A313" sqref="A313:XFD313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10861,10 +10759,10 @@
         <v>33</v>
       </c>
       <c r="D312" s="8" t="s">
-        <v>557</v>
+        <v>506</v>
       </c>
       <c r="E312" s="8" t="s">
-        <v>558</v>
+        <v>519</v>
       </c>
       <c r="F312" s="8" t="s">
         <v>26</v>
@@ -10891,10 +10789,10 @@
         <v>33</v>
       </c>
       <c r="D313" s="8" t="s">
-        <v>506</v>
+        <v>557</v>
       </c>
       <c r="E313" s="8" t="s">
-        <v>519</v>
+        <v>558</v>
       </c>
       <c r="F313" s="8" t="s">
         <v>26</v>
@@ -13656,7 +13554,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A324 B308 B313">
+  <conditionalFormatting sqref="A324 B308 B312">
     <cfRule type="containsText" priority="5731" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13680,7 +13578,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B343 A308 A313 B64:B86 B88:B134 B136:B140 B179:B190 B193:B218 B221:B228 B232:B241 B244:B261 B268:B276 B278:B281 A87:B87 A94:A98 A184 A45:B45 B266 B263 B143:B176">
+  <conditionalFormatting sqref="B343 A308 A312 B64:B86 B88:B134 B136:B140 B179:B190 B193:B218 B221:B228 B232:B241 B244:B261 B268:B276 B278:B281 A87:B87 A94:A98 A184 A45:B45 B266 B263 B143:B176">
     <cfRule type="containsText" dxfId="23" priority="5897" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13888,7 +13786,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B312">
+  <conditionalFormatting sqref="B313">
     <cfRule type="containsText" priority="33" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13896,7 +13794,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A312">
+  <conditionalFormatting sqref="A313">
     <cfRule type="containsText" dxfId="9" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
merged DWM_fromOct3 into trunk, through rev 155
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@157 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -1900,7 +1900,109 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="52">
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <u val="none"/>
@@ -3151,10 +3253,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="50" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3168,7 +3270,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="15" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A313" sqref="A313:XFD313"/>
+      <selection pane="bottomLeft" activeCell="A311" sqref="A311:XFD311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10718,33 +10820,32 @@
       </c>
       <c r="I310" s="4"/>
     </row>
-    <row r="311" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A311" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B311" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C311" s="8" t="s">
+    <row r="311" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B311" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C311" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D311" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E311" s="8" t="s">
+      <c r="D311" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E311" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F311" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G311" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H311" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I311" s="9"/>
-      <c r="J311" s="8" t="s">
+      <c r="F311" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G311" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H311" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J311" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -10817,33 +10918,32 @@
       </c>
       <c r="I315" s="4"/>
     </row>
-    <row r="316" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B316" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C316" s="8" t="s">
+    <row r="316" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B316" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C316" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D316" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E316" s="8" t="s">
+      <c r="D316" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E316" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F316" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G316" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H316" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I316" s="9"/>
-      <c r="J316" s="8" t="s">
+      <c r="F316" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G316" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H316" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J316" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -10916,33 +11016,32 @@
       </c>
       <c r="I320" s="4"/>
     </row>
-    <row r="321" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A321" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B321" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C321" s="8" t="s">
+    <row r="321" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A321" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B321" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C321" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D321" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E321" s="8" t="s">
+      <c r="D321" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E321" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F321" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G321" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H321" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I321" s="9"/>
-      <c r="J321" s="8" t="s">
+      <c r="F321" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G321" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H321" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J321" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -11020,33 +11119,32 @@
       </c>
       <c r="I326" s="4"/>
     </row>
-    <row r="327" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A327" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B327" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C327" s="8" t="s">
+    <row r="327" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C327" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D327" s="8" t="s">
+      <c r="D327" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E327" s="8" t="s">
+      <c r="E327" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F327" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G327" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H327" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I327" s="9"/>
-      <c r="J327" s="8" t="s">
+      <c r="F327" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G327" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H327" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J327" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -13275,342 +13373,390 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A364:A366">
-    <cfRule type="containsText" dxfId="37" priority="197" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="49" priority="211" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A364)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="198" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="48" priority="212" operator="beginsWith" text="#">
       <formula>LEFT(A364,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A304">
-    <cfRule type="containsText" dxfId="35" priority="169" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="47" priority="183" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A304)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="170" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="46" priority="184" operator="beginsWith" text="#">
       <formula>LEFT(A304,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A315">
-    <cfRule type="containsText" dxfId="33" priority="165" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="45" priority="179" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A315)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="166" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="44" priority="180" operator="beginsWith" text="#">
       <formula>LEFT(A315,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A320">
-    <cfRule type="containsText" dxfId="31" priority="161" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="43" priority="175" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A320)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="162" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="42" priority="176" operator="beginsWith" text="#">
       <formula>LEFT(A320,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A326">
-    <cfRule type="containsText" dxfId="29" priority="159" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="41" priority="173" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A326)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="160" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="40" priority="174" operator="beginsWith" text="#">
       <formula>LEFT(A326,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A417:A420 A351:A354 B358 A385:A387 A359:B359 B360 B367:B375 B54:B61 B327:B341 B392:B405 B377:B390 B415">
-    <cfRule type="containsText" priority="359" operator="containsText" text="......">
+  <conditionalFormatting sqref="A417:A420 A351:A354 B358 A385:A387 A359:B359 B360 B367:B375 B54:B61 B328:B341 B392:B405 B377:B390 B415">
+    <cfRule type="containsText" priority="373" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="360" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="374" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B344:B350 B321 B319 A355:B357">
-    <cfRule type="containsText" priority="335" operator="containsText" text="......">
+  <conditionalFormatting sqref="B344:B350 B319 A355:B357">
+    <cfRule type="containsText" priority="349" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="336" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="350" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A344:A350 A321 A319 B305 B298 B265">
-    <cfRule type="containsText" priority="337" operator="containsText" text="......">
+  <conditionalFormatting sqref="A344:A350 A319 B305 B298 B265">
+    <cfRule type="containsText" priority="351" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="338" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="352" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B422">
-    <cfRule type="containsText" priority="251" operator="containsText" text="......">
+    <cfRule type="containsText" priority="265" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="252" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="266" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A422">
-    <cfRule type="containsText" priority="253" operator="containsText" text="......">
+    <cfRule type="containsText" priority="267" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="254" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="268" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A408:A411">
-    <cfRule type="containsText" priority="2671" operator="containsText" text="......">
+    <cfRule type="containsText" priority="2685" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2672" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2686" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A25 A34:A42 A28:A31">
-    <cfRule type="containsText" priority="2773" operator="containsText" text="......">
+    <cfRule type="containsText" priority="2787" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2774" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2788" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A325">
-    <cfRule type="containsText" priority="2917" operator="containsText" text="......">
+    <cfRule type="containsText" priority="2931" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2918" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2932" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A414 B311 B306">
-    <cfRule type="containsText" priority="2921" operator="containsText" text="......">
+  <conditionalFormatting sqref="A414 B306">
+    <cfRule type="containsText" priority="2935" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2922" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2936" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A388:A390 A316 B318 A289:A293 A295 A302 B289:B296 A358 A360 A367:A375 A327:A341 A363 A392:A404 A377:A384">
-    <cfRule type="containsText" priority="2941" operator="containsText" text="......">
+  <conditionalFormatting sqref="A388:A390 B318 A289:A293 A295 A302 B289:B296 A358 A360 A367:A375 A328:A341 A363 A392:A404 A377:A384">
+    <cfRule type="containsText" priority="2955" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2942" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="2956" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A423">
-    <cfRule type="containsText" priority="3133" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3147" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3134" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3148" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47 A63 A135 A142 A178 A192 A21 A27 A33 A44">
-    <cfRule type="containsText" priority="3383" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3397" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3384" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3398" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A220">
-    <cfRule type="containsText" priority="3405" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3419" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3406" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3420" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:B52 A48">
-    <cfRule type="containsText" priority="3555" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3569" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3556" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3570" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A5 A11:A16 A9">
-    <cfRule type="containsText" priority="3675" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3689" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3676" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3690" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A243 A267 A277">
-    <cfRule type="containsText" priority="3741" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3755" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3742" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3756" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A298 B28:B31 B34:B42 B22:B25 A265">
-    <cfRule type="containsText" priority="149" operator="containsText" text="......">
+    <cfRule type="containsText" priority="163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="150" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="164" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A282:A283 A231">
-    <cfRule type="containsText" priority="3851" operator="containsText" text="......">
+    <cfRule type="containsText" priority="3865" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3852" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="3866" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A305">
-    <cfRule type="containsText" priority="4195" operator="containsText" text="......">
+    <cfRule type="containsText" priority="4209" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4196" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4210" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A362">
-    <cfRule type="containsText" priority="125" operator="containsText" text="......">
+    <cfRule type="containsText" priority="139" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="126" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="140" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A309:A310">
-    <cfRule type="containsText" priority="4263" operator="containsText" text="......">
+    <cfRule type="containsText" priority="4277" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4264" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4278" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A314 A287:B287">
-    <cfRule type="containsText" priority="4363" operator="containsText" text="......">
+    <cfRule type="containsText" priority="4377" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4364" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4378" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B362">
-    <cfRule type="containsText" priority="119" operator="containsText" text="......">
+    <cfRule type="containsText" priority="133" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="120" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="134" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B423 A323">
-    <cfRule type="containsText" priority="4467" operator="containsText" text="......">
+    <cfRule type="containsText" priority="4481" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4468" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4482" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B413:B414 A413">
-    <cfRule type="containsText" priority="4659" operator="containsText" text="......">
+    <cfRule type="containsText" priority="4673" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4660" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4674" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A416 B314">
-    <cfRule type="containsText" priority="4665" operator="containsText" text="......">
+    <cfRule type="containsText" priority="4679" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4666" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4680" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B416">
-    <cfRule type="containsText" priority="5209" operator="containsText" text="......">
+    <cfRule type="containsText" priority="5223" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5210" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5224" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B363 B302 B316">
-    <cfRule type="containsText" priority="5503" operator="containsText" text="......">
+  <conditionalFormatting sqref="B363 B302">
+    <cfRule type="containsText" priority="5517" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5504" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5518" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A405">
-    <cfRule type="containsText" priority="5521" operator="containsText" text="......">
+    <cfRule type="containsText" priority="5535" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5522" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5536" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A296 A318">
-    <cfRule type="containsText" priority="5655" operator="containsText" text="......">
+    <cfRule type="containsText" priority="5669" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5656" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5670" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A324 B308 B312">
-    <cfRule type="containsText" priority="5731" operator="containsText" text="......">
+    <cfRule type="containsText" priority="5745" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="5732" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5746" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B324">
-    <cfRule type="containsText" dxfId="27" priority="5873" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="39" priority="5887" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="5874" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="38" priority="5888" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A343 A64:A86 A88:A92 A99:A134 A136:A140 A179:A183 A185:A190 A193:A195 A197:A209 A211:A216 A218 A221:A228 A232:A241 A244:A261 A268:A276 A278:A281 A266 A263 A143:A176">
-    <cfRule type="containsText" dxfId="25" priority="5877" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="37" priority="5891" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="5878" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="36" priority="5892" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B343 A308 A312 B64:B86 B88:B134 B136:B140 B179:B190 B193:B218 B221:B228 B232:B241 B244:B261 B268:B276 B278:B281 A87:B87 A94:A98 A184 A45:B45 B266 B263 B143:B176">
-    <cfRule type="containsText" dxfId="23" priority="5897" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="35" priority="5911" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="5898" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="34" priority="5912" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B323 A284:B285 A306 A311">
-    <cfRule type="containsText" dxfId="21" priority="6131" operator="containsText" text="......">
+  <conditionalFormatting sqref="B323 A284:B285 A306">
+    <cfRule type="containsText" dxfId="33" priority="6145" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="6132" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="32" priority="6146" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A288:B288">
-    <cfRule type="containsText" dxfId="19" priority="87" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="31" priority="101" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="88" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="30" priority="102" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A286:B286">
-    <cfRule type="containsText" dxfId="17" priority="85" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="29" priority="99" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="86" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="28" priority="100" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
+    <cfRule type="containsText" priority="97" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="98" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A8">
+    <cfRule type="containsText" priority="95" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="96" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A412:B412">
+    <cfRule type="containsText" priority="93" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="94" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B421">
+    <cfRule type="containsText" priority="89" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="90" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A421">
+    <cfRule type="containsText" priority="91" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="92" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A264">
+    <cfRule type="containsText" priority="81" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="82" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B264">
     <cfRule type="containsText" priority="83" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13618,15 +13764,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A8">
-    <cfRule type="containsText" priority="81" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="82" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A412:B412">
+  <conditionalFormatting sqref="B300">
     <cfRule type="containsText" priority="79" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13634,7 +13772,23 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B421">
+  <conditionalFormatting sqref="A300">
+    <cfRule type="containsText" priority="77" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="78" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A299">
+    <cfRule type="containsText" priority="73" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="74" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B299">
     <cfRule type="containsText" priority="75" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13642,15 +13796,31 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A421">
-    <cfRule type="containsText" priority="77" operator="containsText" text="......">
+  <conditionalFormatting sqref="A262">
+    <cfRule type="containsText" dxfId="27" priority="69" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="78" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="26" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A264">
+  <conditionalFormatting sqref="B262">
+    <cfRule type="containsText" dxfId="25" priority="71" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="24" priority="72" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A391">
+    <cfRule type="containsText" priority="65" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="66" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B391">
     <cfRule type="containsText" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13658,23 +13828,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B264">
-    <cfRule type="containsText" priority="69" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="70" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B300">
-    <cfRule type="containsText" priority="65" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="66" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A300">
+  <conditionalFormatting sqref="B53">
     <cfRule type="containsText" priority="63" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13682,7 +13836,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A299">
+  <conditionalFormatting sqref="B376">
     <cfRule type="containsText" priority="59" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13690,7 +13844,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B299">
+  <conditionalFormatting sqref="A376">
     <cfRule type="containsText" priority="61" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13698,23 +13852,23 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A262">
-    <cfRule type="containsText" dxfId="15" priority="55" operator="containsText" text="......">
+  <conditionalFormatting sqref="B297">
+    <cfRule type="containsText" priority="55" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="56" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="56" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B262">
-    <cfRule type="containsText" dxfId="13" priority="57" operator="containsText" text="......">
+  <conditionalFormatting sqref="A297">
+    <cfRule type="containsText" priority="57" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="58" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A391">
+  <conditionalFormatting sqref="B307">
     <cfRule type="containsText" priority="51" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13722,23 +13876,39 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B391">
-    <cfRule type="containsText" priority="53" operator="containsText" text="......">
+  <conditionalFormatting sqref="A307">
+    <cfRule type="containsText" dxfId="23" priority="53" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="54" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="22" priority="54" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53">
-    <cfRule type="containsText" priority="49" operator="containsText" text="......">
+  <conditionalFormatting sqref="B313">
+    <cfRule type="containsText" priority="47" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="50" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="48" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B376">
+  <conditionalFormatting sqref="A313">
+    <cfRule type="containsText" dxfId="21" priority="49" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="20" priority="50" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A301">
+    <cfRule type="containsText" priority="43" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="44" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B301">
     <cfRule type="containsText" priority="45" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13746,31 +13916,31 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A376">
-    <cfRule type="containsText" priority="47" operator="containsText" text="......">
+  <conditionalFormatting sqref="B303">
+    <cfRule type="containsText" priority="39" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="48" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="40" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B297">
-    <cfRule type="containsText" priority="41" operator="containsText" text="......">
+  <conditionalFormatting sqref="A303">
+    <cfRule type="containsText" dxfId="19" priority="41" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="42" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="18" priority="42" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A297">
-    <cfRule type="containsText" priority="43" operator="containsText" text="......">
+  <conditionalFormatting sqref="B317">
+    <cfRule type="containsText" priority="35" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="44" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B307">
+  <conditionalFormatting sqref="A317">
     <cfRule type="containsText" priority="37" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13778,39 +13948,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A307">
-    <cfRule type="containsText" dxfId="11" priority="39" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="40" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B313">
-    <cfRule type="containsText" priority="33" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="34" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A313">
-    <cfRule type="containsText" dxfId="9" priority="35" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="36" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A301">
-    <cfRule type="containsText" priority="29" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="30" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B301">
+  <conditionalFormatting sqref="A322">
     <cfRule type="containsText" priority="31" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13818,7 +13956,39 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B303">
+  <conditionalFormatting sqref="B322">
+    <cfRule type="containsText" dxfId="17" priority="33" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="34" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A342">
+    <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="28" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B342">
+    <cfRule type="containsText" dxfId="13" priority="29" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="12" priority="30" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B406">
+    <cfRule type="containsText" priority="23" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="24" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A406">
     <cfRule type="containsText" priority="25" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13826,15 +13996,15 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A303">
-    <cfRule type="containsText" dxfId="7" priority="27" operator="containsText" text="......">
+  <conditionalFormatting sqref="A424">
+    <cfRule type="containsText" priority="19" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="20" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B317">
+  <conditionalFormatting sqref="B424">
     <cfRule type="containsText" priority="21" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13842,15 +14012,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A317">
-    <cfRule type="containsText" priority="23" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="24" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A322">
+  <conditionalFormatting sqref="A361">
     <cfRule type="containsText" priority="17" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13858,47 +14020,23 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B322">
-    <cfRule type="containsText" dxfId="5" priority="19" operator="containsText" text="......">
+  <conditionalFormatting sqref="B361">
+    <cfRule type="containsText" priority="15" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="20" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="16" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A342">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="......">
+  <conditionalFormatting sqref="A327">
+    <cfRule type="containsText" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="14" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B342">
-    <cfRule type="containsText" dxfId="1" priority="15" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="16" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B406">
-    <cfRule type="containsText" priority="9" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="10" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A406">
-    <cfRule type="containsText" priority="11" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="12" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A424">
+  <conditionalFormatting sqref="A321">
     <cfRule type="containsText" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13906,15 +14044,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B424">
-    <cfRule type="containsText" priority="7" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="8" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A361">
+  <conditionalFormatting sqref="A316">
     <cfRule type="containsText" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13922,7 +14052,7 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B361">
+  <conditionalFormatting sqref="A311">
     <cfRule type="containsText" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
added air density as initialization output (for OpenFOAM coupling) modified for mesh orientation fields changed to R8Ki and compiling in both single and double precision added some blank lines to *.AD.out file so headers are on same line as FAST output
git-svn-id: https://windsvn2.nrel.gov/AeroDyn/trunk@200 9add3c13-68b6-420a-9438-b3321c957034
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
+++ b/modules-local/aerodyn14/src/AD_RegistryEntries.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="560">
   <si>
     <t>###################################################################################################################################</t>
   </si>
@@ -1191,9 +1191,6 @@
     <t>Rho</t>
   </si>
   <si>
-    <t>kg/m&amp;3</t>
-  </si>
-  <si>
     <t>KinVisc</t>
   </si>
   <si>
@@ -1755,12 +1752,6 @@
     <t>"hub height wrt inertial origin"</t>
   </si>
   <si>
-    <t>MWS</t>
-  </si>
-  <si>
-    <t>"mean wind speed (for check on dynamic inflow)"</t>
-  </si>
-  <si>
     <t>AeroDyn14/AD14</t>
   </si>
   <si>
@@ -1768,6 +1759,12 @@
   </si>
   <si>
     <t># This Registry file is used to create MODULE AeroDyn_Types  which contains all of the user-defined types needed in AeroDyn14.</t>
+  </si>
+  <si>
+    <t>AirDens</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
   </si>
 </sst>
 </file>
@@ -1864,7 +1861,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <u val="none"/>
@@ -2117,6 +2165,57 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -3047,10 +3146,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="2" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="36" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3062,9 +3161,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K416"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A454" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C457" sqref="C457"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="15" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A301" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3090,13 +3189,13 @@
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -3120,19 +3219,19 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -3214,10 +3313,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3231,7 +3330,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>110</v>
@@ -3246,7 +3345,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>26</v>
@@ -3276,7 +3375,7 @@
         <v>114</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>26</v>
@@ -3306,7 +3405,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>26</v>
@@ -3336,7 +3435,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>26</v>
@@ -3357,7 +3456,7 @@
         <v>47</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>117</v>
@@ -3435,7 +3534,7 @@
         <v>22</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>121</v>
@@ -3711,7 +3810,7 @@
         <v>47</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>131</v>
@@ -3747,7 +3846,7 @@
         <v>22</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>132</v>
@@ -4142,7 +4241,7 @@
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I62" s="4"/>
     </row>
@@ -4154,7 +4253,7 @@
         <v>27</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>34</v>
@@ -4184,7 +4283,7 @@
         <v>27</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>34</v>
@@ -4214,7 +4313,7 @@
         <v>27</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>34</v>
@@ -4244,7 +4343,7 @@
         <v>27</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>34</v>
@@ -4274,7 +4373,7 @@
         <v>27</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>34</v>
@@ -4304,7 +4403,7 @@
         <v>27</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>34</v>
@@ -4334,7 +4433,7 @@
         <v>27</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>34</v>
@@ -4364,7 +4463,7 @@
         <v>27</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>34</v>
@@ -4394,7 +4493,7 @@
         <v>27</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>34</v>
@@ -4424,7 +4523,7 @@
         <v>27</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>99</v>
@@ -4454,7 +4553,7 @@
         <v>27</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>99</v>
@@ -4484,7 +4583,7 @@
         <v>27</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>34</v>
@@ -4514,7 +4613,7 @@
         <v>27</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>34</v>
@@ -4544,7 +4643,7 @@
         <v>27</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>34</v>
@@ -4574,7 +4673,7 @@
         <v>27</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>34</v>
@@ -4604,7 +4703,7 @@
         <v>27</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>34</v>
@@ -4634,7 +4733,7 @@
         <v>27</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>34</v>
@@ -4664,7 +4763,7 @@
         <v>27</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>34</v>
@@ -4694,7 +4793,7 @@
         <v>27</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>34</v>
@@ -4724,7 +4823,7 @@
         <v>27</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>34</v>
@@ -4754,7 +4853,7 @@
         <v>27</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>34</v>
@@ -4784,7 +4883,7 @@
         <v>27</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>34</v>
@@ -4814,7 +4913,7 @@
         <v>27</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>34</v>
@@ -4844,7 +4943,7 @@
         <v>27</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>34</v>
@@ -4874,7 +4973,7 @@
         <v>27</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>34</v>
@@ -4904,7 +5003,7 @@
         <v>27</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>34</v>
@@ -4934,7 +5033,7 @@
         <v>27</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>34</v>
@@ -4964,7 +5063,7 @@
         <v>27</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>34</v>
@@ -4994,7 +5093,7 @@
         <v>27</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>34</v>
@@ -5024,7 +5123,7 @@
         <v>27</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>34</v>
@@ -5054,7 +5153,7 @@
         <v>27</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>34</v>
@@ -5084,7 +5183,7 @@
         <v>27</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>34</v>
@@ -5114,7 +5213,7 @@
         <v>27</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>34</v>
@@ -5144,7 +5243,7 @@
         <v>27</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>34</v>
@@ -5174,7 +5273,7 @@
         <v>27</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>34</v>
@@ -5204,7 +5303,7 @@
         <v>27</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>34</v>
@@ -5234,7 +5333,7 @@
         <v>27</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>34</v>
@@ -5264,7 +5363,7 @@
         <v>27</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>34</v>
@@ -5294,7 +5393,7 @@
         <v>27</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>34</v>
@@ -5324,7 +5423,7 @@
         <v>27</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>34</v>
@@ -5354,7 +5453,7 @@
         <v>27</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>34</v>
@@ -5384,7 +5483,7 @@
         <v>27</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>34</v>
@@ -5414,7 +5513,7 @@
         <v>27</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>34</v>
@@ -5444,7 +5543,7 @@
         <v>27</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>34</v>
@@ -5474,7 +5573,7 @@
         <v>27</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>34</v>
@@ -5504,7 +5603,7 @@
         <v>27</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>34</v>
@@ -5534,7 +5633,7 @@
         <v>27</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>34</v>
@@ -5564,7 +5663,7 @@
         <v>27</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D110" s="8" t="s">
         <v>34</v>
@@ -5594,7 +5693,7 @@
         <v>27</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>34</v>
@@ -5624,7 +5723,7 @@
         <v>27</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>34</v>
@@ -5654,7 +5753,7 @@
         <v>27</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>34</v>
@@ -5684,7 +5783,7 @@
         <v>27</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>34</v>
@@ -5714,7 +5813,7 @@
         <v>27</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>34</v>
@@ -5744,7 +5843,7 @@
         <v>27</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D116" s="8" t="s">
         <v>34</v>
@@ -5774,7 +5873,7 @@
         <v>27</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D117" s="8" t="s">
         <v>34</v>
@@ -5804,7 +5903,7 @@
         <v>27</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>34</v>
@@ -5834,7 +5933,7 @@
         <v>27</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>34</v>
@@ -5864,7 +5963,7 @@
         <v>27</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>34</v>
@@ -5894,7 +5993,7 @@
         <v>27</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>34</v>
@@ -5924,7 +6023,7 @@
         <v>27</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>34</v>
@@ -5954,7 +6053,7 @@
         <v>27</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>34</v>
@@ -5984,7 +6083,7 @@
         <v>27</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>34</v>
@@ -6014,7 +6113,7 @@
         <v>27</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>34</v>
@@ -6044,7 +6143,7 @@
         <v>27</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>34</v>
@@ -6076,7 +6175,7 @@
         <v>27</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D127" s="8" t="s">
         <v>34</v>
@@ -6108,7 +6207,7 @@
         <v>27</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>34</v>
@@ -6140,7 +6239,7 @@
         <v>27</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>34</v>
@@ -6172,7 +6271,7 @@
         <v>27</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>34</v>
@@ -6204,7 +6303,7 @@
         <v>27</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>99</v>
@@ -6234,7 +6333,7 @@
         <v>27</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>99</v>
@@ -6261,7 +6360,7 @@
     </row>
     <row r="134" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I134" s="4"/>
     </row>
@@ -6291,7 +6390,7 @@
         <v>26</v>
       </c>
       <c r="I135" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="136" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6320,7 +6419,7 @@
         <v>26</v>
       </c>
       <c r="I136" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="137" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6349,7 +6448,7 @@
         <v>26</v>
       </c>
       <c r="I137" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="138" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6378,7 +6477,7 @@
         <v>26</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="139" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6407,12 +6506,12 @@
         <v>26</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="141" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I141" s="4"/>
     </row>
@@ -6457,7 +6556,7 @@
         <v>22</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C145" s="8" t="s">
         <v>229</v>
@@ -7186,7 +7285,7 @@
         <v>26</v>
       </c>
       <c r="I171" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -7215,7 +7314,7 @@
         <v>26</v>
       </c>
       <c r="I172" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="173" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -7301,7 +7400,7 @@
     </row>
     <row r="177" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I177" s="4"/>
     </row>
@@ -7455,7 +7554,7 @@
         <v>26</v>
       </c>
       <c r="K182" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="183" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -7488,7 +7587,7 @@
         <v>26</v>
       </c>
       <c r="K183" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="184" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -7673,7 +7772,7 @@
     </row>
     <row r="191" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I191" s="4"/>
     </row>
@@ -8303,7 +8402,7 @@
         <v>26</v>
       </c>
       <c r="I212" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="213" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -8452,12 +8551,12 @@
         <v>26</v>
       </c>
       <c r="I217" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="219" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I219" s="4"/>
     </row>
@@ -8514,7 +8613,7 @@
         <v>26</v>
       </c>
       <c r="I221" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J221" s="8" t="s">
         <v>26</v>
@@ -8546,7 +8645,7 @@
         <v>26</v>
       </c>
       <c r="I222" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="223" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -8575,7 +8674,7 @@
         <v>26</v>
       </c>
       <c r="I223" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="224" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -8604,7 +8703,7 @@
         <v>26</v>
       </c>
       <c r="I224" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="225" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -8633,7 +8732,7 @@
         <v>26</v>
       </c>
       <c r="I225" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="226" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -8662,7 +8761,7 @@
         <v>26</v>
       </c>
       <c r="I226" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="227" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -8691,12 +8790,12 @@
         <v>26</v>
       </c>
       <c r="I227" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="230" spans="1:9" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I230" s="4"/>
     </row>
@@ -8726,7 +8825,7 @@
         <v>26</v>
       </c>
       <c r="I231" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="232" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -8974,7 +9073,7 @@
     </row>
     <row r="242" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I242" s="4"/>
     </row>
@@ -9166,7 +9265,7 @@
         <v>26</v>
       </c>
       <c r="I249" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="250" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9195,7 +9294,7 @@
         <v>26</v>
       </c>
       <c r="I250" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="251" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9224,7 +9323,7 @@
         <v>26</v>
       </c>
       <c r="I251" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="252" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9253,7 +9352,7 @@
         <v>26</v>
       </c>
       <c r="I252" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="253" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9282,7 +9381,7 @@
         <v>26</v>
       </c>
       <c r="I253" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="254" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9311,7 +9410,7 @@
         <v>26</v>
       </c>
       <c r="I254" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="255" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9340,7 +9439,7 @@
         <v>26</v>
       </c>
       <c r="I255" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J255" s="8" t="s">
         <v>103</v>
@@ -9372,7 +9471,7 @@
         <v>26</v>
       </c>
       <c r="I256" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="257" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9401,7 +9500,7 @@
         <v>26</v>
       </c>
       <c r="I257" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="258" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9430,7 +9529,7 @@
         <v>26</v>
       </c>
       <c r="I258" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="259" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9459,7 +9558,7 @@
         <v>26</v>
       </c>
       <c r="I259" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="260" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9488,7 +9587,7 @@
         <v>26</v>
       </c>
       <c r="I260" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="261" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9517,7 +9616,7 @@
         <v>26</v>
       </c>
       <c r="I261" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J261" s="8" t="s">
         <v>103</v>
@@ -9537,19 +9636,19 @@
         <v>99</v>
       </c>
       <c r="E262" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="F262" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G262" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H262" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I262" s="9" t="s">
         <v>520</v>
-      </c>
-      <c r="F262" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G262" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H262" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I262" s="9" t="s">
-        <v>521</v>
       </c>
       <c r="J262" s="8" t="s">
         <v>103</v>
@@ -9569,7 +9668,7 @@
         <v>41</v>
       </c>
       <c r="E263" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F263" s="8" t="s">
         <v>26</v>
@@ -9581,7 +9680,7 @@
         <v>26</v>
       </c>
       <c r="I263" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="264" spans="1:10" s="8" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -9598,7 +9697,7 @@
         <v>34</v>
       </c>
       <c r="E264" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F264" s="8" t="s">
         <v>31</v>
@@ -9610,7 +9709,7 @@
         <v>26</v>
       </c>
       <c r="I264" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J264" s="8" t="s">
         <v>26</v>
@@ -9621,7 +9720,7 @@
     </row>
     <row r="266" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I266" s="4"/>
     </row>
@@ -9813,10 +9912,10 @@
         <v>26</v>
       </c>
       <c r="I273" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J273" s="8" t="s">
-        <v>368</v>
+        <v>559</v>
       </c>
     </row>
     <row r="274" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9833,22 +9932,22 @@
         <v>34</v>
       </c>
       <c r="E274" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="F274" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G274" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H274" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I274" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="J274" s="8" t="s">
         <v>369</v>
-      </c>
-      <c r="F274" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G274" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H274" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I274" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="J274" s="8" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="275" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9856,19 +9955,19 @@
     </row>
     <row r="276" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B276" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="B276" s="3" t="s">
+      <c r="C276" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="C276" s="3" t="s">
+      <c r="D276" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="D276" s="3" t="s">
+      <c r="E276" s="3" t="s">
         <v>374</v>
-      </c>
-      <c r="E276" s="3" t="s">
-        <v>375</v>
       </c>
       <c r="I276" s="4"/>
     </row>
@@ -9880,16 +9979,16 @@
         <v>22</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C278" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="D278" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E278" s="8" t="s">
         <v>376</v>
-      </c>
-      <c r="D278" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E278" s="8" t="s">
-        <v>377</v>
       </c>
       <c r="F278" s="8">
         <v>3</v>
@@ -9901,7 +10000,7 @@
         <v>26</v>
       </c>
       <c r="I278" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="279" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9909,16 +10008,16 @@
         <v>22</v>
       </c>
       <c r="B279" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C279" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="D279" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E279" s="8" t="s">
         <v>378</v>
-      </c>
-      <c r="D279" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E279" s="8" t="s">
-        <v>379</v>
       </c>
       <c r="F279" s="8" t="s">
         <v>114</v>
@@ -9930,7 +10029,7 @@
         <v>26</v>
       </c>
       <c r="I279" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="280" spans="1:10" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9953,7 +10052,7 @@
         <v>47</v>
       </c>
       <c r="B283" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C283" s="8" t="s">
         <v>23</v>
@@ -9980,7 +10079,7 @@
         <v>22</v>
       </c>
       <c r="B284" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C284" s="8" t="s">
         <v>23</v>
@@ -9989,7 +10088,7 @@
         <v>24</v>
       </c>
       <c r="E284" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F284" s="8" t="s">
         <v>26</v>
@@ -10001,7 +10100,7 @@
         <v>26</v>
       </c>
       <c r="I284" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="285" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10018,7 +10117,7 @@
         <v>24</v>
       </c>
       <c r="E285" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F285" s="8" t="s">
         <v>26</v>
@@ -10045,7 +10144,7 @@
         <v>24</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F286" s="8" t="s">
         <v>26</v>
@@ -10057,7 +10156,7 @@
         <v>26</v>
       </c>
       <c r="I286" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="287" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10086,7 +10185,7 @@
         <v>26</v>
       </c>
       <c r="I287" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="288" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10115,7 +10214,7 @@
         <v>26</v>
       </c>
       <c r="I288" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="289" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10144,7 +10243,7 @@
         <v>26</v>
       </c>
       <c r="I289" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="290" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10173,7 +10272,7 @@
         <v>26</v>
       </c>
       <c r="I290" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="291" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10187,10 +10286,10 @@
         <v>23</v>
       </c>
       <c r="D291" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E291" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F291" s="8" t="s">
         <v>87</v>
@@ -10202,7 +10301,7 @@
         <v>26</v>
       </c>
       <c r="I291" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="292" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10216,10 +10315,10 @@
         <v>23</v>
       </c>
       <c r="D292" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E292" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F292" s="8" t="s">
         <v>26</v>
@@ -10231,7 +10330,7 @@
         <v>26</v>
       </c>
       <c r="I292" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="293" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10245,10 +10344,10 @@
         <v>23</v>
       </c>
       <c r="D293" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E293" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F293" s="8" t="s">
         <v>87</v>
@@ -10260,7 +10359,7 @@
         <v>26</v>
       </c>
       <c r="I293" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="294" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10277,7 +10376,7 @@
         <v>99</v>
       </c>
       <c r="E294" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I294" s="9"/>
     </row>
@@ -10295,19 +10394,19 @@
         <v>99</v>
       </c>
       <c r="E295" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="F295" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G295" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H295" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I295" s="9" t="s">
         <v>527</v>
-      </c>
-      <c r="F295" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G295" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="H295" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I295" s="9" t="s">
-        <v>528</v>
       </c>
       <c r="J295" s="8" t="s">
         <v>26</v>
@@ -10327,7 +10426,7 @@
         <v>121</v>
       </c>
       <c r="E296" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F296" s="8" t="s">
         <v>26</v>
@@ -10357,7 +10456,7 @@
         <v>41</v>
       </c>
       <c r="E297" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F297" s="8" t="s">
         <v>26</v>
@@ -10369,7 +10468,7 @@
         <v>26</v>
       </c>
       <c r="I297" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="298" spans="1:10" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -10386,7 +10485,7 @@
         <v>34</v>
       </c>
       <c r="E298" s="8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F298" s="8" t="s">
         <v>87</v>
@@ -10398,7 +10497,7 @@
         <v>26</v>
       </c>
       <c r="I298" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J298" s="8" t="s">
         <v>26</v>
@@ -10418,19 +10517,19 @@
         <v>34</v>
       </c>
       <c r="E299" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="F299" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G299" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H299" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I299" s="9" t="s">
         <v>554</v>
-      </c>
-      <c r="F299" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G299" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H299" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I299" s="9" t="s">
-        <v>555</v>
       </c>
       <c r="J299" s="8" t="s">
         <v>103</v>
@@ -10447,10 +10546,10 @@
         <v>23</v>
       </c>
       <c r="D300" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="E300" s="8" t="s">
         <v>534</v>
-      </c>
-      <c r="E300" s="8" t="s">
-        <v>535</v>
       </c>
       <c r="F300" s="8" t="s">
         <v>26</v>
@@ -10467,61 +10566,58 @@
       </c>
     </row>
     <row r="301" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B301" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C301" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D301" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E301" s="8" t="s">
-        <v>556</v>
-      </c>
-      <c r="F301" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G301" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H301" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I301" s="9" t="s">
-        <v>557</v>
-      </c>
-      <c r="J301" s="8" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="302" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="I302" s="9"/>
-    </row>
-    <row r="303" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A303" s="3" t="s">
+      <c r="I301" s="9"/>
+    </row>
+    <row r="302" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A302" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I303" s="4"/>
+      <c r="I302" s="4"/>
+    </row>
+    <row r="303" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A303" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B303" s="8" t="s">
+        <v>555</v>
+      </c>
+      <c r="C303" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D303" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E303" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F303" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G303" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H303" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I303" s="9" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="304" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A304" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>558</v>
+        <v>27</v>
       </c>
       <c r="C304" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D304" s="8" t="s">
-        <v>91</v>
+        <v>529</v>
       </c>
       <c r="E304" s="8" t="s">
-        <v>92</v>
+        <v>530</v>
       </c>
       <c r="F304" s="8" t="s">
         <v>26</v>
@@ -10532,8 +10628,9 @@
       <c r="H304" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I304" s="9" t="s">
-        <v>499</v>
+      <c r="I304" s="9"/>
+      <c r="J304" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="305" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10547,10 +10644,10 @@
         <v>28</v>
       </c>
       <c r="D305" s="8" t="s">
-        <v>530</v>
+        <v>34</v>
       </c>
       <c r="E305" s="8" t="s">
-        <v>531</v>
+        <v>558</v>
       </c>
       <c r="F305" s="8" t="s">
         <v>26</v>
@@ -10561,14 +10658,14 @@
       <c r="H305" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I305" s="9"/>
+      <c r="I305" s="9" t="s">
+        <v>464</v>
+      </c>
       <c r="J305" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="306" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="I306" s="9"/>
-    </row>
+        <v>559</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="307" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A307" s="3" t="s">
         <v>7</v>
@@ -10621,10 +10718,10 @@
         <v>33</v>
       </c>
       <c r="D310" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="E310" s="8" t="s">
         <v>532</v>
-      </c>
-      <c r="E310" s="8" t="s">
-        <v>533</v>
       </c>
       <c r="F310" s="8" t="s">
         <v>26</v>
@@ -10689,10 +10786,10 @@
         <v>36</v>
       </c>
       <c r="D314" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="E314" s="8" t="s">
         <v>536</v>
-      </c>
-      <c r="E314" s="8" t="s">
-        <v>537</v>
       </c>
       <c r="F314" s="8" t="s">
         <v>26</v>
@@ -10757,10 +10854,10 @@
         <v>38</v>
       </c>
       <c r="D318" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="E318" s="8" t="s">
         <v>538</v>
-      </c>
-      <c r="E318" s="8" t="s">
-        <v>539</v>
       </c>
       <c r="F318" s="8" t="s">
         <v>26</v>
@@ -10781,7 +10878,7 @@
     </row>
     <row r="320" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A320" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="321" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -10845,7 +10942,7 @@
         <v>26</v>
       </c>
       <c r="I323" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J323" s="8" t="s">
         <v>46</v>
@@ -10895,7 +10992,7 @@
         <v>44</v>
       </c>
       <c r="E325" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F325" s="8" t="s">
         <v>26</v>
@@ -10922,7 +11019,7 @@
         <v>34</v>
       </c>
       <c r="E326" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F326" s="8" t="s">
         <v>26</v>
@@ -10934,7 +11031,7 @@
         <v>26</v>
       </c>
       <c r="I326" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="327" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10951,7 +11048,7 @@
         <v>34</v>
       </c>
       <c r="E327" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F327" s="8" t="s">
         <v>26</v>
@@ -10963,7 +11060,7 @@
         <v>26</v>
       </c>
       <c r="I327" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="328" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -10980,7 +11077,7 @@
         <v>34</v>
       </c>
       <c r="E328" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F328" s="8" t="s">
         <v>26</v>
@@ -10992,7 +11089,7 @@
         <v>26</v>
       </c>
       <c r="I328" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="329" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11009,7 +11106,7 @@
         <v>34</v>
       </c>
       <c r="E329" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F329" s="8" t="s">
         <v>26</v>
@@ -11021,7 +11118,7 @@
         <v>26</v>
       </c>
       <c r="I329" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="330" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11038,19 +11135,19 @@
         <v>99</v>
       </c>
       <c r="E330" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="F330" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G330" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="F330" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G330" s="8" t="s">
-        <v>393</v>
-      </c>
       <c r="H330" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I330" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="331" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11067,19 +11164,19 @@
         <v>99</v>
       </c>
       <c r="E331" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="F331" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G331" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="F331" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G331" s="8" t="s">
-        <v>395</v>
-      </c>
       <c r="H331" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I331" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="332" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11096,19 +11193,19 @@
         <v>99</v>
       </c>
       <c r="E332" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F332" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G332" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H332" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I332" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="333" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11125,19 +11222,19 @@
         <v>99</v>
       </c>
       <c r="E333" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F333" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G333" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H333" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I333" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="334" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11154,13 +11251,13 @@
         <v>99</v>
       </c>
       <c r="E334" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F334" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G334" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H334" s="8" t="s">
         <v>26</v>
@@ -11183,13 +11280,13 @@
         <v>99</v>
       </c>
       <c r="E335" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F335" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G335" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H335" s="8" t="s">
         <v>26</v>
@@ -11213,7 +11310,7 @@
         <v>89</v>
       </c>
       <c r="E336" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F336" s="8" t="s">
         <v>26</v>
@@ -11225,7 +11322,7 @@
         <v>26</v>
       </c>
       <c r="I336" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="337" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11239,10 +11336,10 @@
         <v>40</v>
       </c>
       <c r="D337" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="E337" s="8" t="s">
         <v>540</v>
-      </c>
-      <c r="E337" s="8" t="s">
-        <v>541</v>
       </c>
       <c r="F337" s="8" t="s">
         <v>26</v>
@@ -11287,10 +11384,10 @@
         <v>40</v>
       </c>
       <c r="D339" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E339" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I339" s="9"/>
     </row>
@@ -11392,19 +11489,19 @@
     </row>
     <row r="346" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A346" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I346" s="4"/>
     </row>
     <row r="347" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A347" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I347" s="4"/>
     </row>
     <row r="348" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A348" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B348" s="10" t="s">
         <v>27</v>
@@ -11416,7 +11513,7 @@
         <v>131</v>
       </c>
       <c r="E348" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F348" s="10" t="s">
         <v>26</v>
@@ -11428,7 +11525,7 @@
         <v>26</v>
       </c>
       <c r="I348" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="349" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11445,13 +11542,13 @@
         <v>111</v>
       </c>
       <c r="E349" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F349" s="8" t="s">
         <v>88</v>
       </c>
       <c r="I349" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="350" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11468,13 +11565,13 @@
         <v>111</v>
       </c>
       <c r="E350" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F350" s="8" t="s">
         <v>88</v>
       </c>
       <c r="I350" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="351" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11491,19 +11588,19 @@
         <v>99</v>
       </c>
       <c r="E351" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="F351" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G351" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H351" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I351" s="8" t="s">
         <v>522</v>
-      </c>
-      <c r="F351" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G351" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H351" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I351" s="8" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="352" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11520,7 +11617,7 @@
         <v>289</v>
       </c>
       <c r="E352" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I352" s="9"/>
     </row>
@@ -11538,7 +11635,7 @@
         <v>99</v>
       </c>
       <c r="E353" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F353" s="8" t="s">
         <v>26</v>
@@ -11565,7 +11662,7 @@
         <v>99</v>
       </c>
       <c r="E354" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F354" s="8" t="s">
         <v>26</v>
@@ -11577,7 +11674,7 @@
         <v>26</v>
       </c>
       <c r="I354" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="355" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11591,10 +11688,10 @@
         <v>40</v>
       </c>
       <c r="D355" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="E355" s="8" t="s">
         <v>546</v>
-      </c>
-      <c r="E355" s="8" t="s">
-        <v>547</v>
       </c>
       <c r="F355" s="8" t="s">
         <v>26</v>
@@ -11663,7 +11760,7 @@
         <v>24</v>
       </c>
       <c r="E361" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F361" s="8" t="s">
         <v>26</v>
@@ -11675,7 +11772,7 @@
         <v>26</v>
       </c>
       <c r="I361" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="362" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11692,7 +11789,7 @@
         <v>99</v>
       </c>
       <c r="E362" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F362" s="8" t="s">
         <v>26</v>
@@ -11713,13 +11810,13 @@
         <v>99</v>
       </c>
       <c r="E363" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F363" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G363" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H363" s="8" t="s">
         <v>26</v>
@@ -11740,7 +11837,7 @@
         <v>99</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F364" s="8" t="s">
         <v>26</v>
@@ -11761,7 +11858,7 @@
         <v>99</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I365" s="9"/>
     </row>
@@ -11779,13 +11876,13 @@
         <v>99</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F366" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G366" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I366" s="9"/>
     </row>
@@ -11803,13 +11900,13 @@
         <v>99</v>
       </c>
       <c r="E367" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F367" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G367" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H367" s="8" t="s">
         <v>26</v>
@@ -11833,19 +11930,19 @@
         <v>99</v>
       </c>
       <c r="E368" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="F368" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G368" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H368" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I368" s="9" t="s">
         <v>527</v>
-      </c>
-      <c r="F368" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G368" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="H368" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I368" s="9" t="s">
-        <v>528</v>
       </c>
       <c r="J368" s="8" t="s">
         <v>26</v>
@@ -11877,7 +11974,7 @@
         <v>26</v>
       </c>
       <c r="I369" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J369" s="8" t="s">
         <v>26</v>
@@ -11909,7 +12006,7 @@
         <v>26</v>
       </c>
       <c r="I370" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="371" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11938,7 +12035,7 @@
         <v>26</v>
       </c>
       <c r="I371" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="372" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11955,7 +12052,7 @@
         <v>99</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F372" s="8" t="s">
         <v>26</v>
@@ -11982,7 +12079,7 @@
         <v>99</v>
       </c>
       <c r="E373" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F373" s="8" t="s">
         <v>26</v>
@@ -11994,7 +12091,7 @@
         <v>26</v>
       </c>
       <c r="I373" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="374" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12011,7 +12108,7 @@
         <v>99</v>
       </c>
       <c r="E374" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F374" s="8" t="s">
         <v>26</v>
@@ -12023,7 +12120,7 @@
         <v>26</v>
       </c>
       <c r="I374" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="375" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12040,7 +12137,7 @@
         <v>99</v>
       </c>
       <c r="E375" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F375" s="8" t="s">
         <v>26</v>
@@ -12061,7 +12158,7 @@
         <v>99</v>
       </c>
       <c r="E376" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F376" s="8" t="s">
         <v>26</v>
@@ -12073,7 +12170,7 @@
         <v>26</v>
       </c>
       <c r="I376" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="377" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12090,7 +12187,7 @@
         <v>99</v>
       </c>
       <c r="E377" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F377" s="8" t="s">
         <v>26</v>
@@ -12102,7 +12199,7 @@
         <v>26</v>
       </c>
       <c r="I377" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="378" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12119,7 +12216,7 @@
         <v>99</v>
       </c>
       <c r="E378" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F378" s="8" t="s">
         <v>26</v>
@@ -12131,7 +12228,7 @@
         <v>26</v>
       </c>
       <c r="I378" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="379" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12148,7 +12245,7 @@
         <v>44</v>
       </c>
       <c r="E379" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F379" s="8" t="s">
         <v>26</v>
@@ -12160,7 +12257,7 @@
         <v>26</v>
       </c>
       <c r="I379" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="380" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12189,7 +12286,7 @@
         <v>26</v>
       </c>
       <c r="I380" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J380" s="8" t="s">
         <v>103</v>
@@ -12209,7 +12306,7 @@
         <v>34</v>
       </c>
       <c r="E381" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F381" s="8" t="s">
         <v>26</v>
@@ -12221,7 +12318,7 @@
         <v>26</v>
       </c>
       <c r="I381" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J381" s="8" t="s">
         <v>103</v>
@@ -12241,16 +12338,16 @@
         <v>41</v>
       </c>
       <c r="E382" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F382" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G382" s="8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I382" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="383" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12267,13 +12364,13 @@
         <v>41</v>
       </c>
       <c r="E383" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="F383" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G383" s="8" t="s">
         <v>524</v>
-      </c>
-      <c r="F383" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G383" s="8" t="s">
-        <v>525</v>
       </c>
       <c r="I383" s="9"/>
     </row>
@@ -12291,16 +12388,16 @@
         <v>41</v>
       </c>
       <c r="E384" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F384" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G384" s="8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I384" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="385" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12317,7 +12414,7 @@
         <v>41</v>
       </c>
       <c r="E385" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F385" s="8" t="s">
         <v>26</v>
@@ -12329,7 +12426,7 @@
         <v>26</v>
       </c>
       <c r="I385" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="386" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12346,19 +12443,19 @@
         <v>99</v>
       </c>
       <c r="E386" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F386" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G386" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H386" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I386" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="387" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12375,7 +12472,7 @@
         <v>89</v>
       </c>
       <c r="E387" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F387" s="8" t="s">
         <v>26</v>
@@ -12435,10 +12532,10 @@
         <v>43</v>
       </c>
       <c r="D390" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E390" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I390" s="9"/>
     </row>
@@ -12561,10 +12658,10 @@
         <v>43</v>
       </c>
       <c r="D397" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="E397" s="8" t="s">
         <v>542</v>
-      </c>
-      <c r="E397" s="8" t="s">
-        <v>543</v>
       </c>
       <c r="F397" s="8" t="s">
         <v>26</v>
@@ -12644,7 +12741,7 @@
         <v>56</v>
       </c>
       <c r="E403" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F403" s="8" t="s">
         <v>31</v>
@@ -12656,7 +12753,7 @@
         <v>26</v>
       </c>
       <c r="I403" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J403" s="8" t="s">
         <v>26</v>
@@ -12676,19 +12773,19 @@
         <v>56</v>
       </c>
       <c r="E404" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="F404" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G404" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H404" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I404" s="9" t="s">
         <v>509</v>
-      </c>
-      <c r="F404" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G404" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H404" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I404" s="9" t="s">
-        <v>510</v>
       </c>
       <c r="J404" s="8" t="s">
         <v>26</v>
@@ -12708,7 +12805,7 @@
         <v>121</v>
       </c>
       <c r="E405" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F405" s="8" t="s">
         <v>26</v>
@@ -12720,7 +12817,7 @@
         <v>26</v>
       </c>
       <c r="I405" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="406" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12758,7 +12855,7 @@
         <v>34</v>
       </c>
       <c r="E407" s="8" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F407" s="8" t="s">
         <v>87</v>
@@ -12770,10 +12867,10 @@
         <v>26</v>
       </c>
       <c r="I407" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="J407" s="8" t="s">
         <v>549</v>
-      </c>
-      <c r="J407" s="8" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="408" spans="1:10" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12790,22 +12887,22 @@
         <v>34</v>
       </c>
       <c r="E408" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="F408" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="F408" s="8" t="s">
+      <c r="G408" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H408" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I408" s="9" t="s">
         <v>552</v>
       </c>
-      <c r="G408" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H408" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I408" s="9" t="s">
-        <v>553</v>
-      </c>
       <c r="J408" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="409" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -12875,7 +12972,7 @@
         <v>56</v>
       </c>
       <c r="E414" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F414" s="8" t="s">
         <v>31</v>
@@ -12887,7 +12984,7 @@
         <v>26</v>
       </c>
       <c r="I414" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J414" s="8" t="s">
         <v>26</v>
@@ -12907,19 +13004,19 @@
         <v>56</v>
       </c>
       <c r="E415" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="F415" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G415" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H415" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I415" s="9" t="s">
         <v>511</v>
-      </c>
-      <c r="F415" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G415" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H415" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I415" s="9" t="s">
-        <v>512</v>
       </c>
       <c r="J415" s="8" t="s">
         <v>26</v>
@@ -12936,10 +13033,10 @@
         <v>50</v>
       </c>
       <c r="D416" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="E416" s="8" t="s">
         <v>544</v>
-      </c>
-      <c r="E416" s="8" t="s">
-        <v>545</v>
       </c>
       <c r="F416" s="8" t="s">
         <v>26</v>
@@ -12957,462 +13054,494 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A357:A359">
-    <cfRule type="containsText" dxfId="29" priority="221" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="35" priority="229" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",A357)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="222" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="34" priority="230" operator="beginsWith" text="#">
       <formula>LEFT(A357,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A302">
+    <cfRule type="containsText" dxfId="33" priority="201" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A302)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="32" priority="202" operator="beginsWith" text="#">
+      <formula>LEFT(A302,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A312">
+    <cfRule type="containsText" dxfId="31" priority="197" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A312)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="30" priority="198" operator="beginsWith" text="#">
+      <formula>LEFT(A312,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A316">
+    <cfRule type="containsText" dxfId="29" priority="193" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A316)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="28" priority="194" operator="beginsWith" text="#">
+      <formula>LEFT(A316,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A321">
+    <cfRule type="containsText" dxfId="27" priority="191" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",A321)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="26" priority="192" operator="beginsWith" text="#">
+      <formula>LEFT(A321,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A410:A413 A345:A348 B352 A377:A379 A353:B353 B354 B53:B60 B323:B336 B384:B396 B369:B382 B406:B407 B360:B367">
+    <cfRule type="containsText" priority="391" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="392" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B338:B344 B315 A349:B351">
+    <cfRule type="containsText" priority="367" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="368" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A338:A344 A315 B303 B296 B264">
+    <cfRule type="containsText" priority="369" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="370" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B415">
+    <cfRule type="containsText" priority="283" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="284" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A415">
+    <cfRule type="containsText" priority="285" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="286" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A399:A402">
+    <cfRule type="containsText" priority="2703" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="2704" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:A24 A33:A41 A27:A30">
+    <cfRule type="containsText" priority="2805" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="2806" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A320">
+    <cfRule type="containsText" priority="2949" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="2950" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A405">
+    <cfRule type="containsText" priority="2953" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="2954" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A380:A382 B314 A287:A291 A293 A300 B287:B294 A352 A354 A323:A336 A356 A384:A396 A369:A376 A360:A367">
+    <cfRule type="containsText" priority="2973" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="2974" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46 A62 A134 A141 A177 A191 A20 A26 A32 A43">
+    <cfRule type="containsText" priority="3415" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="3416" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A219">
+    <cfRule type="containsText" priority="3437" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="3438" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:B51 A47">
+    <cfRule type="containsText" priority="3587" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="3588" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A5 A11:A16 A9">
+    <cfRule type="containsText" priority="3707" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="3708" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A242 A266 A276">
+    <cfRule type="containsText" priority="3773" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="3774" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A296 B27:B30 B33:B41 B21:B24 A264">
+    <cfRule type="containsText" priority="181" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="182" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A281:A282 A230">
+    <cfRule type="containsText" priority="3883" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="3884" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A303">
-    <cfRule type="containsText" dxfId="27" priority="193" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A303)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="194" operator="beginsWith" text="#">
-      <formula>LEFT(A303,LEN("#"))="#"</formula>
+    <cfRule type="containsText" priority="4227" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="4228" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A312">
-    <cfRule type="containsText" dxfId="25" priority="189" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A312)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="190" operator="beginsWith" text="#">
-      <formula>LEFT(A312,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="A355">
+    <cfRule type="containsText" priority="157" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="158" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A316">
-    <cfRule type="containsText" dxfId="23" priority="185" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A316)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="186" operator="beginsWith" text="#">
-      <formula>LEFT(A316,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="A307:A308">
+    <cfRule type="containsText" priority="4295" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="4296" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A321">
-    <cfRule type="containsText" dxfId="21" priority="183" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",A321)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="184" operator="beginsWith" text="#">
-      <formula>LEFT(A321,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="A311 A286:B286">
+    <cfRule type="containsText" priority="4395" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="4396" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A410:A413 A345:A348 B352 A377:A379 A353:B353 B354 B53:B60 B323:B336 B384:B396 B369:B382 B406:B407 B360:B367">
-    <cfRule type="containsText" priority="383" operator="containsText" text="......">
+  <conditionalFormatting sqref="B355">
+    <cfRule type="containsText" priority="151" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="384" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="152" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B338:B344 B315 A349:B351">
-    <cfRule type="containsText" priority="359" operator="containsText" text="......">
+  <conditionalFormatting sqref="A318">
+    <cfRule type="containsText" priority="4499" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="360" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4500" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A338:A344 A315 B304 B296 B264">
-    <cfRule type="containsText" priority="361" operator="containsText" text="......">
+  <conditionalFormatting sqref="B404:B405 A404">
+    <cfRule type="containsText" priority="4691" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="362" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4692" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B415">
-    <cfRule type="containsText" priority="275" operator="containsText" text="......">
+  <conditionalFormatting sqref="A409 B311">
+    <cfRule type="containsText" priority="4697" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="276" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="4698" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A415">
-    <cfRule type="containsText" priority="277" operator="containsText" text="......">
+  <conditionalFormatting sqref="B409">
+    <cfRule type="containsText" priority="5241" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="278" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5242" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A399:A402">
-    <cfRule type="containsText" priority="2695" operator="containsText" text="......">
+  <conditionalFormatting sqref="B356 B300">
+    <cfRule type="containsText" priority="5535" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2696" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5536" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:A24 A33:A41 A27:A30">
-    <cfRule type="containsText" priority="2797" operator="containsText" text="......">
+  <conditionalFormatting sqref="A294 A314">
+    <cfRule type="containsText" priority="5687" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2798" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5688" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A320">
-    <cfRule type="containsText" priority="2941" operator="containsText" text="......">
+  <conditionalFormatting sqref="A319">
+    <cfRule type="containsText" priority="5763" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2942" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="5764" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A405">
-    <cfRule type="containsText" priority="2945" operator="containsText" text="......">
+  <conditionalFormatting sqref="B319">
+    <cfRule type="containsText" dxfId="25" priority="5905" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2946" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="24" priority="5906" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A380:A382 B314 A287:A291 A293 A300 B287:B294 A352 A354 A323:A336 A356 A384:A396 A369:A376 A360:A367">
-    <cfRule type="containsText" priority="2965" operator="containsText" text="......">
+  <conditionalFormatting sqref="A337 A63:A85 A87:A91 A98:A133 A135:A139 A178:A182 A184:A189 A192:A194 A196:A208 A210:A215 A217 A220:A227 A231:A240 A243:A260 A267:A275 A277:A280 A265 A262 A142:A175">
+    <cfRule type="containsText" dxfId="23" priority="5909" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="2966" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="22" priority="5910" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A46 A62 A134 A141 A177 A191 A20 A26 A32 A43">
-    <cfRule type="containsText" priority="3407" operator="containsText" text="......">
+  <conditionalFormatting sqref="B337 B63:B85 B87:B133 B135:B139 B178:B189 B192:B217 B220:B227 B231:B240 B243:B260 B267:B275 B277:B280 A86:B86 A93:A97 A183 A44:B44 B265 B262 B142:B175">
+    <cfRule type="containsText" dxfId="21" priority="5929" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3408" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="20" priority="5930" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A219">
-    <cfRule type="containsText" priority="3429" operator="containsText" text="......">
+  <conditionalFormatting sqref="B318 A283:B284">
+    <cfRule type="containsText" dxfId="19" priority="6163" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3430" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="18" priority="6164" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47:B51 A47">
-    <cfRule type="containsText" priority="3579" operator="containsText" text="......">
+  <conditionalFormatting sqref="A285:B285">
+    <cfRule type="containsText" dxfId="17" priority="117" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3580" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="16" priority="118" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A5 A11:A16 A9">
-    <cfRule type="containsText" priority="3699" operator="containsText" text="......">
+  <conditionalFormatting sqref="A10">
+    <cfRule type="containsText" priority="115" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3700" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="116" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A242 A266 A276">
-    <cfRule type="containsText" priority="3765" operator="containsText" text="......">
+  <conditionalFormatting sqref="A6:A8">
+    <cfRule type="containsText" priority="113" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3766" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="114" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A296 B27:B30 B33:B41 B21:B24 A264">
-    <cfRule type="containsText" priority="173" operator="containsText" text="......">
+  <conditionalFormatting sqref="A403:B403">
+    <cfRule type="containsText" priority="111" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="174" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="112" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A281:A282 A230">
-    <cfRule type="containsText" priority="3875" operator="containsText" text="......">
+  <conditionalFormatting sqref="B414">
+    <cfRule type="containsText" priority="107" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="3876" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="108" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A414">
+    <cfRule type="containsText" priority="109" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="110" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A263">
+    <cfRule type="containsText" priority="99" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="100" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B263">
+    <cfRule type="containsText" priority="101" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="102" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B298">
+    <cfRule type="containsText" priority="97" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="98" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A298">
+    <cfRule type="containsText" priority="95" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="96" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A297">
+    <cfRule type="containsText" priority="91" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="92" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B297">
+    <cfRule type="containsText" priority="93" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="94" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A261">
+    <cfRule type="containsText" dxfId="15" priority="87" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="88" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B261">
+    <cfRule type="containsText" dxfId="13" priority="89" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="12" priority="90" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A383">
+    <cfRule type="containsText" priority="83" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="84" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B383">
+    <cfRule type="containsText" priority="85" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="86" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="containsText" priority="81" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="82" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B368">
+    <cfRule type="containsText" priority="77" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="78" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A368">
+    <cfRule type="containsText" priority="79" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="80" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B295">
+    <cfRule type="containsText" priority="73" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="74" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A295">
+    <cfRule type="containsText" priority="75" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="76" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B304">
+    <cfRule type="containsText" priority="69" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="70" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A304">
-    <cfRule type="containsText" priority="4219" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="11" priority="71" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="4220" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="10" priority="72" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A355">
-    <cfRule type="containsText" priority="149" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="150" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A307:A308">
-    <cfRule type="containsText" priority="4287" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="4288" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A311 A286:B286">
-    <cfRule type="containsText" priority="4387" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="4388" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B355">
-    <cfRule type="containsText" priority="143" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="144" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A318">
-    <cfRule type="containsText" priority="4491" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="4492" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B404:B405 A404">
-    <cfRule type="containsText" priority="4683" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="4684" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A409 B311">
-    <cfRule type="containsText" priority="4689" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="4690" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B409">
-    <cfRule type="containsText" priority="5233" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="5234" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B356 B300">
-    <cfRule type="containsText" priority="5527" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="5528" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A294 A314">
-    <cfRule type="containsText" priority="5679" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="5680" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A319 B306">
-    <cfRule type="containsText" priority="5755" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="5756" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B319">
-    <cfRule type="containsText" dxfId="19" priority="5897" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="5898" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A337 A63:A85 A87:A91 A98:A133 A135:A139 A178:A182 A184:A189 A192:A194 A196:A208 A210:A215 A217 A220:A227 A231:A240 A243:A260 A267:A275 A277:A280 A265 A262 A142:A175">
-    <cfRule type="containsText" dxfId="17" priority="5901" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="5902" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B337 A306 B63:B85 B87:B133 B135:B139 B178:B189 B192:B217 B220:B227 B231:B240 B243:B260 B267:B275 B277:B280 A86:B86 A93:A97 A183 A44:B44 B265 B262 B142:B175">
-    <cfRule type="containsText" dxfId="15" priority="5921" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="5922" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B318 A283:B284">
-    <cfRule type="containsText" dxfId="13" priority="6155" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="6156" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A285:B285">
-    <cfRule type="containsText" dxfId="11" priority="109" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="110" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="containsText" priority="107" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="108" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A8">
-    <cfRule type="containsText" priority="105" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="106" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A403:B403">
-    <cfRule type="containsText" priority="103" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="104" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B414">
-    <cfRule type="containsText" priority="99" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="100" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A414">
-    <cfRule type="containsText" priority="101" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="102" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A263">
-    <cfRule type="containsText" priority="91" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="92" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B263">
-    <cfRule type="containsText" priority="93" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="94" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B298">
-    <cfRule type="containsText" priority="89" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="90" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A298">
-    <cfRule type="containsText" priority="87" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="88" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A297">
-    <cfRule type="containsText" priority="83" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="84" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B297">
-    <cfRule type="containsText" priority="85" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="86" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A261">
-    <cfRule type="containsText" dxfId="9" priority="79" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="80" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B261">
-    <cfRule type="containsText" dxfId="7" priority="81" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="82" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A383">
-    <cfRule type="containsText" priority="75" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="76" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B383">
-    <cfRule type="containsText" priority="77" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="78" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="containsText" priority="73" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="74" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B368">
-    <cfRule type="containsText" priority="69" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="70" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A368">
-    <cfRule type="containsText" priority="71" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="72" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B295">
+  <conditionalFormatting sqref="B310">
     <cfRule type="containsText" priority="65" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
@@ -13420,163 +13549,147 @@
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A295">
-    <cfRule type="containsText" priority="67" operator="containsText" text="......">
+  <conditionalFormatting sqref="A310">
+    <cfRule type="containsText" dxfId="9" priority="67" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="68" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="8" priority="68" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B301">
+    <cfRule type="containsText" priority="57" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="58" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A301">
+    <cfRule type="containsText" dxfId="7" priority="59" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="60" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B397">
+    <cfRule type="containsText" priority="41" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="42" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A397">
+    <cfRule type="containsText" priority="43" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="44" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A416">
+    <cfRule type="containsText" priority="37" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="38" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B416">
+    <cfRule type="containsText" priority="39" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="40" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A322">
+    <cfRule type="containsText" priority="25" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="26" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A317">
+    <cfRule type="containsText" priority="23" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="24" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A313">
+    <cfRule type="containsText" priority="21" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="22" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A309">
+    <cfRule type="containsText" priority="19" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="20" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B408">
+    <cfRule type="containsText" priority="17" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="18" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B299">
+    <cfRule type="containsText" priority="15" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="16" operator="beginsWith" text="#">
+      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A299">
+    <cfRule type="containsText" priority="13" operator="containsText" text="......">
+      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" priority="14" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B305">
-    <cfRule type="containsText" priority="61" operator="containsText" text="......">
+    <cfRule type="containsText" priority="5" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="62" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" priority="6" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A305">
-    <cfRule type="containsText" dxfId="5" priority="63" operator="containsText" text="......">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="64" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="4" priority="8" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B310">
-    <cfRule type="containsText" priority="57" operator="containsText" text="......">
+  <conditionalFormatting sqref="A306">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="58" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A310">
-    <cfRule type="containsText" dxfId="3" priority="59" operator="containsText" text="......">
+  <conditionalFormatting sqref="B306">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="......">
       <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="60" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B302">
-    <cfRule type="containsText" priority="49" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="50" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A302">
-    <cfRule type="containsText" dxfId="1" priority="51" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="52" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B397">
-    <cfRule type="containsText" priority="33" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="34" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A397">
-    <cfRule type="containsText" priority="35" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="36" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A416">
-    <cfRule type="containsText" priority="29" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="30" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B416">
-    <cfRule type="containsText" priority="31" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="32" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A322">
-    <cfRule type="containsText" priority="17" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="18" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A317">
-    <cfRule type="containsText" priority="15" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="16" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A313">
-    <cfRule type="containsText" priority="13" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="14" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A309">
-    <cfRule type="containsText" priority="11" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="12" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B408">
-    <cfRule type="containsText" priority="9" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="10" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B299">
-    <cfRule type="containsText" priority="7" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="8" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A299">
-    <cfRule type="containsText" priority="5" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="6" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A301">
-    <cfRule type="containsText" priority="1" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="2" operator="beginsWith" text="#">
-      <formula>LEFT(#REF!,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B301">
-    <cfRule type="containsText" priority="3" operator="containsText" text="......">
-      <formula>NOT(ISERROR(SEARCH("......",#REF!)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="4" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="0" priority="4" operator="beginsWith" text="#">
       <formula>LEFT(#REF!,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>